<commit_message>
completed automating the stories 28631, 28282, 28286, 28287, 28291,28293, 29653
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PolicyPageData" sheetId="3" r:id="rId1"/>
-    <sheet name="LoginPageData" sheetId="1" r:id="rId2"/>
-    <sheet name="DashboardPageData" sheetId="5" r:id="rId3"/>
-    <sheet name="BrokerPageData" sheetId="2" r:id="rId4"/>
+    <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
+    <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
+    <sheet name="BrokerPageData" sheetId="2" r:id="rId3"/>
+    <sheet name="InsuredPageData" sheetId="6" r:id="rId4"/>
+    <sheet name="PolicyPageData" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="81">
   <si>
     <t>userName</t>
   </si>
@@ -173,9 +174,6 @@
     <t>testPoliciesDashboardUI</t>
   </si>
   <si>
-    <t>HUB International - NetGuard® Plus</t>
-  </si>
-  <si>
     <t>userId</t>
   </si>
   <si>
@@ -204,6 +202,75 @@
   </si>
   <si>
     <t>brokerPortal#123</t>
+  </si>
+  <si>
+    <t>agencyOfficeId</t>
+  </si>
+  <si>
+    <t>Caring Communities, A Reciprocal Risk Re</t>
+  </si>
+  <si>
+    <t>https://caringcomm.org/</t>
+  </si>
+  <si>
+    <t>QA Program 5204</t>
+  </si>
+  <si>
+    <t>testCreateInsured</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>spellegrino@caringcomm.org</t>
+  </si>
+  <si>
+    <t>Professional Risk Associates, Inc.</t>
+  </si>
+  <si>
+    <t>https://www.profrisk.com/</t>
+  </si>
+  <si>
+    <t>cfessler@profrisk.com</t>
+  </si>
+  <si>
+    <t>Crop Risk Services</t>
+  </si>
+  <si>
+    <t>testCreateInsuredFieldsValidation</t>
+  </si>
+  <si>
+    <t>testSearchAgainFunctionality</t>
+  </si>
+  <si>
+    <t>secondApplicant</t>
+  </si>
+  <si>
+    <t>Medical Assurance Company of Mississippi</t>
+  </si>
+  <si>
+    <t>https://macm.net/</t>
+  </si>
+  <si>
+    <t>secondWebsite</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>policyLabel</t>
+  </si>
+  <si>
+    <t>effDateLabel</t>
+  </si>
+  <si>
+    <t>expDateLabel</t>
+  </si>
+  <si>
+    <t>Policy #</t>
+  </si>
+  <si>
+    <t>policyTitle</t>
   </si>
 </sst>
 </file>
@@ -273,12 +340,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,89 +634,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6328125" customWidth="1"/>
-    <col min="5" max="5" width="61.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -649,14 +706,22 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
+      <c r="D5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -667,80 +732,427 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H21" sqref="H21:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20217</v>
+      </c>
+      <c r="E3" s="2">
+        <v>173</v>
+      </c>
+      <c r="F3" s="2">
+        <v>237</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>56</v>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2">
+        <v>25997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7166</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8414</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G9" s="2">
+        <v>173</v>
+      </c>
+      <c r="H9" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G10" s="2">
+        <v>237</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>55</v>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2">
+        <v>25997</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7166</v>
+      </c>
+      <c r="H11" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G16" s="2">
+        <v>173</v>
+      </c>
+      <c r="H16" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="2">
+        <v>25997</v>
+      </c>
+      <c r="G17" s="2">
+        <v>7166</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C22" s="2">
+        <v>173</v>
+      </c>
+      <c r="D22" s="2">
+        <v>237</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C23" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D23" s="2">
+        <v>8414</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -751,226 +1163,106 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>36</v>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2">
-        <v>20217</v>
-      </c>
-      <c r="E3" s="2">
-        <v>237</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="2">
-        <v>20217</v>
-      </c>
-      <c r="G7" s="2">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="2">
-        <v>20217</v>
-      </c>
-      <c r="G12" s="2">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2">
-        <v>6854</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3179</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -981,29 +1273,413 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H3" s="5">
+        <v>173</v>
+      </c>
+      <c r="I3" s="5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H10" s="5">
+        <v>173</v>
+      </c>
+      <c r="I10" s="5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H11" s="5">
+        <v>237</v>
+      </c>
+      <c r="I11" s="5">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I12" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H17" s="5">
+        <v>237</v>
+      </c>
+      <c r="I17" s="5">
+        <v>8006</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8414</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6328125" customWidth="1"/>
-    <col min="5" max="5" width="61.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1043,7 +1719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1063,7 +1739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
added test for searchRelatedRecords
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-testsLatest\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3F3DF-D142-4DCC-9D24-4CD6B8A31F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="94">
   <si>
     <t>userName</t>
   </si>
@@ -271,12 +272,51 @@
   </si>
   <si>
     <t>policyTitle</t>
+  </si>
+  <si>
+    <t>testBrokerSearchRelatedRecords</t>
+  </si>
+  <si>
+    <t>referenceNumber</t>
+  </si>
+  <si>
+    <t>Test Partner API</t>
+  </si>
+  <si>
+    <t>quoteName</t>
+  </si>
+  <si>
+    <t>policyName</t>
+  </si>
+  <si>
+    <t>Kelley Buick GMC</t>
+  </si>
+  <si>
+    <t>12825076</t>
+  </si>
+  <si>
+    <t>afd98afd</t>
+  </si>
+  <si>
+    <t>noSuchARecord</t>
+  </si>
+  <si>
+    <t>expForNoSuchARecord</t>
+  </si>
+  <si>
+    <t>Your search has no results</t>
+  </si>
+  <si>
+    <t>policyNumber</t>
+  </si>
+  <si>
+    <t>H20NPP70603-00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -354,6 +394,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,28 +675,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -668,7 +710,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -682,7 +724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -696,7 +738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -710,7 +752,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -731,35 +773,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H23"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -794,7 +836,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -829,7 +871,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -864,7 +906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -877,13 +919,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -909,7 +951,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -935,7 +977,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -961,7 +1003,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -987,13 +1029,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1061,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1087,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1071,13 +1113,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,7 +1145,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1129,7 +1171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1153,39 +1195,134 @@
       </c>
       <c r="H23" s="4" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C28" s="2">
+        <v>173</v>
+      </c>
+      <c r="D28" s="2">
+        <v>237</v>
+      </c>
+      <c r="E28" s="9">
+        <v>12825076</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C29" s="2">
+        <v>237</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E29" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1225,7 +1362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1272,35 +1409,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1329,7 +1466,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1495,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1524,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1416,13 +1553,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1451,7 +1588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -1480,7 +1617,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1509,7 +1646,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1538,13 +1675,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1579,7 +1716,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1751,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1656,30 +1793,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1699,7 +1836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1719,7 +1856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1739,7 +1876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
N2020-28566, 28565 and 29053
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="103">
   <si>
     <t>userName</t>
   </si>
@@ -271,6 +271,72 @@
   </si>
   <si>
     <t>policyTitle</t>
+  </si>
+  <si>
+    <t>testBrokerFilteringSubmissionsList</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>NetGuard® Plus</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>NetGuard® Plus;Generic Program - NetGuard® Plus</t>
+  </si>
+  <si>
+    <t>Active;Cancelled;Declined</t>
+  </si>
+  <si>
+    <t>testBrokerFilteringPoliciesList</t>
+  </si>
+  <si>
+    <t>Renewed;Renewal Started;Expired</t>
+  </si>
+  <si>
+    <t>testCheckDuplicateSubmission</t>
+  </si>
+  <si>
+    <t>Glasscock Chevrolet, Inc.</t>
+  </si>
+  <si>
+    <t>dialogText</t>
+  </si>
+  <si>
+    <t>An existing submission already exists for the selected Product and Insured</t>
+  </si>
+  <si>
+    <t>testPresenceOfContinueButtonOnQuotes</t>
+  </si>
+  <si>
+    <t>NetGuard® Plus;QA Program 5204</t>
+  </si>
+  <si>
+    <t>allProducts</t>
+  </si>
+  <si>
+    <t>All Products</t>
+  </si>
+  <si>
+    <t>allStatuses</t>
+  </si>
+  <si>
+    <t>All Statuses</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>12/30/2021</t>
+  </si>
+  <si>
+    <t>12/31/2021</t>
   </si>
 </sst>
 </file>
@@ -340,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -354,6 +420,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H23"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +812,7 @@
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
@@ -796,7 +863,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>36</v>
@@ -808,10 +875,10 @@
         <v>20217</v>
       </c>
       <c r="E3" s="2">
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2">
-        <v>237</v>
+        <v>8006</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>27</v>
@@ -831,7 +898,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
@@ -1045,7 +1112,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1071,13 +1138,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,18 +1170,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="2">
         <v>20217</v>
       </c>
       <c r="C22" s="2">
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="D22" s="2">
-        <v>237</v>
+        <v>8006</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>79</v>
@@ -1129,9 +1196,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2">
         <v>25997</v>
@@ -1153,6 +1220,231 @@
       </c>
       <c r="H23" s="4" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C28" s="2">
+        <v>237</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8414</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C34" s="2">
+        <v>237</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C35" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D35" s="2">
+        <v>8414</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C40" s="2">
+        <v>237</v>
+      </c>
+      <c r="D40" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C41" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D41" s="2">
+        <v>8414</v>
       </c>
     </row>
   </sheetData>
@@ -1273,23 +1565,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1647,6 +1938,70 @@
       </c>
       <c r="K18" s="2" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G23" s="5">
+        <v>237</v>
+      </c>
+      <c r="H23" s="5">
+        <v>8006</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pom.xml with allure dependency
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="110">
   <si>
     <t>corp</t>
   </si>
@@ -329,6 +329,33 @@
   </si>
   <si>
     <t>testSubmissionRenewal</t>
+  </si>
+  <si>
+    <t>testSubmissionClearancesFunctionality</t>
+  </si>
+  <si>
+    <t>QA Program 5203</t>
+  </si>
+  <si>
+    <t>www.ui.com</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>functionality</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>clearanceText</t>
+  </si>
+  <si>
+    <t>Test purpose</t>
+  </si>
+  <si>
+    <t>cancel</t>
   </si>
 </sst>
 </file>
@@ -794,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -1577,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2017,6 +2044,108 @@
         <v>99</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G28" s="5">
+        <v>237</v>
+      </c>
+      <c r="H28" s="5">
+        <v>8006</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G29" s="5">
+        <v>237</v>
+      </c>
+      <c r="H29" s="5">
+        <v>8006</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added test for sort by quote
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-testsQAT-105\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56361037-3811-4D4B-93C8-010B01B4CF53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
   <si>
     <t>corp</t>
   </si>
@@ -329,12 +330,15 @@
   </si>
   <si>
     <t>testSubmissionRenewal</t>
+  </si>
+  <si>
+    <t>sortQuoteList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -693,28 +697,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -728,7 +732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -742,7 +746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -756,7 +760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -770,7 +774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -791,35 +795,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -854,7 +858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -889,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -924,7 +928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -937,13 +941,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -969,7 +973,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -995,7 +999,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1025,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1047,13 +1051,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1083,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1131,13 +1135,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1163,7 +1167,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1215,13 +1219,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1257,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1279,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1307,13 +1311,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1400,13 +1404,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1462,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1484,13 +1488,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1522,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -1532,13 +1536,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -1564,6 +1568,54 @@
       </c>
       <c r="D52" s="2">
         <v>8006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C57" s="2">
+        <v>237</v>
+      </c>
+      <c r="D57" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C58" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D58" s="2">
+        <v>8414</v>
       </c>
     </row>
   </sheetData>
@@ -1576,35 +1628,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +1685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1714,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1743,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1720,13 +1772,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -1755,7 +1807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1784,7 +1836,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1865,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -1842,13 +1894,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1935,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1918,7 +1970,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -1953,13 +2005,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1988,7 +2040,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added test for sortMyPolicyPage
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-testsQAT-105\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-testsQAT-121\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56361037-3811-4D4B-93C8-010B01B4CF53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6703FB-75F2-4B9E-A796-7E0A967F211B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
   <si>
     <t>corp</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>sortQuoteList</t>
+  </si>
+  <si>
+    <t>sortPolicyList</t>
   </si>
 </sst>
 </file>
@@ -796,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,6 +1618,54 @@
         <v>7166</v>
       </c>
       <c r="D58" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C64" s="2">
+        <v>237</v>
+      </c>
+      <c r="D64" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C65" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D65" s="2">
         <v>8414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rating criteria pages and Insured, Dashboard actions
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -217,9 +217,6 @@
     <t>expDateLabel</t>
   </si>
   <si>
-    <t>Policy #</t>
-  </si>
-  <si>
     <t>policyTitle</t>
   </si>
   <si>
@@ -337,12 +334,6 @@
     <t>QA Program 5203</t>
   </si>
   <si>
-    <t>www.ui.com</t>
-  </si>
-  <si>
-    <t>ui</t>
-  </si>
-  <si>
     <t>functionality</t>
   </si>
   <si>
@@ -356,6 +347,15 @@
   </si>
   <si>
     <t>cancel</t>
+  </si>
+  <si>
+    <t>Policy#</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>SecurTest</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -441,6 +441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,64 +1188,64 @@
         <v>62</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="2">
         <v>20217</v>
       </c>
       <c r="C22" s="2">
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="D22" s="2">
-        <v>237</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="4" t="s">
+        <v>8006</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2">
-        <v>25997</v>
+        <v>20217</v>
       </c>
       <c r="C23" s="2">
-        <v>7166</v>
+        <v>237</v>
       </c>
       <c r="D23" s="2">
-        <v>8414</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="4" t="s">
+        <v>8006</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -1262,22 +1263,22 @@
         <v>42</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="H27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="J27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1316,27 +1317,27 @@
         <v>8006</v>
       </c>
       <c r="E29" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="I29" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -1354,19 +1355,19 @@
         <v>42</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1383,19 +1384,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1412,24 +1413,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="G35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1447,16 +1448,16 @@
         <v>42</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="G39" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1473,16 +1474,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="G40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1499,21 +1500,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1561,7 +1562,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1606,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1859,14 +1860,14 @@
       <c r="F12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="2">
-        <v>25997</v>
-      </c>
-      <c r="H12" s="2">
-        <v>7166</v>
-      </c>
-      <c r="I12" s="2">
-        <v>8414</v>
+      <c r="G12" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H12" s="5">
+        <v>237</v>
+      </c>
+      <c r="I12" s="5">
+        <v>8006</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1982,7 +1983,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -2012,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2020,10 +2021,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>50</v>
@@ -2041,12 +2042,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -2076,10 +2077,10 @@
         <v>42</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2087,13 +2088,13 @@
         <v>3</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>51</v>
@@ -2108,24 +2109,24 @@
         <v>8006</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>51</v>
@@ -2140,10 +2141,10 @@
         <v>8006</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for renewal submission
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\qat-140\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE71F0-A2B9-4248-A2B0-FBF1E4BEBF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="111">
   <si>
     <t>corp</t>
   </si>
@@ -356,12 +357,15 @@
   </si>
   <si>
     <t>Technical support ticket details 89083@#</t>
+  </si>
+  <si>
+    <t>brokersCanContinueRenewalSubmission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -720,28 +724,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -755,7 +759,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -769,7 +773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -783,7 +787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -797,7 +801,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -818,35 +822,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,7 +885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -916,7 +920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -951,7 +955,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -964,13 +968,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1074,13 +1078,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1158,13 +1162,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1242,13 +1246,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1302,7 +1306,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1334,13 +1338,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1369,7 +1373,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1402,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1427,13 +1431,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1459,7 +1463,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1489,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1511,13 +1515,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -1559,13 +1563,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -1593,13 +1597,13 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1613,7 +1617,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1631,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -1641,13 +1645,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1675,7 +1679,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -1689,13 +1693,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -1706,7 +1710,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -1726,6 +1730,54 @@
       </c>
       <c r="C71" s="2" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C76" s="2">
+        <v>237</v>
+      </c>
+      <c r="D76" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="2">
+        <v>25997</v>
+      </c>
+      <c r="C77" s="2">
+        <v>7166</v>
+      </c>
+      <c r="D77" s="2">
+        <v>8414</v>
       </c>
     </row>
   </sheetData>
@@ -1738,35 +1790,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1795,7 +1847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1824,7 +1876,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1853,7 +1905,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1882,13 +1934,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -1917,7 +1969,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1946,7 +1998,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -1975,7 +2027,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2004,13 +2056,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -2045,7 +2097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +2132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -2115,13 +2167,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -2150,7 +2202,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Chnaged name of tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\qat-140\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE71F0-A2B9-4248-A2B0-FBF1E4BEBF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADC82C1-5A12-4772-85E3-BF2E90DB29E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,12 +332,6 @@
     <t>testSubmissionRenewal</t>
   </si>
   <si>
-    <t>sortQuoteList</t>
-  </si>
-  <si>
-    <t>sortPolicyList</t>
-  </si>
-  <si>
     <t>testSupportRequestFunctionality</t>
   </si>
   <si>
@@ -359,7 +353,13 @@
     <t>Technical support ticket details 89083@#</t>
   </si>
   <si>
-    <t>brokersCanContinueRenewalSubmission</t>
+    <t>testBrokersCanContinueRenewalSubmission</t>
+  </si>
+  <si>
+    <t>testSortPolicyList</t>
+  </si>
+  <si>
+    <t>testSortQuoteList</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:E78"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1704,10 +1704,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,10 +1715,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1726,15 +1726,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B74" s="3"/>
     </row>

</xml_diff>

<commit_message>
added rating criteria test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\qat-140\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-138\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADC82C1-5A12-4772-85E3-BF2E90DB29E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68BAFC8-5866-457A-819A-E9C623960C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
-    <sheet name="InsuredPageData" sheetId="6" r:id="rId3"/>
+    <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId3"/>
+    <sheet name="InsuredPageData" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="114">
   <si>
     <t>corp</t>
   </si>
@@ -360,16 +361,33 @@
   </si>
   <si>
     <t>testSortQuoteList</t>
+  </si>
+  <si>
+    <t>testBusinessClassRatingCriteria</t>
+  </si>
+  <si>
+    <t>numberOfResidentialUnits</t>
+  </si>
+  <si>
+    <t>totalCommercialSquareFeet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,10 +444,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -445,8 +464,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -825,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="A7:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,6 +1812,205 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF225D3-E606-4AF6-A62B-6FD700D61264}">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G4" s="2">
+        <v>173</v>
+      </c>
+      <c r="H4" s="2">
+        <v>237</v>
+      </c>
+      <c r="I4" s="2">
+        <v>173</v>
+      </c>
+      <c r="J4" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G5" s="2">
+        <v>237</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8006</v>
+      </c>
+      <c r="I5" s="2">
+        <v>237</v>
+      </c>
+      <c r="J5" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G6" s="2">
+        <v>237</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8006</v>
+      </c>
+      <c r="I6" s="2">
+        <v>345</v>
+      </c>
+      <c r="J6" s="2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2">
+        <v>25997</v>
+      </c>
+      <c r="G7" s="2">
+        <v>7166</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8414</v>
+      </c>
+      <c r="I7" s="2">
+        <v>7166</v>
+      </c>
+      <c r="J7" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{7AD2ACDB-3694-4B59-9301-E2459120C957}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{0020B867-C65E-411C-ABAA-861427088C85}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{704174E4-1049-42EF-9B0A-338A4536675B}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{E5665601-356E-4845-8E9E-D2DF78CAE73E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>

</xml_diff>

<commit_message>
submission clearenace scripts updates
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="121">
   <si>
     <t>corp</t>
   </si>
@@ -322,9 +322,6 @@
     <t>dialogText</t>
   </si>
   <si>
-    <t>Glasscock Chevrolet, Inc.</t>
-  </si>
-  <si>
     <t>An existing submission already exists for the selected Product and Insured</t>
   </si>
   <si>
@@ -356,6 +353,42 @@
   </si>
   <si>
     <t>Technical support ticket details 89083@#</t>
+  </si>
+  <si>
+    <t>functionality</t>
+  </si>
+  <si>
+    <t>clearanceText</t>
+  </si>
+  <si>
+    <t>QA Program 5203</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Test purpose</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>testClearancesSubmissionFunctionality</t>
+  </si>
+  <si>
+    <t>testCancelClearancesFunctionality</t>
+  </si>
+  <si>
+    <t>testSubmissionClearanceComplete</t>
+  </si>
+  <si>
+    <t>venkat qa</t>
+  </si>
+  <si>
+    <t>venkatqa.com</t>
+  </si>
+  <si>
+    <t>venkatqa</t>
   </si>
 </sst>
 </file>
@@ -821,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
@@ -1561,7 +1594,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1595,7 +1628,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1643,7 +1676,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1691,7 +1724,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1700,10 +1733,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1711,10 +1744,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1722,10 +1755,10 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1739,23 +1772,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.109375" customWidth="1"/>
     <col min="5" max="5" width="28.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2158,10 +2190,10 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>51</v>
@@ -2176,7 +2208,180 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E28" s="5">
+        <v>237</v>
+      </c>
+      <c r="F28" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E33" s="5">
+        <v>237</v>
+      </c>
+      <c r="F33" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G38" s="5">
+        <v>237</v>
+      </c>
+      <c r="H38" s="5">
+        <v>8006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hard decline test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-138\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-testsn-QAT-171\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68BAFC8-5866-457A-819A-E9C623960C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F128A554-2F09-4458-A1CE-02F6238B5C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="120">
   <si>
     <t>corp</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t>totalCommercialSquareFeet</t>
+  </si>
+  <si>
+    <t>testHardDeclineAfterRatingCriteria</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>testUWDemo</t>
+  </si>
+  <si>
+    <t>bitcoin</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
   </si>
 </sst>
 </file>
@@ -753,21 +771,21 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -781,7 +799,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -795,7 +813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -809,7 +827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -823,7 +841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -851,28 +869,28 @@
       <selection activeCell="I12" sqref="A7:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" customWidth="1"/>
-    <col min="10" max="10" width="41.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.5546875" customWidth="1"/>
+    <col min="10" max="10" width="41.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -907,7 +925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -942,7 +960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -977,7 +995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -990,13 +1008,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1066,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1074,7 +1092,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1100,13 +1118,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -1158,7 +1176,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1184,13 +1202,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1234,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1242,7 +1260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1268,13 +1286,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1306,7 +1324,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1328,7 +1346,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1360,13 +1378,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1413,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1442,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1453,13 +1471,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1485,7 +1503,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1511,7 +1529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1537,13 +1555,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1557,7 +1575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -1571,7 +1589,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -1585,13 +1603,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -1619,13 +1637,13 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1639,7 +1657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1653,7 +1671,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -1667,13 +1685,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -1687,7 +1705,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1701,7 +1719,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -1715,13 +1733,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -1732,7 +1750,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1761,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -1754,13 +1772,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -1774,7 +1792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1806,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -1813,33 +1831,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF225D3-E606-4AF6-A62B-6FD700D61264}">
-  <dimension ref="A2:J7"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1871,8 +1889,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1903,8 +1921,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1935,8 +1953,8 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1967,8 +1985,8 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1999,12 +2017,182 @@
         <v>8414</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G13" s="2">
+        <v>173</v>
+      </c>
+      <c r="H13" s="2">
+        <v>237</v>
+      </c>
+      <c r="I13" s="2">
+        <v>173</v>
+      </c>
+      <c r="J13" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G14" s="2">
+        <v>237</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8006</v>
+      </c>
+      <c r="I14" s="2">
+        <v>237</v>
+      </c>
+      <c r="J14" s="2">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20217</v>
+      </c>
+      <c r="G15" s="2">
+        <v>237</v>
+      </c>
+      <c r="H15" s="2">
+        <v>8006</v>
+      </c>
+      <c r="I15" s="2">
+        <v>34534534</v>
+      </c>
+      <c r="J15" s="2">
+        <v>34534534</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="2">
+        <v>25997</v>
+      </c>
+      <c r="G16" s="2">
+        <v>7166</v>
+      </c>
+      <c r="H16" s="2">
+        <v>8414</v>
+      </c>
+      <c r="I16" s="2">
+        <v>7166</v>
+      </c>
+      <c r="J16" s="2">
+        <v>8414</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{7AD2ACDB-3694-4B59-9301-E2459120C957}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{0020B867-C65E-411C-ABAA-861427088C85}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{704174E4-1049-42EF-9B0A-338A4536675B}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{E5665601-356E-4845-8E9E-D2DF78CAE73E}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{0E96E55B-11D0-4CA4-A243-023A8A9D606C}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{CFB11501-0188-4183-BE92-5CEE7252C16C}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{0C6DAEB4-674F-438C-B058-900C8755B474}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{95FC012E-17CA-4E6B-9ACD-A1CC4046C87A}"/>
+    <hyperlink ref="D15" r:id="rId5" display="https://www.profrisk.com/" xr:uid="{861028F0-4DFE-4398-8ECC-29EFB65C4143}"/>
+    <hyperlink ref="D13" r:id="rId6" xr:uid="{EF208C9B-8A59-4791-BCB5-0148C68F6436}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{02897155-9A5D-4731-A723-DF058A731684}"/>
+    <hyperlink ref="D16" r:id="rId8" xr:uid="{A0D34BE4-DA9F-48E1-8406-10088CEBC0A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2018,28 +2206,28 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2068,7 +2256,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2285,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2314,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2155,13 +2343,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -2190,7 +2378,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -2219,7 +2407,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2248,7 +2436,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2277,13 +2465,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -2318,7 +2506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2353,7 +2541,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -2388,13 +2576,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -2423,7 +2611,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added quote option test file and updated test data
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
     <sheet name="InsuredPageData" sheetId="6" r:id="rId3"/>
-    <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId4"/>
+    <sheet name="QuoteOptionPageData" sheetId="8" r:id="rId4"/>
+    <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="127">
   <si>
     <t>corp</t>
   </si>
@@ -405,6 +406,9 @@
   </si>
   <si>
     <t>Business to Business</t>
+  </si>
+  <si>
+    <t>testAddQuoteOption</t>
   </si>
 </sst>
 </file>
@@ -1855,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2322,6 +2326,107 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="13">
+        <v>20217</v>
+      </c>
+      <c r="F3" s="13">
+        <v>173</v>
+      </c>
+      <c r="G3" s="13">
+        <v>237</v>
+      </c>
+      <c r="H3" s="13">
+        <v>173</v>
+      </c>
+      <c r="I3" s="13">
+        <v>237</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>

</xml_diff>

<commit_message>
added test for UW
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-testsn-QAT-171\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-qat-165\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F128A554-2F09-4458-A1CE-02F6238B5C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CAC15F-2901-40CF-8851-3EFBF5712F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
     <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId3"/>
-    <sheet name="InsuredPageData" sheetId="6" r:id="rId4"/>
+    <sheet name="UnderwritingQuestionsPageData" sheetId="8" r:id="rId4"/>
+    <sheet name="InsuredPageData" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="123">
   <si>
     <t>corp</t>
   </si>
@@ -388,6 +389,15 @@
   </si>
   <si>
     <t>Bitcoin</t>
+  </si>
+  <si>
+    <t>testBrokerAnswersUnderWriterQuestions</t>
+  </si>
+  <si>
+    <t>reffNumber</t>
+  </si>
+  <si>
+    <t>"13725999"</t>
   </si>
 </sst>
 </file>
@@ -866,7 +876,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="A7:I12"/>
+      <selection activeCell="A26" sqref="A26:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1833,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF225D3-E606-4AF6-A62B-6FD700D61264}">
   <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2199,6 +2209,69 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92AFBCD-B540-4B8C-8E25-A6FB992873C9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C3" s="2">
+        <v>237</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>

</xml_diff>

<commit_message>
added quote download test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-latest-156\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650037D5-EC88-4398-84AD-8043DD863F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -18,6 +19,7 @@
     <sheet name="UnderwritingQuestionsPageData" sheetId="8" r:id="rId4"/>
     <sheet name="QuoteOptionPageData" sheetId="9" r:id="rId5"/>
     <sheet name="InsuredPageData" sheetId="6" r:id="rId6"/>
+    <sheet name="QuotesPageData" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="143">
   <si>
     <t>corp</t>
   </si>
@@ -452,12 +454,18 @@
   </si>
   <si>
     <t>venkatqa.com</t>
+  </si>
+  <si>
+    <t>testBrokerDownloadConfirmedQuote</t>
+  </si>
+  <si>
+    <t>13725777</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -533,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -551,6 +559,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -831,7 +840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -929,7 +938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1897,7 +1906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2060,15 +2069,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2131,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2352,10 +2361,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -2912,4 +2921,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25655E2E-26FF-408A-A5FA-32D7A8EF798A}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>20217</v>
+      </c>
+      <c r="C3">
+        <v>237</v>
+      </c>
+      <c r="D3">
+        <v>8006</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test for policy renew hide button
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-qat-104\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D960F90E-0B67-4B92-8927-734EB8C1B803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="144">
   <si>
     <t>corp</t>
   </si>
@@ -452,12 +453,21 @@
   </si>
   <si>
     <t>venkatqa.com</t>
+  </si>
+  <si>
+    <t>testHideRenewButtonOnPolicyList</t>
+  </si>
+  <si>
+    <t>Cancelled;Renewal Started;Express Renewal;Non Renewed</t>
+  </si>
+  <si>
+    <t>"H21NPP70841-00";"H21NPP70098-01";"H21NPP70175-01";"H21NPP70840-00"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -831,7 +841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -929,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +953,7 @@
     <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" customWidth="1"/>
     <col min="9" max="9" width="34.5546875" customWidth="1"/>
@@ -1786,7 +1796,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -1800,13 +1810,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -1817,7 +1827,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -1828,7 +1838,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -1839,13 +1849,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1869,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -1873,7 +1883,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -1885,6 +1895,52 @@
       </c>
       <c r="D77" s="2">
         <v>8414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C81" s="2">
+        <v>237</v>
+      </c>
+      <c r="D81" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2060,15 +2116,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2131,7 +2187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2352,10 +2408,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed automation failure for download report
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-latest-156\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650037D5-EC88-4398-84AD-8043DD863F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7193CD-610F-4BBA-BAAC-6DBEC81A6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="UnderwritingQuestionsPageData" sheetId="8" r:id="rId4"/>
     <sheet name="QuoteOptionPageData" sheetId="9" r:id="rId5"/>
     <sheet name="InsuredPageData" sheetId="6" r:id="rId6"/>
-    <sheet name="QuotesPageData" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="149">
   <si>
     <t>corp</t>
   </si>
@@ -459,7 +458,25 @@
     <t>testBrokerDownloadConfirmedQuote</t>
   </si>
   <si>
-    <t>13725777</t>
+    <t>"13725777"</t>
+  </si>
+  <si>
+    <t>pdfFilename</t>
+  </si>
+  <si>
+    <t>TMHCC_Quote_2196819.pdf</t>
+  </si>
+  <si>
+    <t>wordFilename</t>
+  </si>
+  <si>
+    <t>TMHCC_Quote_2196819.docx</t>
+  </si>
+  <si>
+    <t>wordPDFFilename</t>
+  </si>
+  <si>
+    <t>TMHCC_Marketing_Materials_Quote_2196819.pdf</t>
   </si>
 </sst>
 </file>
@@ -541,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -560,6 +577,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2141,17 +2159,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2355,8 +2377,66 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>20217</v>
+      </c>
+      <c r="C13">
+        <v>237</v>
+      </c>
+      <c r="D13">
+        <v>8006</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H13" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2921,66 +3001,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25655E2E-26FF-408A-A5FA-32D7A8EF798A}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>20217</v>
-      </c>
-      <c r="C3">
-        <v>237</v>
-      </c>
-      <c r="D3">
-        <v>8006</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue on confirm and lock
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-QAT-174\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038730F3-0437-489C-BC9A-F68856589D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="144">
   <si>
     <t>corp</t>
   </si>
@@ -452,12 +453,21 @@
   </si>
   <si>
     <t>venkatqa.com</t>
+  </si>
+  <si>
+    <t>testConfirmAndLockQuoteOption</t>
+  </si>
+  <si>
+    <t>$ 2MM</t>
+  </si>
+  <si>
+    <t>$ 5MM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -831,7 +841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -929,7 +939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1897,7 +1907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2060,15 +2070,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2131,18 +2141,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2346,16 +2359,110 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E13" s="5">
+        <v>237</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8006</v>
+      </c>
+      <c r="G13" s="5">
+        <v>173</v>
+      </c>
+      <c r="H13" s="5">
+        <v>237</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="5">
+        <v>445</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N13" s="12">
+        <v>12000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added confrim and lock test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-QAT-174\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F272EC-73ED-4082-924E-49C55212803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC116CFD-AC06-478C-B58F-12E811804870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="154">
   <si>
     <t>corp</t>
   </si>
@@ -483,6 +483,16 @@
   </si>
   <si>
     <t>TMHCC_Marketing_Materials_Quote_2196819.pdf</t>
+  </si>
+  <si>
+    <t>Success
+Quote is successfully locked.</t>
+  </si>
+  <si>
+    <t>quoteSuccessMessage</t>
+  </si>
+  <si>
+    <t>"13726167"</t>
   </si>
 </sst>
 </file>
@@ -582,7 +592,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2167,7 +2179,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,6 +2193,7 @@
     <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2431,8 +2444,11 @@
       <c r="N12" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -2475,61 +2491,64 @@
       <c r="N13" s="12">
         <v>12000</v>
       </c>
+      <c r="O13" s="13" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>20217</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>237</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>8006</v>
       </c>
-      <c r="E18">
-        <v>13725777</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quote Option and Delete scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="149">
   <si>
     <t>corp</t>
   </si>
@@ -91,12 +91,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>MY QUOTES</t>
-  </si>
-  <si>
-    <t>MY POLICIES</t>
-  </si>
-  <si>
     <t>testQuotesDashboardUI</t>
   </si>
   <si>
@@ -397,12 +391,6 @@
     <t>reffNumber</t>
   </si>
   <si>
-    <t>"13725999"</t>
-  </si>
-  <si>
-    <t>testAddQuoteOption</t>
-  </si>
-  <si>
     <t>businessClass</t>
   </si>
   <si>
@@ -424,9 +412,6 @@
     <t>$ 7MM</t>
   </si>
   <si>
-    <t>testDeleteQuoteOption</t>
-  </si>
-  <si>
     <t>testCancelClearancesFunctionality</t>
   </si>
   <si>
@@ -452,6 +437,45 @@
   </si>
   <si>
     <t>venkatqa.com</t>
+  </si>
+  <si>
+    <t>"12854831"</t>
+  </si>
+  <si>
+    <t>addQuoteOption</t>
+  </si>
+  <si>
+    <t>deleteQuoteOption</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>uwQuestionsOption</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>uwQuestionsAnswer</t>
+  </si>
+  <si>
+    <t>testAddAndDeleteQuoteOption</t>
+  </si>
+  <si>
+    <t>testAddQuote</t>
+  </si>
+  <si>
+    <t>NetGaurd Plus</t>
+  </si>
+  <si>
+    <t>My Policies</t>
+  </si>
+  <si>
+    <t>My Quotes</t>
+  </si>
+  <si>
+    <t>testLockQuote</t>
   </si>
 </sst>
 </file>
@@ -533,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -551,6 +575,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -848,7 +875,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -857,13 +884,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -871,13 +898,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -885,13 +912,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -913,13 +940,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +960,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E29"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,7 +980,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -974,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>16</v>
@@ -989,7 +1016,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -997,10 +1024,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>147</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1032,10 +1059,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>147</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1086,16 +1113,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -1104,7 +1131,7 @@
         <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1112,16 +1139,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2">
         <v>20217</v>
@@ -1138,16 +1165,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2">
         <v>20217</v>
@@ -1164,16 +1191,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2">
         <v>25997</v>
@@ -1196,16 +1223,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
@@ -1214,7 +1241,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1222,16 +1249,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F16" s="2">
         <v>20217</v>
@@ -1248,16 +1275,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F17" s="2">
         <v>25997</v>
@@ -1271,7 +1298,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
@@ -1286,19 +1313,19 @@
         <v>9</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1315,7 +1342,7 @@
         <v>237</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>13</v>
@@ -1324,7 +1351,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1341,7 +1368,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1350,12 +1377,12 @@
         <v>14</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -1370,25 +1397,25 @@
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1427,27 +1454,27 @@
         <v>8006</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="I29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -1462,22 +1489,22 @@
         <v>9</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1494,19 +1521,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="I34" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1523,24 +1550,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1555,19 +1582,19 @@
         <v>9</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="H39" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1584,16 +1611,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1610,21 +1637,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1639,7 +1666,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1672,7 +1699,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1687,7 +1714,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1706,7 +1733,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1721,7 +1748,7 @@
         <v>9</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1754,7 +1781,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1769,7 +1796,7 @@
         <v>9</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,7 +1829,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1811,10 +1838,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1822,10 +1849,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1833,15 +1860,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -1856,7 +1883,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1920,7 +1947,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1929,16 +1956,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
@@ -1947,13 +1974,13 @@
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1961,16 +1988,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2">
         <v>20217</v>
@@ -1990,7 +2017,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -1999,16 +2026,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -2017,13 +2044,13 @@
         <v>9</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2031,16 +2058,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2072,7 +2099,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,7 +2113,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2101,27 +2128,27 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="13">
         <v>20217</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="13">
         <v>237</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="13">
         <v>8006</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>122</v>
+      <c r="E3" s="13" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2132,218 +2159,434 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>125</v>
+      <c r="M2" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>85</v>
+      <c r="B3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="5">
-        <v>20217</v>
+        <v>83</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="F3" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G3" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I3" s="5">
         <v>173</v>
       </c>
-      <c r="G3" s="5">
+      <c r="J3" s="5">
         <v>237</v>
       </c>
-      <c r="H3" s="5">
+      <c r="K3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M3" s="5">
+        <v>445</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P3" s="12">
+        <v>10000</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G4" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I4" s="5">
         <v>173</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J4" s="5">
         <v>237</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M4" s="5">
+        <v>445</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="6">
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G9" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I9" s="5">
+        <v>173</v>
+      </c>
+      <c r="J9" s="5">
+        <v>237</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="6">
         <v>1000000</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M9" s="5">
         <v>445</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O3" s="12">
+      <c r="N9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P9" s="12">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="Q9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="F14" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G14" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I14" s="5">
+        <v>173</v>
+      </c>
+      <c r="J14" s="5">
+        <v>237</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="L14" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M14" s="5">
+        <v>445</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="5">
-        <v>20217</v>
-      </c>
-      <c r="F8" s="5">
-        <v>173</v>
-      </c>
-      <c r="G8" s="5">
-        <v>237</v>
-      </c>
-      <c r="H8" s="5">
-        <v>173</v>
-      </c>
-      <c r="I8" s="5">
-        <v>237</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="L8" s="5">
-        <v>445</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O8" s="12">
+      <c r="P14" s="12">
         <v>10000</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2355,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2376,7 +2619,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2385,19 +2628,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>8</v>
@@ -2406,7 +2649,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2414,19 +2657,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5">
         <v>20217</v>
@@ -2443,19 +2686,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2">
         <v>25997</v>
@@ -2472,19 +2715,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2">
         <v>25997</v>
@@ -2498,7 +2741,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
@@ -2507,19 +2750,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>8</v>
@@ -2528,7 +2771,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2536,19 +2779,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="5">
         <v>20217</v>
@@ -2565,19 +2808,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="5">
         <v>20217</v>
@@ -2594,19 +2837,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2">
         <v>25997</v>
@@ -2620,7 +2863,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
@@ -2629,19 +2872,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>8</v>
@@ -2650,13 +2893,13 @@
         <v>9</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2664,19 +2907,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="5">
         <v>20217</v>
@@ -2688,10 +2931,10 @@
         <v>8006</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2699,19 +2942,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2">
         <v>25997</v>
@@ -2723,15 +2966,15 @@
         <v>8414</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -2740,16 +2983,16 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>8</v>
@@ -2758,10 +3001,10 @@
         <v>9</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2769,16 +3012,16 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F23" s="5">
         <v>20217</v>
@@ -2790,12 +3033,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -2804,10 +3047,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>8</v>
@@ -2816,13 +3059,13 @@
         <v>9</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2830,10 +3073,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" s="5">
         <v>20217</v>
@@ -2845,15 +3088,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2861,16 +3104,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>8</v>
@@ -2879,7 +3122,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2887,16 +3130,16 @@
         <v>3</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F33" s="5">
         <v>20217</v>

</xml_diff>

<commit_message>
added test for quote preview
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-QAT-174\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-qat-229\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC116CFD-AC06-478C-B58F-12E811804870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335BF11F-C2CD-4538-B2C4-AD3B9CD338C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="155">
   <si>
     <t>corp</t>
   </si>
@@ -396,9 +396,6 @@
   </si>
   <si>
     <t>reffNumber</t>
-  </si>
-  <si>
-    <t>"13725999"</t>
   </si>
   <si>
     <t>testAddQuoteOption</t>
@@ -493,6 +490,12 @@
   </si>
   <si>
     <t>"13726167"</t>
+  </si>
+  <si>
+    <t>testQuotePreview</t>
+  </si>
+  <si>
+    <t>"13726192"</t>
   </si>
 </sst>
 </file>
@@ -2115,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2165,7 +2168,7 @@
         <v>8006</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2176,10 +2179,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2231,7 +2234,7 @@
         <v>113</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>115</v>
@@ -2240,13 +2243,13 @@
         <v>116</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2278,7 +2281,7 @@
         <v>237</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K3" s="6">
         <v>1000000</v>
@@ -2287,10 +2290,10 @@
         <v>445</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="O3" s="12">
         <v>10000</v>
@@ -2298,7 +2301,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2331,7 +2334,7 @@
         <v>113</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>115</v>
@@ -2340,13 +2343,13 @@
         <v>116</v>
       </c>
       <c r="M7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2378,7 +2381,7 @@
         <v>237</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K8" s="6">
         <v>1000000</v>
@@ -2387,10 +2390,10 @@
         <v>445</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="O8" s="12">
         <v>10000</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2427,7 +2430,7 @@
         <v>113</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>115</v>
@@ -2436,19 +2439,19 @@
         <v>116</v>
       </c>
       <c r="L12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="O12" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2477,7 @@
         <v>237</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J13" s="6">
         <v>1000000</v>
@@ -2483,24 +2486,24 @@
         <v>445</v>
       </c>
       <c r="L13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="N13" s="12">
         <v>12000</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2517,16 +2520,16 @@
         <v>121</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2540,16 +2543,109 @@
         <v>8006</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>150</v>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E23" s="5">
+        <v>237</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8006</v>
+      </c>
+      <c r="G23" s="5">
+        <v>173</v>
+      </c>
+      <c r="H23" s="5">
+        <v>237</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K23" s="5">
+        <v>445</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N23" s="12">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>
@@ -3002,7 +3098,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3026,10 +3122,10 @@
         <v>42</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3037,7 +3133,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>51</v>
@@ -3052,15 +3148,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3094,13 +3190,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
updated UW question changes
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-QAT-174\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC116CFD-AC06-478C-B58F-12E811804870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="165">
   <si>
     <t>corp</t>
   </si>
@@ -92,12 +91,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>MY QUOTES</t>
-  </si>
-  <si>
-    <t>MY POLICIES</t>
-  </si>
-  <si>
     <t>testQuotesDashboardUI</t>
   </si>
   <si>
@@ -401,9 +394,6 @@
     <t>"13725999"</t>
   </si>
   <si>
-    <t>testAddQuoteOption</t>
-  </si>
-  <si>
     <t>businessClass</t>
   </si>
   <si>
@@ -425,9 +415,6 @@
     <t>$ 7MM</t>
   </si>
   <si>
-    <t>testDeleteQuoteOption</t>
-  </si>
-  <si>
     <t>testCancelClearancesFunctionality</t>
   </si>
   <si>
@@ -435,9 +422,6 @@
   </si>
   <si>
     <t>clearanceText</t>
-  </si>
-  <si>
-    <t>QA Program 5203</t>
   </si>
   <si>
     <t>cancel</t>
@@ -493,12 +477,60 @@
   </si>
   <si>
     <t>"13726167"</t>
+  </si>
+  <si>
+    <t>testAddAndDeleteQuoteOption</t>
+  </si>
+  <si>
+    <t>uwQuestionsOption</t>
+  </si>
+  <si>
+    <t>uwQuestionsAnswer</t>
+  </si>
+  <si>
+    <t>addQuoteOption</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>deleteQuoteOption</t>
+  </si>
+  <si>
+    <t>testAddQuote</t>
+  </si>
+  <si>
+    <t>testLockQuote</t>
+  </si>
+  <si>
+    <t>My Quotes</t>
+  </si>
+  <si>
+    <t>My Policies</t>
+  </si>
+  <si>
+    <t>welcomeText</t>
+  </si>
+  <si>
+    <t>Welcome to QuoteIt</t>
+  </si>
+  <si>
+    <t>testClearancesSubmissionFunctionality</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>clearance test text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -533,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -569,12 +601,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -595,6 +638,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -875,7 +927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -892,7 +944,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -901,13 +953,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -915,13 +967,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -929,13 +981,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -949,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -957,13 +1009,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -973,11 +1025,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E29"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,13 +1047,13 @@
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>16</v>
@@ -1033,18 +1085,21 @@
         <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1070,16 +1125,19 @@
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1105,8 +1163,11 @@
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1119,27 +1180,27 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -1148,24 +1209,24 @@
         <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2">
         <v>20217</v>
@@ -1177,21 +1238,21 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2">
         <v>20217</v>
@@ -1203,21 +1264,21 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2">
         <v>25997</v>
@@ -1229,27 +1290,27 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
@@ -1258,24 +1319,24 @@
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F16" s="2">
         <v>20217</v>
@@ -1292,16 +1353,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F17" s="2">
         <v>25997</v>
@@ -1315,7 +1376,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
@@ -1330,19 +1391,19 @@
         <v>9</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1359,7 +1420,7 @@
         <v>237</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>13</v>
@@ -1367,8 +1428,8 @@
       <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>21</v>
+      <c r="H22" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1385,7 +1446,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1393,13 +1454,13 @@
       <c r="G23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>21</v>
+      <c r="H23" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -1414,25 +1475,25 @@
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1471,27 +1532,27 @@
         <v>8006</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="I29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -1506,22 +1567,22 @@
         <v>9</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1538,19 +1599,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="I34" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1567,24 +1628,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1599,19 +1660,19 @@
         <v>9</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="H39" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1628,16 +1689,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1654,21 +1715,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1683,7 +1744,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1716,7 +1777,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1731,7 +1792,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1750,7 +1811,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1765,7 +1826,7 @@
         <v>9</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1798,7 +1859,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1813,7 +1874,7 @@
         <v>9</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1846,7 +1907,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1855,10 +1916,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1866,10 +1927,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1877,15 +1938,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -1900,7 +1961,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1941,7 +2002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1964,7 +2025,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1973,16 +2034,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
@@ -1991,13 +2052,13 @@
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2005,16 +2066,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2">
         <v>20217</v>
@@ -2034,7 +2095,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2043,16 +2104,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -2061,13 +2122,13 @@
         <v>9</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2075,16 +2136,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2104,15 +2165,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2130,7 +2191,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2145,10 +2206,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2165,7 +2226,7 @@
         <v>8006</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2175,11 +2236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2196,360 +2257,593 @@
     <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>85</v>
+      <c r="B3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="5">
+        <v>83</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G3" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I3" s="5">
+        <v>173</v>
+      </c>
+      <c r="J3" s="5">
+        <v>237</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M3" s="5">
+        <v>445</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P3" s="12">
+        <v>10000</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G4" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I4" s="5">
+        <v>173</v>
+      </c>
+      <c r="J4" s="5">
+        <v>237</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M4" s="5">
+        <v>445</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G9" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I9" s="5">
+        <v>173</v>
+      </c>
+      <c r="J9" s="5">
+        <v>237</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="M9" s="5">
+        <v>445</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="12">
+        <v>10000</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="5">
         <v>20217</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E14" s="5">
+        <v>237</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8006</v>
+      </c>
+      <c r="G14" s="5">
         <v>173</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H14" s="5">
         <v>237</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K14" s="5">
+        <v>445</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N14" s="12">
+        <v>12000</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C19" s="2">
+        <v>237</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G24" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H24" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I24" s="5">
         <v>173</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J24" s="5">
         <v>237</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="K24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="6">
         <v>1000000</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M24" s="5">
         <v>445</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O3" s="12">
+      <c r="N24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P24" s="12">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="5">
-        <v>20217</v>
-      </c>
-      <c r="F8" s="5">
-        <v>173</v>
-      </c>
-      <c r="G8" s="5">
-        <v>237</v>
-      </c>
-      <c r="H8" s="5">
-        <v>173</v>
-      </c>
-      <c r="I8" s="5">
-        <v>237</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="L8" s="5">
-        <v>445</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="O8" s="12">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E13" s="5">
-        <v>237</v>
-      </c>
-      <c r="F13" s="2">
-        <v>8006</v>
-      </c>
-      <c r="G13" s="5">
-        <v>173</v>
-      </c>
-      <c r="H13" s="5">
-        <v>237</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J13" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="K13" s="5">
-        <v>445</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="N13" s="12">
-        <v>12000</v>
-      </c>
-      <c r="O13" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2">
-        <v>20217</v>
-      </c>
-      <c r="C18" s="2">
-        <v>237</v>
-      </c>
-      <c r="D18" s="2">
-        <v>8006</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="Q24" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>150</v>
+      <c r="R24" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2559,11 +2853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2583,7 +2877,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2592,19 +2886,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>8</v>
@@ -2613,7 +2907,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2621,19 +2915,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5">
         <v>20217</v>
@@ -2650,19 +2944,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2">
         <v>25997</v>
@@ -2678,20 +2972,20 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>45</v>
+      <c r="B5" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2">
         <v>25997</v>
@@ -2705,7 +2999,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
@@ -2714,19 +3008,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>8</v>
@@ -2735,7 +3029,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2743,19 +3037,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="5">
         <v>20217</v>
@@ -2772,19 +3066,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="5">
         <v>20217</v>
@@ -2800,20 +3094,20 @@
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>45</v>
+      <c r="B12" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2">
         <v>25997</v>
@@ -2827,7 +3121,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
@@ -2836,19 +3130,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>8</v>
@@ -2857,13 +3151,13 @@
         <v>9</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2871,19 +3165,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="5">
         <v>20217</v>
@@ -2895,30 +3189,30 @@
         <v>8006</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>45</v>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2">
         <v>25997</v>
@@ -2930,15 +3224,15 @@
         <v>8414</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -2947,16 +3241,16 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>8</v>
@@ -2965,10 +3259,10 @@
         <v>9</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2976,16 +3270,16 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F23" s="5">
         <v>20217</v>
@@ -2997,12 +3291,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3011,10 +3305,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>8</v>
@@ -3023,24 +3317,24 @@
         <v>9</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>135</v>
+      <c r="B28" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" s="5">
         <v>20217</v>
@@ -3052,15 +3346,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3068,16 +3362,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>8</v>
@@ -3086,24 +3380,24 @@
         <v>9</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F33" s="5">
         <v>20217</v>
@@ -3115,8 +3409,44 @@
         <v>8006</v>
       </c>
     </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made all scripts work on bp10
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\api-tests\bp-ui-tests\bp-ui-tests-maintanance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3472E1F-E8BC-4D2F-8412-460614000C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D352A6F-CBB2-4AB5-A0AC-27AD56F05082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -981,7 +981,7 @@
   <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1998,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,8 +2176,8 @@
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
+      <c r="B13" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C13" s="2">
         <v>20217</v>

</xml_diff>

<commit_message>
updated test data for testpoliciesUI script
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="166">
   <si>
     <t>corp</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>clearance test text</t>
+  </si>
+  <si>
+    <t>Policy#</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,7 +1449,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -2856,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H37" sqref="H37:H38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated scripts as per stage environment and product specific test data
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="167">
   <si>
     <t>corp</t>
   </si>
@@ -277,9 +277,6 @@
     <t>endDate</t>
   </si>
   <si>
-    <t>NetGuard® Plus</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -292,18 +289,12 @@
     <t>12/31/2021</t>
   </si>
   <si>
-    <t>NetGuard® Plus;QA Program 5204</t>
-  </si>
-  <si>
     <t>Active;Cancelled;Declined</t>
   </si>
   <si>
     <t>testBrokerFilteringPoliciesList</t>
   </si>
   <si>
-    <t>NetGuard® Plus;Generic Program - NetGuard® Plus</t>
-  </si>
-  <si>
     <t>Renewed;Renewal Started;Expired</t>
   </si>
   <si>
@@ -322,9 +313,6 @@
     <t>Glasscock Chevrolet, Inc.</t>
   </si>
   <si>
-    <t>An existing submission already exists for the selected Product and Insured</t>
-  </si>
-  <si>
     <t>testSubmissionRenewal</t>
   </si>
   <si>
@@ -409,12 +397,6 @@
     <t>Business to Business</t>
   </si>
   <si>
-    <t>$ 4MM</t>
-  </si>
-  <si>
-    <t>$ 7MM</t>
-  </si>
-  <si>
     <t>testCancelClearancesFunctionality</t>
   </si>
   <si>
@@ -440,12 +422,6 @@
   </si>
   <si>
     <t>testConfirmAndLockQuoteOption</t>
-  </si>
-  <si>
-    <t>$ 2MM</t>
-  </si>
-  <si>
-    <t>$ 5MM</t>
   </si>
   <si>
     <t>testBrokerDownloadConfirmedQuote</t>
@@ -528,6 +504,33 @@
   </si>
   <si>
     <t>Policy#</t>
+  </si>
+  <si>
+    <t>NetGuard® SELECT</t>
+  </si>
+  <si>
+    <t>NetGuard® SELECT;QA Program 5204</t>
+  </si>
+  <si>
+    <t>NetGuard® SELECT;Generic Program - NetGuard® SELECT</t>
+  </si>
+  <si>
+    <t>Submission already exists for the selected Product and Insured.</t>
+  </si>
+  <si>
+    <t>netWorth</t>
+  </si>
+  <si>
+    <t>businessClass2</t>
+  </si>
+  <si>
+    <t>Celebrity</t>
+  </si>
+  <si>
+    <t>$ 1MM</t>
+  </si>
+  <si>
+    <t>testQuotePreview</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -650,6 +653,9 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1031,7 +1037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1091,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1099,10 +1105,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1129,7 +1135,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1137,10 +1143,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1167,7 +1173,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1272,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1330,7 +1336,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1356,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1432,7 +1438,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1449,7 +1455,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1458,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1602,19 +1608,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1631,24 +1637,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1692,16 +1698,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1718,21 +1724,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1780,7 +1786,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1814,7 +1820,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1862,7 +1868,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1910,7 +1916,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1919,10 +1925,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1930,10 +1936,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1941,15 +1947,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -2006,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,13 +2032,13 @@
     <col min="10" max="10" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2058,18 +2064,30 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2095,14 +2113,26 @@
       <c r="J3" s="2">
         <v>345</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="5">
+        <v>50000</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2113,7 +2143,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -2128,27 +2158,39 @@
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2164,6 +2206,18 @@
       </c>
       <c r="J8" s="2">
         <v>34534534</v>
+      </c>
+      <c r="K8" s="5">
+        <v>50000</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2194,7 +2248,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2212,7 +2266,7 @@
         <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2229,7 +2283,7 @@
         <v>8006</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2240,16 +2294,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
@@ -2258,21 +2312,23 @@
     <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -2293,48 +2349,54 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>42</v>
@@ -2355,7 +2417,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2364,33 +2426,39 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="P3" s="12">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="S3" s="5">
+        <v>50000</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>42</v>
@@ -2411,7 +2479,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2420,22 +2488,28 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="P4" s="12">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="S4" s="5">
+        <v>50000</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="14"/>
@@ -2455,19 +2529,19 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
@@ -2488,48 +2562,54 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="N8" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>42</v>
@@ -2550,7 +2630,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2559,27 +2639,33 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="P9" s="12">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="S9" s="5">
+        <v>50000</v>
+      </c>
+      <c r="T9" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -2599,42 +2685,54 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="L13" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D14" s="5">
         <v>20217</v>
@@ -2642,7 +2740,7 @@
       <c r="E14" s="5">
         <v>237</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="5">
         <v>8006</v>
       </c>
       <c r="G14" s="5">
@@ -2652,7 +2750,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2661,24 +2759,36 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="N14" s="12">
         <v>12000</v>
       </c>
       <c r="O14" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="P14" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="S14" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2692,57 +2802,57 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="2">
         <v>20217</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="5">
         <v>237</v>
       </c>
       <c r="D19" s="2">
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
@@ -2763,48 +2873,54 @@
         <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="N23" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T23" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>42</v>
@@ -2825,7 +2941,7 @@
         <v>237</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L24" s="6">
         <v>1000000</v>
@@ -2834,19 +2950,148 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="P24" s="12">
         <v>10000</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+      <c r="S24" s="5">
+        <v>50000</v>
+      </c>
+      <c r="T24" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E29" s="5">
+        <v>237</v>
+      </c>
+      <c r="F29" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G29" s="5">
+        <v>173</v>
+      </c>
+      <c r="H29" s="5">
+        <v>237</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K29" s="5">
+        <v>445</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N29" s="12">
+        <v>12000</v>
+      </c>
+      <c r="O29" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="P29" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2859,21 +3104,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37:H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.109375" customWidth="1"/>
     <col min="5" max="5" width="28.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2976,7 +3220,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3098,7 +3342,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3203,7 +3447,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3235,7 +3479,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3265,7 +3509,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3273,10 +3517,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -3294,12 +3538,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3323,10 +3567,10 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3334,7 +3578,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3349,15 +3593,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3391,13 +3635,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -3414,7 +3658,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3425,10 +3669,10 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3436,13 +3680,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and fixed test scripts for cross-browser testing.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="169">
   <si>
     <t>corp</t>
   </si>
@@ -250,9 +250,6 @@
     <t>expForNoSuchARecord</t>
   </si>
   <si>
-    <t>Your search has no results</t>
-  </si>
-  <si>
     <t>policyNumber</t>
   </si>
   <si>
@@ -434,12 +431,6 @@
   </si>
   <si>
     <t>wordPDFFilename</t>
-  </si>
-  <si>
-    <t>TMHCC_Quote_2196819.pdf</t>
-  </si>
-  <si>
-    <t>TMHCC_Quote_2196819.docx</t>
   </si>
   <si>
     <t>TMHCC_Marketing_Materials_Quote_2196819.pdf</t>
@@ -452,9 +443,6 @@
     <t>quoteSuccessMessage</t>
   </si>
   <si>
-    <t>"13726167"</t>
-  </si>
-  <si>
     <t>testAddAndDeleteQuoteOption</t>
   </si>
   <si>
@@ -531,6 +519,24 @@
   </si>
   <si>
     <t>testQuotePreview</t>
+  </si>
+  <si>
+    <t>Your search has returned no results.</t>
+  </si>
+  <si>
+    <t>testHideRenewButtonOnPolicyList</t>
+  </si>
+  <si>
+    <t>Cancelled;Renewal Started;Express Renewal;Non Renewed</t>
+  </si>
+  <si>
+    <t>H21NPP70841-00;"H21NPP70098-01";"H21NPP70175-01";"H21NPP70840-00"</t>
+  </si>
+  <si>
+    <t>"13869826"</t>
+  </si>
+  <si>
+    <t>TMHCC_Quote_</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,7 +1103,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1105,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1135,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1143,10 +1149,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1173,7 +1179,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1278,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1336,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1362,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1438,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1455,7 +1461,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1464,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1502,7 +1508,7 @@
         <v>72</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1553,15 +1559,15 @@
         <v>70</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -1579,19 +1585,19 @@
         <v>40</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1608,19 +1614,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1637,24 +1643,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1672,16 +1678,16 @@
         <v>40</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="G39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1698,16 +1704,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1724,21 +1730,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1784,13 +1790,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -1803,8 +1809,11 @@
       <c r="D51" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -1817,14 +1826,17 @@
       <c r="D52" s="2">
         <v>8006</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -1866,13 +1878,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1900,7 +1912,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -1914,52 +1926,52 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +1999,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -1999,6 +2011,56 @@
       </c>
       <c r="D77" s="2">
         <v>8414</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C82" s="2">
+        <v>237</v>
+      </c>
+      <c r="D82" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2014,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:N8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2096,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2064,22 +2126,22 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2087,7 +2149,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2117,18 +2179,18 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2143,7 +2205,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -2158,22 +2220,22 @@
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2181,16 +2243,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2211,13 +2273,13 @@
         <v>50000</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2248,7 +2310,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2266,7 +2328,7 @@
         <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2283,7 +2345,7 @@
         <v>8006</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2296,8 +2358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28:S29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2313,12 +2375,12 @@
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2328,13 +2390,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>28</v>
@@ -2349,40 +2411,40 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2390,13 +2452,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>42</v>
@@ -2417,7 +2479,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2426,25 +2488,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P3" s="12">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2452,13 +2514,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>42</v>
@@ -2479,7 +2541,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2488,25 +2550,25 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P4" s="12">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2531,7 +2593,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2541,13 +2603,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -2562,40 +2624,40 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="K8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="Q8" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="T8" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2603,13 +2665,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>42</v>
@@ -2630,7 +2692,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2639,30 +2701,30 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P9" s="12">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2673,7 +2735,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2685,43 +2747,43 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="I13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="O13" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2729,10 +2791,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="5">
         <v>20217</v>
@@ -2750,7 +2812,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2759,33 +2821,33 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N14" s="12">
         <v>12000</v>
       </c>
       <c r="O14" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
@@ -2802,16 +2864,16 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -2828,21 +2890,21 @@
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2852,13 +2914,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>28</v>
@@ -2873,40 +2935,40 @@
         <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="K23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="Q23" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -2914,13 +2976,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>42</v>
@@ -2941,7 +3003,7 @@
         <v>237</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L24" s="6">
         <v>1000000</v>
@@ -2950,30 +3012,30 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P24" s="12">
         <v>10000</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S24" s="5">
         <v>50000</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -2984,7 +3046,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
@@ -2996,43 +3058,43 @@
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="I28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="N28" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="O28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -3040,10 +3102,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="5">
         <v>20217</v>
@@ -3061,7 +3123,7 @@
         <v>237</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J29" s="6">
         <v>1000000</v>
@@ -3070,28 +3132,28 @@
         <v>445</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N29" s="12">
         <v>12000</v>
       </c>
       <c r="O29" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P29" s="5">
         <v>50000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3282,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3342,7 +3404,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3447,7 +3509,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3479,7 +3541,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3509,7 +3571,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3517,10 +3579,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -3538,12 +3600,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3567,10 +3629,10 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3578,7 +3640,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3593,15 +3655,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3635,13 +3697,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -3658,7 +3720,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3669,10 +3731,10 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3680,13 +3742,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the script to make it compatible with stg
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_238_QAT\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE15DA5-064A-4201-995F-01DB5DC535DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="169">
   <si>
     <t>corp</t>
   </si>
@@ -238,9 +239,6 @@
     <t>Kelley Buick GMC</t>
   </si>
   <si>
-    <t>12825076</t>
-  </si>
-  <si>
     <t>afd98afd</t>
   </si>
   <si>
@@ -374,9 +372,6 @@
   </si>
   <si>
     <t>reffNumber</t>
-  </si>
-  <si>
-    <t>"13725999"</t>
   </si>
   <si>
     <t>businessClass</t>
@@ -527,22 +522,28 @@
     <t>testHideRenewButtonOnPolicyList</t>
   </si>
   <si>
-    <t>Cancelled;Renewal Started;Express Renewal;Non Renewed</t>
-  </si>
-  <si>
-    <t>H21NPP70841-00;"H21NPP70098-01";"H21NPP70175-01";"H21NPP70840-00"</t>
-  </si>
-  <si>
     <t>"13869826"</t>
   </si>
   <si>
     <t>TMHCC_Quote_</t>
+  </si>
+  <si>
+    <t>testQuotesInvalidatedWhenEdited</t>
+  </si>
+  <si>
+    <t>Renewal Started</t>
+  </si>
+  <si>
+    <t>H21OMC20060-00</t>
+  </si>
+  <si>
+    <t>testProposedPolicyPeriod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -629,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -643,7 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -942,7 +942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1040,11 +1040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,8 +1102,8 @@
       <c r="K2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="17" t="s">
-        <v>148</v>
+      <c r="L2" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1111,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1140,8 +1140,8 @@
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>149</v>
+      <c r="L3" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1149,10 +1149,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1178,8 +1178,8 @@
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="17" t="s">
-        <v>149</v>
+      <c r="L4" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1368,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1461,7 +1461,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1470,14 +1470,13 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1495,20 +1494,20 @@
       <c r="E27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1524,14 +1523,14 @@
       <c r="D28" s="2">
         <v>237</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="2">
         <v>12825076</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -1546,28 +1545,28 @@
       <c r="D29" s="2">
         <v>8006</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="2">
+        <v>12825076</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>74</v>
+      <c r="I29" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -1585,19 +1584,19 @@
         <v>40</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1614,19 +1613,19 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1643,24 +1642,24 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1678,16 +1677,16 @@
         <v>40</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="G39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1704,16 +1703,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1730,21 +1729,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1792,7 +1791,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1810,7 +1809,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1827,12 +1826,12 @@
         <v>8006</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1880,7 +1879,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1912,7 +1911,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -1926,52 +1925,52 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2013,71 +2012,47 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="2">
-        <v>20217</v>
-      </c>
-      <c r="C82" s="2">
-        <v>237</v>
-      </c>
-      <c r="D82" s="2">
-        <v>8006</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>166</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E29" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,11 +2067,12 @@
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="29.109375" customWidth="1"/>
     <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2126,22 +2102,22 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2149,12 +2125,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -2179,18 +2155,18 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2205,7 +2181,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -2220,22 +2196,22 @@
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2243,16 +2219,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>110</v>
+      <c r="D8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2273,80 +2249,187 @@
         <v>50000</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>20217</v>
+      <c r="B3" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="C3" s="2">
-        <v>237</v>
-      </c>
-      <c r="D3" s="2">
-        <v>8006</v>
+        <v>50000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="2">
+        <v>50000</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2355,11 +2438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2376,11 +2459,12 @@
     <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2390,13 +2474,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>28</v>
@@ -2411,40 +2495,40 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2452,13 +2536,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>42</v>
@@ -2479,7 +2563,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2488,25 +2572,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="P3" s="12">
+        <v>159</v>
+      </c>
+      <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
-      <c r="T3" s="19" t="s">
-        <v>160</v>
+      <c r="T3" s="18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2514,13 +2598,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>42</v>
@@ -2541,7 +2625,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2550,50 +2634,50 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="P4" s="12">
+        <v>159</v>
+      </c>
+      <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
-      <c r="T4" s="19" t="s">
-        <v>160</v>
+      <c r="T4" s="18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="14"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2603,13 +2687,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -2624,40 +2708,40 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="K8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="Q8" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="T8" s="17" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2665,13 +2749,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>42</v>
@@ -2692,7 +2776,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2701,30 +2785,30 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="P9" s="12">
+        <v>159</v>
+      </c>
+      <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
-      <c r="T9" s="19" t="s">
-        <v>160</v>
+      <c r="T9" s="18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2735,7 +2819,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2747,43 +2831,43 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="I13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="O13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="S13" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2791,10 +2875,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5">
         <v>20217</v>
@@ -2812,7 +2896,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2821,33 +2905,33 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="N14" s="12">
+        <v>159</v>
+      </c>
+      <c r="N14" s="11">
         <v>12000</v>
       </c>
-      <c r="O14" s="13" t="s">
-        <v>135</v>
+      <c r="O14" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
@@ -2864,16 +2948,16 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -2890,21 +2974,21 @@
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2914,13 +2998,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>28</v>
@@ -2935,40 +3019,40 @@
         <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="K23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="Q23" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="T23" s="17" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -2976,13 +3060,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>42</v>
@@ -3003,7 +3087,7 @@
         <v>237</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L24" s="6">
         <v>1000000</v>
@@ -3012,30 +3096,30 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="P24" s="12">
+        <v>159</v>
+      </c>
+      <c r="P24" s="11">
         <v>10000</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S24" s="5">
         <v>50000</v>
       </c>
-      <c r="T24" s="19" t="s">
-        <v>160</v>
+      <c r="T24" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -3046,7 +3130,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
@@ -3058,43 +3142,43 @@
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="I28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="O28" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="S28" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -3102,10 +3186,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="5">
         <v>20217</v>
@@ -3123,7 +3207,7 @@
         <v>237</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J29" s="6">
         <v>1000000</v>
@@ -3132,28 +3216,28 @@
         <v>445</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="N29" s="12">
+        <v>159</v>
+      </c>
+      <c r="N29" s="11">
         <v>12000</v>
       </c>
-      <c r="O29" s="13" t="s">
-        <v>135</v>
+      <c r="O29" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="P29" s="5">
         <v>50000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3163,7 +3247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3282,7 +3366,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3404,7 +3488,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3509,7 +3593,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3535,13 +3619,13 @@
       <c r="J18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3571,7 +3655,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3579,10 +3663,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -3600,12 +3684,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3629,10 +3713,10 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3640,7 +3724,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3655,15 +3739,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3697,13 +3781,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -3720,7 +3804,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3731,10 +3815,10 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3742,18 +3826,18 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
updated confir quote download test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="170">
   <si>
     <t>corp</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>H21NGP208318-01</t>
+  </si>
+  <si>
+    <t>$ 15,000</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
@@ -2440,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2909,8 +2912,8 @@
       <c r="M14" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="N14" s="11">
-        <v>12000</v>
+      <c r="N14" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O14" s="12" t="s">
         <v>133</v>
@@ -3100,8 +3103,8 @@
       <c r="O24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="P24" s="11">
-        <v>10000</v>
+      <c r="P24" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>139</v>
@@ -3220,8 +3223,8 @@
       <c r="M29" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="N29" s="11">
-        <v>12000</v>
+      <c r="N29" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O29" s="12" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
submission clearances tests updated
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="173">
   <si>
     <t>corp</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>Renewed;Renewal Started;Expired</t>
-  </si>
-  <si>
-    <t>12/30/2021</t>
   </si>
   <si>
     <t>testPresenceOfContinueButtonOnQuotes</t>
@@ -540,6 +537,18 @@
   </si>
   <si>
     <t>$ 15,000</t>
+  </si>
+  <si>
+    <t>12/30/2022</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1114,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1113,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1143,7 +1152,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1151,10 +1160,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1181,7 +1190,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1286,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1344,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1370,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1446,7 +1455,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1463,7 +1472,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1472,7 +1481,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1560,7 +1569,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>73</v>
@@ -1615,7 +1624,7 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>80</v>
@@ -1644,7 +1653,7 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>84</v>
@@ -1705,7 +1714,7 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>86</v>
@@ -1714,7 +1723,7 @@
         <v>82</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1731,7 +1740,7 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>86</v>
@@ -1740,12 +1749,12 @@
         <v>82</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1793,7 +1802,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1833,7 +1842,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1881,7 +1890,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1929,7 +1938,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1938,10 +1947,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1949,10 +1958,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1960,15 +1969,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -2016,7 +2025,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2037,10 +2046,10 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2074,7 +2083,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2104,22 +2113,22 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2127,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2157,18 +2166,18 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2183,7 +2192,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -2198,22 +2207,22 @@
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="K7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="M7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2221,16 +2230,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2251,18 +2260,18 @@
         <v>50000</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2283,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>47</v>
@@ -2318,7 +2327,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2334,16 +2343,16 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2351,24 +2360,24 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="2">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2387,22 +2396,22 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="G7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -2411,25 +2420,25 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="2">
         <v>50000</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="G8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -2443,7 +2452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+    <sheetView topLeftCell="H5" workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
@@ -2466,7 +2475,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2476,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -2497,40 +2506,40 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="S2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="T2" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2538,10 +2547,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>80</v>
@@ -2565,7 +2574,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2574,25 +2583,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2600,10 +2609,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>80</v>
@@ -2627,7 +2636,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2636,25 +2645,25 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2679,7 +2688,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2689,7 +2698,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
@@ -2710,40 +2719,40 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="K8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="S8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="T8" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2751,10 +2760,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>80</v>
@@ -2778,7 +2787,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2787,30 +2796,30 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2833,43 +2842,43 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="I13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O13" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="R13" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2877,7 +2886,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>80</v>
@@ -2898,7 +2907,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2907,33 +2916,33 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S14" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
@@ -2950,16 +2959,16 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -2976,21 +2985,21 @@
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3000,7 +3009,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
@@ -3021,40 +3030,40 @@
         <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="K23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="S23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="T23" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -3062,10 +3071,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>80</v>
@@ -3089,7 +3098,7 @@
         <v>237</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L24" s="6">
         <v>1000000</v>
@@ -3098,30 +3107,30 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="R24" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="S24" s="5">
         <v>50000</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -3144,43 +3153,43 @@
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="I28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N28" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O28" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q28" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="R28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -3188,7 +3197,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>80</v>
@@ -3209,7 +3218,7 @@
         <v>237</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J29" s="6">
         <v>1000000</v>
@@ -3218,28 +3227,28 @@
         <v>445</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P29" s="5">
         <v>50000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S29" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="S29" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3252,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3368,7 +3377,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3490,7 +3499,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3595,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3627,7 +3636,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3657,7 +3666,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3665,10 +3674,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -3686,12 +3695,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3715,10 +3724,16 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>121</v>
+      <c r="I27" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3726,7 +3741,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3741,15 +3756,21 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>123</v>
+      <c r="I28" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3783,13 +3804,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -3806,7 +3827,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3817,10 +3838,16 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>121</v>
+      <c r="E37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3828,13 +3855,19 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>150</v>
+      <c r="E38" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for edit criteria
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_238_QAT\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-236\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE15DA5-064A-4201-995F-01DB5DC535DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC958D3-2BD8-4013-A8A0-BBB5B9FD2AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="170">
   <si>
     <t>corp</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>testProposedPolicyPeriod</t>
+  </si>
+  <si>
+    <t>testBrokerReturnPreviousRatingAndUWPages</t>
   </si>
 </sst>
 </file>
@@ -2049,15 +2052,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.21875" customWidth="1"/>
     <col min="3" max="3" width="38.77734375" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
@@ -2287,12 +2290,70 @@
         <v>47</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="5">
+        <v>50000</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="2">
+        <v>34534534</v>
+      </c>
+      <c r="H18" s="2">
+        <v>34534534</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2441,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added new test quote option place order
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="176">
   <si>
     <t>corp</t>
   </si>
@@ -549,6 +549,15 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>testQuoteOptionPlaceOrder</t>
+  </si>
+  <si>
+    <t>quoteStatus</t>
+  </si>
+  <si>
+    <t>Order Placed</t>
   </si>
 </sst>
 </file>
@@ -2450,10 +2459,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3251,6 +3260,33 @@
         <v>139</v>
       </c>
     </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3261,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+    <sheetView topLeftCell="E21" workbookViewId="0">
       <selection activeCell="I27" sqref="I27:J28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed rating criteria hard decline
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-236\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC958D3-2BD8-4013-A8A0-BBB5B9FD2AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76DA0A-AF6F-4D6B-8613-023C5AFF498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="173">
   <si>
     <t>corp</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>testBrokerReturnPreviousRatingAndUWPages</t>
+  </si>
+  <si>
+    <t>Ophthalmic Mutual Insurance Company (OMIC) - e-MD®/Broad Regulatory Protection Plus</t>
+  </si>
+  <si>
+    <t>Physicians</t>
+  </si>
+  <si>
+    <t>noPhysicians</t>
   </si>
 </sst>
 </file>
@@ -2054,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2070,6 +2079,7 @@
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="29.109375" customWidth="1"/>
     <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2181,7 +2191,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>110</v>
@@ -2190,30 +2200,24 @@
         <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="N7" s="2" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2222,10 +2226,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>171</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>111</v>
@@ -2234,30 +2238,24 @@
         <v>109</v>
       </c>
       <c r="F8" s="2">
-        <v>20217</v>
+        <v>4000</v>
       </c>
       <c r="G8" s="2">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2">
-        <v>8006</v>
-      </c>
-      <c r="I8" s="2">
-        <v>34534534</v>
-      </c>
-      <c r="J8" s="2">
-        <v>34534534</v>
-      </c>
-      <c r="K8" s="5">
+        <v>60</v>
+      </c>
+      <c r="I8" s="5">
         <v>50000</v>
       </c>
+      <c r="J8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="L8" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="N8" s="5" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing the failures due to test data miss
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-236\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC958D3-2BD8-4013-A8A0-BBB5B9FD2AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="173">
   <si>
     <t>corp</t>
   </si>
@@ -281,9 +280,6 @@
     <t>All Statuses</t>
   </si>
   <si>
-    <t>12/31/2021</t>
-  </si>
-  <si>
     <t>Active;Cancelled;Declined</t>
   </si>
   <si>
@@ -291,9 +287,6 @@
   </si>
   <si>
     <t>Renewed;Renewal Started;Expired</t>
-  </si>
-  <si>
-    <t>12/30/2021</t>
   </si>
   <si>
     <t>testPresenceOfContinueButtonOnQuotes</t>
@@ -541,12 +534,27 @@
   </si>
   <si>
     <t>testBrokerReturnPreviousRatingAndUWPages</t>
+  </si>
+  <si>
+    <t>testQuoteOptionPlaceOrder</t>
+  </si>
+  <si>
+    <t>quoteStatus</t>
+  </si>
+  <si>
+    <t>Order Placed</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
+  </si>
+  <si>
+    <t>12/30/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -945,7 +953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1043,11 +1051,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,7 +1114,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1114,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1144,7 +1152,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1152,10 +1160,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1182,7 +1190,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1287,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1345,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1371,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1447,7 +1455,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1464,7 +1472,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1473,7 +1481,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1561,7 +1569,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>73</v>
@@ -1616,7 +1624,7 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>80</v>
@@ -1628,7 +1636,7 @@
         <v>82</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1645,10 +1653,10 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>81</v>
@@ -1657,12 +1665,12 @@
         <v>82</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1706,16 +1714,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1732,21 +1740,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>87</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1794,7 +1802,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1834,7 +1842,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1882,7 +1890,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1930,7 +1938,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1939,10 +1947,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1950,10 +1958,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1961,15 +1969,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -2017,7 +2025,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2038,10 +2046,10 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2051,10 +2059,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2075,7 +2083,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2105,22 +2113,22 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2128,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2158,18 +2166,18 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2184,7 +2192,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -2199,22 +2207,22 @@
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2222,16 +2230,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F8" s="2">
         <v>20217</v>
@@ -2252,18 +2260,18 @@
         <v>50000</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2284,7 +2292,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>47</v>
@@ -2292,7 +2300,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2303,22 +2311,22 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2326,19 +2334,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="5">
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G18" s="2">
         <v>34534534</v>
@@ -2349,8 +2357,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2358,7 +2366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2377,7 +2385,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2393,16 +2401,16 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2410,24 +2418,24 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2446,22 +2454,22 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -2470,25 +2478,25 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C8" s="2">
         <v>50000</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -2499,11 +2507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28:S29"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2525,7 +2533,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2535,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -2556,40 +2564,40 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2597,10 +2605,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>80</v>
@@ -2624,7 +2632,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2633,25 +2641,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2659,10 +2667,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>80</v>
@@ -2686,7 +2694,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2695,25 +2703,25 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2738,7 +2746,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2748,7 +2756,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
@@ -2769,40 +2777,40 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q8" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2810,10 +2818,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>80</v>
@@ -2837,7 +2845,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2846,30 +2854,30 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2892,43 +2900,43 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="K13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="S13" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2936,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>80</v>
@@ -2957,7 +2965,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2966,33 +2974,33 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N14" s="11">
         <v>12000</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
@@ -3009,16 +3017,16 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -3035,21 +3043,21 @@
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3059,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
@@ -3080,40 +3088,40 @@
         <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="M23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q23" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -3121,10 +3129,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>80</v>
@@ -3148,7 +3156,7 @@
         <v>237</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L24" s="6">
         <v>1000000</v>
@@ -3157,30 +3165,30 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P24" s="11">
         <v>10000</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S24" s="5">
         <v>50000</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -3203,43 +3211,43 @@
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="K28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R28" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="S28" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -3247,7 +3255,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>80</v>
@@ -3268,7 +3276,7 @@
         <v>237</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J29" s="6">
         <v>1000000</v>
@@ -3277,28 +3285,50 @@
         <v>445</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N29" s="11">
         <v>12000</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P29" s="5">
         <v>50000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3308,7 +3338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3427,7 +3457,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3549,7 +3579,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3654,7 +3684,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3686,7 +3716,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3716,7 +3746,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3724,10 +3754,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -3745,12 +3775,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -3774,10 +3804,10 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3785,7 +3815,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3800,15 +3830,15 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3842,13 +3872,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -3865,7 +3895,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3876,10 +3906,10 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3887,18 +3917,18 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
added new script for qat-234
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-236\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-234\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76DA0A-AF6F-4D6B-8613-023C5AFF498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8AFAC7-890B-40A7-BB1C-9433C5193D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="174">
   <si>
     <t>corp</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>noPhysicians</t>
+  </si>
+  <si>
+    <t>testQuoteOutsideBoundSoftDeclined</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2498,10 +2501,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28:S29"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3296,6 +3299,129 @@
         <v>139</v>
       </c>
       <c r="S29" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E34" s="5">
+        <v>237</v>
+      </c>
+      <c r="F34" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G34" s="5">
+        <v>173</v>
+      </c>
+      <c r="H34" s="5">
+        <v>237</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J34" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K34" s="5">
+        <v>445</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N34" s="11">
+        <v>12000</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="P34" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="S34" s="5" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new script feature/QAT-231
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-234\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-231\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8AFAC7-890B-40A7-BB1C-9433C5193D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD44BA8-D7B4-475E-A33C-73260CFFC988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="177">
   <si>
     <t>corp</t>
   </si>
@@ -534,9 +534,6 @@
     <t>Renewal Started</t>
   </si>
   <si>
-    <t>H21OMC20060-00</t>
-  </si>
-  <si>
     <t>testProposedPolicyPeriod</t>
   </si>
   <si>
@@ -553,6 +550,18 @@
   </si>
   <si>
     <t>testQuoteOutsideBoundSoftDeclined</t>
+  </si>
+  <si>
+    <t>testQuoteSelectUnSelectCoverageGroupOption</t>
+  </si>
+  <si>
+    <t>H21NGP207660-00</t>
+  </si>
+  <si>
+    <t>$ 100k</t>
+  </si>
+  <si>
+    <t>optionCount</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2053,7 +2062,7 @@
         <v>166</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2215,7 @@
         <v>107</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>108</v>
@@ -2229,10 +2238,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>111</v>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2293,7 +2302,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2363,7 +2372,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2372,8 +2381,9 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2435,9 +2445,9 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -2458,13 +2468,9 @@
       <c r="F7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I7" s="2"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -2485,13 +2491,9 @@
       <c r="F8" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2501,15 +2503,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -3304,10 +3306,10 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3366,7 +3368,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
@@ -3423,6 +3425,135 @@
       </c>
       <c r="S34" s="5" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E39" s="5">
+        <v>237</v>
+      </c>
+      <c r="F39" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G39" s="5">
+        <v>173</v>
+      </c>
+      <c r="H39" s="5">
+        <v>237</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J39" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K39" s="5">
+        <v>445</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N39" s="11">
+        <v>12000</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="P39" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="T39" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated base and test data file.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -2370,18 +2370,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2389,11 +2390,6 @@
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2439,13 +2435,6 @@
       <c r="A6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -2509,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3185,9 +3174,53 @@
         <v>156</v>
       </c>
     </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="13"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="13"/>
+    </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -3310,7 +3343,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -3372,7 +3405,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
disabled some tests in quote tests to fix download file validation
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests_QAT-231\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD44BA8-D7B4-475E-A33C-73260CFFC988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="178">
   <si>
     <t>corp</t>
   </si>
@@ -281,9 +280,6 @@
     <t>All Statuses</t>
   </si>
   <si>
-    <t>12/31/2021</t>
-  </si>
-  <si>
     <t>Active;Cancelled;Declined</t>
   </si>
   <si>
@@ -291,9 +287,6 @@
   </si>
   <si>
     <t>Renewed;Renewal Started;Expired</t>
-  </si>
-  <si>
-    <t>12/30/2021</t>
   </si>
   <si>
     <t>testPresenceOfContinueButtonOnQuotes</t>
@@ -534,6 +527,9 @@
     <t>Renewal Started</t>
   </si>
   <si>
+    <t>H21OMC20060-00</t>
+  </si>
+  <si>
     <t>testProposedPolicyPeriod</t>
   </si>
   <si>
@@ -552,22 +548,28 @@
     <t>testQuoteOutsideBoundSoftDeclined</t>
   </si>
   <si>
-    <t>testQuoteSelectUnSelectCoverageGroupOption</t>
-  </si>
-  <si>
-    <t>H21NGP207660-00</t>
-  </si>
-  <si>
-    <t>$ 100k</t>
-  </si>
-  <si>
-    <t>optionCount</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
+  </si>
+  <si>
+    <t>12/12/2022</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -966,7 +968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1064,11 +1066,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1129,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1135,10 +1137,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1165,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1173,10 +1175,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1203,7 +1205,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1308,7 +1310,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1366,7 +1368,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1392,7 +1394,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1468,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1485,7 +1487,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1494,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1582,7 +1584,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>73</v>
@@ -1637,7 +1639,7 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>80</v>
@@ -1649,7 +1651,7 @@
         <v>82</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1666,10 +1668,10 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>81</v>
@@ -1678,12 +1680,12 @@
         <v>82</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
@@ -1727,16 +1729,16 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>87</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1753,21 +1755,21 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
@@ -1815,7 +1817,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
@@ -1855,7 +1857,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
@@ -1903,7 +1905,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
@@ -1951,7 +1953,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
@@ -1960,10 +1962,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1971,10 +1973,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1982,15 +1984,15 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
@@ -2038,7 +2040,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2059,10 +2061,10 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2072,7 +2074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2097,7 +2099,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2127,22 +2129,22 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2150,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2180,18 +2182,18 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
@@ -2203,34 +2205,34 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2238,16 +2240,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F8" s="2">
         <v>4000</v>
@@ -2262,18 +2264,18 @@
         <v>50000</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2294,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>47</v>
@@ -2302,7 +2304,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2313,22 +2315,22 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2336,19 +2338,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="5">
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G18" s="2">
         <v>34534534</v>
@@ -2359,8 +2361,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2368,35 +2370,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2404,52 +2402,44 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2457,43 +2447,49 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C8" s="2">
         <v>50000</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+        <v>138</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2502,16 +2498,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -2519,7 +2515,7 @@
     <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -2528,7 +2524,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2538,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -2559,40 +2555,40 @@
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2600,10 +2596,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>80</v>
@@ -2627,7 +2623,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L3" s="6">
         <v>1000000</v>
@@ -2636,25 +2632,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2662,10 +2658,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>80</v>
@@ -2689,7 +2685,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L4" s="6">
         <v>1000000</v>
@@ -2698,25 +2694,25 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2741,7 +2737,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2751,13 +2747,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -2772,40 +2768,40 @@
         <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="Q8" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2813,10 +2809,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>80</v>
@@ -2840,7 +2836,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L9" s="6">
         <v>1000000</v>
@@ -2849,30 +2845,30 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2895,43 +2891,43 @@
         <v>40</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="K13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="S13" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2939,7 +2935,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>80</v>
@@ -2960,7 +2956,7 @@
         <v>237</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J14" s="6">
         <v>1000000</v>
@@ -2969,36 +2965,36 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N14" s="11">
         <v>12000</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3012,19 +3008,19 @@
         <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -3038,155 +3034,167 @@
         <v>8006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>115</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>117</v>
+        <v>132</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E24" s="5">
+        <v>237</v>
+      </c>
+      <c r="F24" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G24" s="5">
+        <v>173</v>
+      </c>
+      <c r="H24" s="5">
+        <v>237</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K24" s="5">
+        <v>445</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N24" s="11">
+        <v>12000</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="P24" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="S24" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="5">
-        <v>7786</v>
-      </c>
-      <c r="G24" s="5">
-        <v>7352</v>
-      </c>
-      <c r="H24" s="5">
-        <v>3362</v>
-      </c>
-      <c r="I24" s="5">
-        <v>173</v>
-      </c>
-      <c r="J24" s="5">
-        <v>237</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="L24" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="M24" s="5">
-        <v>445</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="P24" s="11">
-        <v>10000</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="S24" s="5">
-        <v>50000</v>
-      </c>
-      <c r="T24" s="6" t="s">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -3206,51 +3214,51 @@
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="K28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="O28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R28" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="S28" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>80</v>
@@ -3271,7 +3279,7 @@
         <v>237</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J29" s="6">
         <v>1000000</v>
@@ -3280,33 +3288,33 @@
         <v>445</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N29" s="11">
         <v>12000</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P29" s="5">
         <v>50000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
@@ -3314,246 +3322,123 @@
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="M33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O33" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L33" s="4" t="s">
+      <c r="P33" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M33" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="O33" s="4" t="s">
+      <c r="Q33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="R33" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="E34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G34" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H34" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I34" s="5">
+        <v>173</v>
+      </c>
+      <c r="J34" s="5">
         <v>237</v>
       </c>
-      <c r="F34" s="5">
-        <v>8006</v>
-      </c>
-      <c r="G34" s="5">
-        <v>173</v>
-      </c>
-      <c r="H34" s="5">
-        <v>237</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J34" s="6">
+      <c r="K34" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L34" s="6">
         <v>1000000</v>
       </c>
-      <c r="K34" s="5">
+      <c r="M34" s="5">
         <v>445</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="N34" s="11">
-        <v>12000</v>
-      </c>
-      <c r="O34" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="P34" s="5">
+      <c r="N34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P34" s="11">
+        <v>10000</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S34" s="5">
         <v>50000</v>
       </c>
-      <c r="Q34" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="R34" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="S34" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P38" s="2" t="s">
+      <c r="T34" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="T38" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E39" s="5">
-        <v>237</v>
-      </c>
-      <c r="F39" s="5">
-        <v>8006</v>
-      </c>
-      <c r="G39" s="5">
-        <v>173</v>
-      </c>
-      <c r="H39" s="5">
-        <v>237</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J39" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="K39" s="5">
-        <v>445</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="N39" s="11">
-        <v>12000</v>
-      </c>
-      <c r="O39" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="P39" s="5">
-        <v>50000</v>
-      </c>
-      <c r="Q39" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="R39" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="S39" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="T39" s="2">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3563,11 +3448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3682,7 +3567,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3804,7 +3689,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3909,7 +3794,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3941,7 +3826,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -3971,7 +3856,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3979,10 +3864,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>48</v>
@@ -4000,12 +3885,12 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
@@ -4029,10 +3914,16 @@
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -4040,7 +3931,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -4055,15 +3946,21 @@
         <v>8006</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -4097,13 +3994,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -4120,7 +4017,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -4131,10 +4028,16 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -4142,18 +4045,24 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
updated add quote test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="177">
   <si>
     <t>corp</t>
   </si>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>12/12/2022</t>
-  </si>
-  <si>
-    <t>k</t>
   </si>
 </sst>
 </file>
@@ -2501,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2753,7 +2750,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Updated test data and test file names
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -15,8 +15,8 @@
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
     <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId3"/>
-    <sheet name="UnderwritingQuestionsPageData" sheetId="8" r:id="rId4"/>
-    <sheet name="QuoteOptionPageData" sheetId="9" r:id="rId5"/>
+    <sheet name="UWQuestionsPageData" sheetId="10" r:id="rId4"/>
+    <sheet name="QuotesPageData" sheetId="9" r:id="rId5"/>
     <sheet name="InsuredPageData" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -653,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -684,6 +684,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2371,14 +2374,13 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -2418,7 +2420,7 @@
       <c r="B3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2466,31 +2468,30 @@
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>50000</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="5" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2499,7 +2500,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2927,7 +2928,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -2986,12 +2987,72 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+    </row>
+    <row r="17" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+    </row>
+    <row r="18" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3016,8 +3077,19 @@
       <c r="H18" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I18" s="14"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+    </row>
+    <row r="19" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -3042,6 +3114,17 @@
       <c r="H19" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>

</xml_diff>

<commit_message>
updated tests on rc4
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -653,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -685,8 +685,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2374,7 +2383,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2500,7 +2509,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,9 +2873,19 @@
         <v>156</v>
       </c>
     </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2928,7 +2947,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -2987,538 +3006,436 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-    </row>
-    <row r="16" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-    </row>
-    <row r="17" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-    </row>
-    <row r="18" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-    </row>
-    <row r="19" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="5">
         <v>20217</v>
       </c>
-      <c r="C19" s="5">
+      <c r="E19" s="5">
         <v>237</v>
       </c>
-      <c r="D19" s="2">
+      <c r="F19" s="5">
         <v>8006</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G19" s="5">
+        <v>173</v>
+      </c>
+      <c r="H19" s="5">
+        <v>237</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K19" s="5">
+        <v>445</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N19" s="11">
+        <v>12000</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="P19" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="P23" s="2" t="s">
+      <c r="Q23" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="S23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="T23" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="E24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G24" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H24" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I24" s="5">
+        <v>173</v>
+      </c>
+      <c r="J24" s="5">
         <v>237</v>
       </c>
-      <c r="F24" s="5">
-        <v>8006</v>
-      </c>
-      <c r="G24" s="5">
-        <v>173</v>
-      </c>
-      <c r="H24" s="5">
-        <v>237</v>
-      </c>
-      <c r="I24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J24" s="6">
+      <c r="L24" s="6">
         <v>1000000</v>
       </c>
-      <c r="K24" s="5">
+      <c r="M24" s="5">
         <v>445</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="N24" s="11">
-        <v>12000</v>
-      </c>
-      <c r="O24" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="P24" s="5">
+      <c r="P24" s="11">
+        <v>10000</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S24" s="5">
         <v>50000</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="T24" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="R24" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="S24" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="5">
+      <c r="B29" s="2">
         <v>20217</v>
       </c>
-      <c r="E29" s="5">
+      <c r="C29" s="5">
         <v>237</v>
       </c>
-      <c r="F29" s="5">
+      <c r="D29" s="2">
         <v>8006</v>
       </c>
-      <c r="G29" s="5">
-        <v>173</v>
-      </c>
-      <c r="H29" s="5">
-        <v>237</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J29" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="K29" s="5">
-        <v>445</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="N29" s="11">
-        <v>12000</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="P29" s="5">
-        <v>50000</v>
-      </c>
-      <c r="Q29" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="R29" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="S29" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M33" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="L33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="N33" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>115</v>
+        <v>132</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="Q33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="S33" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="S33" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+    </row>
+    <row r="34" spans="1:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="5">
-        <v>7786</v>
-      </c>
-      <c r="G34" s="5">
-        <v>7352</v>
-      </c>
-      <c r="H34" s="5">
-        <v>3362</v>
-      </c>
-      <c r="I34" s="5">
+      <c r="D34" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E34" s="20">
+        <v>237</v>
+      </c>
+      <c r="F34" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G34" s="20">
         <v>173</v>
       </c>
-      <c r="J34" s="5">
+      <c r="H34" s="20">
         <v>237</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="I34" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L34" s="6">
+      <c r="J34" s="19">
         <v>1000000</v>
       </c>
-      <c r="M34" s="5">
+      <c r="K34" s="20">
         <v>445</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="L34" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="M34" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="P34" s="11">
-        <v>10000</v>
-      </c>
-      <c r="Q34" s="5" t="s">
+      <c r="N34" s="21">
+        <v>12000</v>
+      </c>
+      <c r="O34" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="P34" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q34" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="R34" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="R34" s="5" t="s">
+      <c r="S34" s="20" t="s">
         <v>138</v>
-      </c>
-      <c r="S34" s="5">
-        <v>50000</v>
-      </c>
-      <c r="T34" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new test in quotes updated tests after executing on master branch
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="179">
   <si>
     <t>corp</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>testSubmissionClearanceComplete</t>
-  </si>
-  <si>
-    <t>venkatqa</t>
   </si>
   <si>
     <t>venkatqa.com</t>
@@ -458,12 +455,6 @@
     <t>testLockQuote</t>
   </si>
   <si>
-    <t>My Quotes</t>
-  </si>
-  <si>
-    <t>My Policies</t>
-  </si>
-  <si>
     <t>welcomeText</t>
   </si>
   <si>
@@ -561,6 +552,21 @@
   </si>
   <si>
     <t>12/12/2022</t>
+  </si>
+  <si>
+    <t>Quotes</t>
+  </si>
+  <si>
+    <t>Policies</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>venkatqa</t>
+  </si>
+  <si>
+    <t>Select Coverage</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,13 +1103,13 @@
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1137,19 +1143,22 @@
       <c r="K2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1175,19 +1184,22 @@
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1213,11 +1225,14 @@
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1230,13 +1245,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1303,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1314,12 +1329,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1340,13 +1355,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1372,12 +1387,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1386,7 +1401,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="F16" s="2">
         <v>20217</v>
@@ -1403,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1412,7 +1427,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="F17" s="2">
         <v>25997</v>
@@ -1479,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1496,7 +1511,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1505,7 +1520,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1593,7 +1608,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>73</v>
@@ -1648,7 +1663,7 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>80</v>
@@ -1660,7 +1675,7 @@
         <v>82</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1677,7 +1692,7 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>83</v>
@@ -1689,7 +1704,7 @@
         <v>82</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1738,7 +1753,7 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>85</v>
@@ -1747,7 +1762,7 @@
         <v>82</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1764,7 +1779,7 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>85</v>
@@ -1773,7 +1788,7 @@
         <v>82</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2049,7 +2064,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2070,10 +2085,10 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2144,16 +2159,16 @@
         <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2161,7 +2176,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -2191,13 +2206,13 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -2226,22 +2241,22 @@
         <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2249,10 +2264,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>109</v>
@@ -2273,18 +2288,18 @@
         <v>50000</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2305,7 +2320,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>47</v>
@@ -2313,7 +2328,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2324,16 +2339,16 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>105</v>
@@ -2347,19 +2362,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C18" s="5">
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="G18" s="2">
         <v>34534534</v>
@@ -2410,16 +2425,16 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2427,24 +2442,24 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2455,22 +2470,22 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="G7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2478,25 +2493,25 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" s="5">
         <v>50000</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="G8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2508,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -2531,7 +2546,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2586,16 +2601,16 @@
         <v>115</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2603,10 +2618,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>80</v>
@@ -2639,25 +2654,25 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2665,10 +2680,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>80</v>
@@ -2701,25 +2716,25 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2744,7 +2759,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2799,16 +2814,16 @@
         <v>115</v>
       </c>
       <c r="Q8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="S8" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2816,10 +2831,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>80</v>
@@ -2852,25 +2867,25 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2885,7 +2900,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2932,19 +2947,19 @@
         <v>115</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -2952,7 +2967,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>80</v>
@@ -2982,33 +2997,33 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N14" s="11">
         <v>12000</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="S14" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
@@ -3055,19 +3070,19 @@
         <v>115</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S18" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3075,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>80</v>
@@ -3105,33 +3120,33 @@
         <v>445</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N19" s="11">
         <v>12000</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P19" s="5">
         <v>50000</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="S19" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
@@ -3184,16 +3199,16 @@
         <v>115</v>
       </c>
       <c r="Q23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="S23" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -3201,10 +3216,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>80</v>
@@ -3237,30 +3252,30 @@
         <v>445</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P24" s="11">
         <v>10000</v>
       </c>
       <c r="Q24" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="R24" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="S24" s="5">
         <v>50000</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -3280,13 +3295,13 @@
         <v>111</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
@@ -3303,21 +3318,21 @@
         <v>8006</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -3364,19 +3379,19 @@
         <v>115</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S33" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="S33" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3384,7 +3399,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>80</v>
@@ -3414,28 +3429,28 @@
         <v>445</v>
       </c>
       <c r="L34" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N34" s="21">
         <v>12000</v>
       </c>
       <c r="O34" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P34" s="20">
         <v>50000</v>
       </c>
       <c r="Q34" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R34" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S34" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="S34" s="20" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3449,7 +3464,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:F38"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3564,7 +3579,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -3686,7 +3701,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -3791,7 +3806,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -3861,7 +3876,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>89</v>
@@ -3882,7 +3897,7 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -3917,7 +3932,7 @@
         <v>119</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>28</v>
@@ -3928,7 +3943,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -3949,10 +3964,10 @@
         <v>121</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3991,13 +4006,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -4014,7 +4029,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -4031,7 +4046,7 @@
         <v>119</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>28</v>
@@ -4042,19 +4057,19 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed coverage group selected unselected scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="184">
   <si>
     <t>corp</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>Select Coverage</t>
+  </si>
+  <si>
+    <t>testQuoteOptionPlaceOrder</t>
+  </si>
+  <si>
+    <t>quoteStatus</t>
+  </si>
+  <si>
+    <t>Order Placed</t>
+  </si>
+  <si>
+    <t>optionCount</t>
+  </si>
+  <si>
+    <t>testQuoteOptionCoverageGroupValidation</t>
   </si>
 </sst>
 </file>
@@ -1084,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1470,57 +1485,66 @@
       <c r="H21" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="I21" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>20217</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="5">
         <v>173</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="5">
         <v>237</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="5" t="s">
         <v>175</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>25997</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>7166</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="5">
         <v>8414</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="5" t="s">
         <v>175</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2521,16 +2545,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="L34" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
@@ -2542,6 +2567,7 @@
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -3335,7 +3361,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3394,7 +3420,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -3451,6 +3477,168 @@
       </c>
       <c r="S34" s="20" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T43" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E44" s="20">
+        <v>237</v>
+      </c>
+      <c r="F44" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G44" s="20">
+        <v>173</v>
+      </c>
+      <c r="H44" s="20">
+        <v>237</v>
+      </c>
+      <c r="I44" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J44" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K44" s="20">
+        <v>445</v>
+      </c>
+      <c r="L44" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M44" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N44" s="21">
+        <v>12000</v>
+      </c>
+      <c r="O44" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P44" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q44" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R44" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S44" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="U44" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed 30385 and 28679
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="191">
   <si>
     <t>corp</t>
   </si>
@@ -582,6 +582,27 @@
   </si>
   <si>
     <t>testQuoteOptionCoverageGroupValidation</t>
+  </si>
+  <si>
+    <t>$ 15,000</t>
+  </si>
+  <si>
+    <t>claim1</t>
+  </si>
+  <si>
+    <t>claim2</t>
+  </si>
+  <si>
+    <t>$ 500k</t>
+  </si>
+  <si>
+    <t>limit2</t>
+  </si>
+  <si>
+    <t>limit1</t>
+  </si>
+  <si>
+    <t>testUpdatedOptionMaxAggLimitAndPremium</t>
   </si>
 </sst>
 </file>
@@ -674,7 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -717,6 +738,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2545,10 +2569,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L34" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3361,7 +3385,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3420,7 +3444,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -3461,7 +3485,7 @@
         <v>154</v>
       </c>
       <c r="N34" s="21">
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="O34" s="22" t="s">
         <v>130</v>
@@ -3479,12 +3503,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -3495,7 +3519,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -3506,12 +3530,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -3575,8 +3599,11 @@
       <c r="U43" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V43" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -3639,6 +3666,150 @@
       </c>
       <c r="U44" s="2">
         <v>1</v>
+      </c>
+      <c r="V44" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T48" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="V48" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E49" s="20">
+        <v>237</v>
+      </c>
+      <c r="F49" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G49" s="20">
+        <v>173</v>
+      </c>
+      <c r="H49" s="20">
+        <v>237</v>
+      </c>
+      <c r="I49" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J49" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K49" s="20">
+        <v>445</v>
+      </c>
+      <c r="L49" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="M49" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P49" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q49" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R49" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S49" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="U49" s="2">
+        <v>1</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added N2020-32172 test case
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="194">
   <si>
     <t>corp</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>testUpdatedOptionMaxAggLimitAndPremium</t>
+  </si>
+  <si>
+    <t>testQuotesByBusinessType</t>
+  </si>
+  <si>
+    <t>Renewals</t>
+  </si>
+  <si>
+    <t>New Business</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2137,6 +2146,35 @@
       </c>
       <c r="C82" s="2" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2571,7 +2609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated QAT - 262
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC51E480-BFA3-4E0F-9CC7-2A59B024E3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B4B2A6-9A11-4002-9C66-73D5C220B79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="193">
   <si>
     <t>corp</t>
   </si>
@@ -609,7 +609,7 @@
     <t>testClickingLogoNavigatesToDashboardPage</t>
   </si>
   <si>
-    <t>testWebsiteRequired</t>
+    <t>No website</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>147</v>
@@ -1446,8 +1446,8 @@
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>25</v>
+      <c r="D16" s="9" t="s">
+        <v>192</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>178</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>147</v>
@@ -2147,33 +2147,6 @@
       </c>
       <c r="C82" s="2" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clear filters test cases added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="202">
   <si>
     <t>corp</t>
   </si>
@@ -615,6 +615,27 @@
   </si>
   <si>
     <t>New Business</t>
+  </si>
+  <si>
+    <t>testClearFiltersButtonFunctionality</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>businessType</t>
+  </si>
+  <si>
+    <t>defaultProductValue</t>
+  </si>
+  <si>
+    <t>defaultStatusValue</t>
+  </si>
+  <si>
+    <t>defaultTypeValue</t>
+  </si>
+  <si>
+    <t>All Types</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M88"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,7 +2153,7 @@
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2143,7 +2164,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2154,12 +2175,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2167,7 +2188,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2175,12 +2196,63 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated testng.xml for quotes page
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B39C7D-AB45-461F-AA8D-07B7498A3343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="205">
   <si>
     <t>corp</t>
   </si>
@@ -652,7 +651,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1069,10 +1068,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1189,7 +1188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2295,7 +2294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2437,7 +2436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2724,8 +2723,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2733,7 +2732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2859,16 +2858,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
@@ -3302,18 +3301,21 @@
       <c r="S13" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="T13" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="2">
         <v>20217</v>
       </c>
       <c r="E14" s="5">
@@ -3331,25 +3333,25 @@
       <c r="I14" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>1000000</v>
       </c>
       <c r="K14" s="5">
         <v>445</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="2">
         <v>12000</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="O14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="11">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
@@ -3360,6 +3362,9 @@
       </c>
       <c r="S14" s="5" t="s">
         <v>137</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
@@ -3425,6 +3430,9 @@
       <c r="S18" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="T18" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="19" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -3483,6 +3491,9 @@
       </c>
       <c r="S19" s="5" t="s">
         <v>137</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
@@ -4110,7 +4121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -4763,7 +4774,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Hard and Soft decline scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-UWHard\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D9D8B-F9F6-4E3B-9D66-25BD59D0E294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC22332-C19E-4077-B7A2-F3E69F5C32B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="207">
   <si>
     <t>corp</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>testSoftDeclineAfterUWQuestions</t>
+  </si>
+  <si>
+    <t>Professional Athlete</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +674,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -742,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -790,6 +800,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2444,13 +2459,13 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
     <col min="3" max="3" width="38.77734375" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
@@ -2601,15 +2616,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="27" t="s">
         <v>165</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>109</v>
@@ -2618,7 +2633,7 @@
         <v>107</v>
       </c>
       <c r="F8" s="2">
-        <v>4000</v>
+        <v>100000</v>
       </c>
       <c r="G8" s="2">
         <v>60</v>
@@ -2627,10 +2642,10 @@
         <v>60</v>
       </c>
       <c r="I8" s="5">
-        <v>50000</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>153</v>
+        <v>30000000</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>136</v>
@@ -2667,6 +2682,9 @@
       <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -2740,7 +2758,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2862,85 +2880,85 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="12">
         <v>4000</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="12">
         <v>20</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="12">
         <v>20</v>
       </c>
-      <c r="I14">
-        <v>10000</v>
-      </c>
-      <c r="J14" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="12" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated login test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2952,7 +2952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+    <sheetView topLeftCell="I7" workbookViewId="0">
       <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated Binding, Dashboard and Quote page tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="207">
   <si>
     <t>corp</t>
   </si>
@@ -1089,14 +1089,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2970,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3410,6 +3410,9 @@
       <c r="S13" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="T13" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -3468,6 +3471,9 @@
       </c>
       <c r="S14" s="5" t="s">
         <v>137</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Minor change in test file
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075AE4B2-02D6-42FD-9894-7793730B9EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="210">
   <si>
     <t>corp</t>
   </si>
@@ -652,16 +653,25 @@
   </si>
   <si>
     <t>Professional Athlete</t>
+  </si>
+  <si>
+    <t>testRejectSubjectivity</t>
+  </si>
+  <si>
+    <t>submissionID1</t>
+  </si>
+  <si>
+    <t>submissionID2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,6 +690,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -751,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -805,6 +821,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1086,7 +1105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1206,7 +1225,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2312,15 +2331,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2448,13 +2470,41 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1298078</v>
+      </c>
+      <c r="C8" s="20">
+        <v>12980838</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2744,8 +2794,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2753,7 +2803,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2967,10 +3017,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
@@ -4224,7 +4274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -4877,7 +4927,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Submisson ID to Submisson Name
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075AE4B2-02D6-42FD-9894-7793730B9EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE72A0B6-F161-443A-BEBC-28D649943ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="212">
   <si>
     <t>corp</t>
   </si>
@@ -658,10 +658,16 @@
     <t>testRejectSubjectivity</t>
   </si>
   <si>
-    <t>submissionID1</t>
-  </si>
-  <si>
-    <t>submissionID2</t>
+    <t>submissionName1</t>
+  </si>
+  <si>
+    <t>Mrs. Donny Dare</t>
+  </si>
+  <si>
+    <t>submissionName2</t>
+  </si>
+  <si>
+    <t>Saul Murazik III</t>
   </si>
 </sst>
 </file>
@@ -2335,13 +2341,13 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2483,18 +2489,18 @@
         <v>208</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19">
-        <v>1298078</v>
-      </c>
-      <c r="C8" s="20">
-        <v>12980838</v>
+      <c r="B8" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed UW question scripts because as part of 334
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schabbenadusreedhar\Documents\bp-ui-tests\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-334-latest\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC3E23-F1AC-4CCF-8D9F-AD17EF1D0248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC11631-91B0-484D-938C-ABADDE9CCFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="1344" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="215">
   <si>
     <t>corp</t>
   </si>
@@ -674,6 +674,9 @@
   </si>
   <si>
     <t>submissionName3</t>
+  </si>
+  <si>
+    <t>Individual/Family - (Non-celebrity/Professional Athlete)</t>
   </si>
 </sst>
 </file>
@@ -1127,21 +1130,21 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1211,13 +1214,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1247,28 +1250,28 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.69140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" customWidth="1"/>
+    <col min="8" max="8" width="25.69140625" customWidth="1"/>
+    <col min="9" max="9" width="34.53515625" customWidth="1"/>
+    <col min="10" max="10" width="41.53515625" customWidth="1"/>
+    <col min="11" max="11" width="10.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1404,13 +1407,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1514,13 +1517,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1598,13 +1601,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1691,12 +1694,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1753,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1782,13 +1785,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1875,13 +1878,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1959,13 +1962,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -1993,7 +1996,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2007,13 +2010,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2047,13 +2050,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2095,13 +2098,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2143,13 +2146,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2182,13 +2185,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2230,14 +2233,14 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2259,12 +2262,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2280,7 +2283,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -2288,12 +2291,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -2349,25 +2352,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.765625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.69140625" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" customWidth="1"/>
+    <col min="15" max="15" width="19.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2485,13 +2488,13 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="12.65" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2533,29 +2536,29 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" customWidth="1"/>
+    <col min="3" max="3" width="38.765625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.84375" customWidth="1"/>
+    <col min="6" max="6" width="14.23046875" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.4609375" customWidth="1"/>
+    <col min="9" max="9" width="29.07421875" customWidth="1"/>
+    <col min="10" max="10" width="26.4609375" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2643,13 +2646,13 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2725,14 +2728,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2743,7 +2746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2754,15 +2757,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2828,28 +2831,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.23046875" customWidth="1"/>
+    <col min="3" max="3" width="23.53515625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.07421875" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2869,7 +2874,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2885,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>136</v>
@@ -2889,12 +2894,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2920,7 +2925,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2931,7 +2936,7 @@
         <v>50000</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>153</v>
+        <v>214</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>136</v>
@@ -2946,12 +2951,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -3003,7 +3008,7 @@
         <v>166</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>107</v>
@@ -3021,7 +3026,7 @@
         <v>100000</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>136</v>
@@ -3046,33 +3051,33 @@
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3134,7 +3139,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3196,7 +3201,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3258,7 +3263,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3278,14 +3283,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3347,7 +3352,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3409,7 +3414,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3419,12 +3424,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3486,7 +3491,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3548,12 +3553,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3612,7 +3617,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -3671,12 +3676,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -3738,7 +3743,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -3800,12 +3805,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -3831,7 +3836,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -3857,12 +3862,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -3980,12 +3985,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -3996,7 +4001,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -4007,12 +4012,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4080,7 +4085,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4148,12 +4153,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4221,7 +4226,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4303,27 +4308,27 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.07421875" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" customWidth="1"/>
+    <col min="6" max="6" width="19.69140625" customWidth="1"/>
+    <col min="7" max="7" width="15.84375" customWidth="1"/>
+    <col min="8" max="9" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.07421875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4352,7 +4357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4381,7 +4386,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4410,7 +4415,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -4439,13 +4444,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4474,7 +4479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -4503,7 +4508,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -4532,7 +4537,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4561,13 +4566,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -4602,7 +4607,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -4637,7 +4642,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -4672,13 +4677,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -4707,7 +4712,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -4736,13 +4741,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -4774,7 +4779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
@@ -4806,12 +4811,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -4837,7 +4842,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
@@ -4863,12 +4868,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -4888,7 +4893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -4908,12 +4913,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="24" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -4930,7 +4935,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
fixed failures from Jenkins execution 01
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="214">
   <si>
     <t>corp</t>
   </si>
@@ -670,6 +670,9 @@
   </si>
   <si>
     <t>testClearancesReviewFunctionality</t>
+  </si>
+  <si>
+    <t>All Coverages</t>
   </si>
 </sst>
 </file>
@@ -1236,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2317,13 +2320,13 @@
         <v>196</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>82</v>
@@ -4285,7 +4288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:B48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates in bp7 env execution
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -564,115 +564,115 @@
     <t>Coverage</t>
   </si>
   <si>
+    <t>Select Coverage</t>
+  </si>
+  <si>
+    <t>testQuoteOptionPlaceOrder</t>
+  </si>
+  <si>
+    <t>quoteStatus</t>
+  </si>
+  <si>
+    <t>Order Placed</t>
+  </si>
+  <si>
+    <t>optionCount</t>
+  </si>
+  <si>
+    <t>testQuoteOptionCoverageGroupValidation</t>
+  </si>
+  <si>
+    <t>$ 15,000</t>
+  </si>
+  <si>
+    <t>claim1</t>
+  </si>
+  <si>
+    <t>claim2</t>
+  </si>
+  <si>
+    <t>$ 500k</t>
+  </si>
+  <si>
+    <t>limit2</t>
+  </si>
+  <si>
+    <t>limit1</t>
+  </si>
+  <si>
+    <t>testUpdatedOptionMaxAggLimitAndPremium</t>
+  </si>
+  <si>
+    <t>testClickingLogoNavigatesToDashboardPage</t>
+  </si>
+  <si>
+    <t>testQuotesByBusinessType</t>
+  </si>
+  <si>
+    <t>Renewals</t>
+  </si>
+  <si>
+    <t>New Business</t>
+  </si>
+  <si>
+    <t>testClearFiltersButtonFunctionality</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>businessType</t>
+  </si>
+  <si>
+    <t>defaultProductValue</t>
+  </si>
+  <si>
+    <t>defaultStatusValue</t>
+  </si>
+  <si>
+    <t>defaultTypeValue</t>
+  </si>
+  <si>
+    <t>All Types</t>
+  </si>
+  <si>
+    <t>No website</t>
+  </si>
+  <si>
+    <t>testVerifyQuoteBinding</t>
+  </si>
+  <si>
+    <t>testResetPassword</t>
+  </si>
+  <si>
+    <t>testSoftDeclineAfterUWQuestions</t>
+  </si>
+  <si>
+    <t>Professional Athlete</t>
+  </si>
+  <si>
+    <t>testRejectSubjectivity</t>
+  </si>
+  <si>
+    <t>submissionName1</t>
+  </si>
+  <si>
+    <t>Mrs. Donny Dare</t>
+  </si>
+  <si>
+    <t>submissionName2</t>
+  </si>
+  <si>
+    <t>Saul Murazik III</t>
+  </si>
+  <si>
+    <t>testClearancesReviewFunctionality</t>
+  </si>
+  <si>
+    <t>All Coverages</t>
+  </si>
+  <si>
     <t>venkatqa</t>
-  </si>
-  <si>
-    <t>Select Coverage</t>
-  </si>
-  <si>
-    <t>testQuoteOptionPlaceOrder</t>
-  </si>
-  <si>
-    <t>quoteStatus</t>
-  </si>
-  <si>
-    <t>Order Placed</t>
-  </si>
-  <si>
-    <t>optionCount</t>
-  </si>
-  <si>
-    <t>testQuoteOptionCoverageGroupValidation</t>
-  </si>
-  <si>
-    <t>$ 15,000</t>
-  </si>
-  <si>
-    <t>claim1</t>
-  </si>
-  <si>
-    <t>claim2</t>
-  </si>
-  <si>
-    <t>$ 500k</t>
-  </si>
-  <si>
-    <t>limit2</t>
-  </si>
-  <si>
-    <t>limit1</t>
-  </si>
-  <si>
-    <t>testUpdatedOptionMaxAggLimitAndPremium</t>
-  </si>
-  <si>
-    <t>testClickingLogoNavigatesToDashboardPage</t>
-  </si>
-  <si>
-    <t>testQuotesByBusinessType</t>
-  </si>
-  <si>
-    <t>Renewals</t>
-  </si>
-  <si>
-    <t>New Business</t>
-  </si>
-  <si>
-    <t>testClearFiltersButtonFunctionality</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>businessType</t>
-  </si>
-  <si>
-    <t>defaultProductValue</t>
-  </si>
-  <si>
-    <t>defaultStatusValue</t>
-  </si>
-  <si>
-    <t>defaultTypeValue</t>
-  </si>
-  <si>
-    <t>All Types</t>
-  </si>
-  <si>
-    <t>No website</t>
-  </si>
-  <si>
-    <t>testVerifyQuoteBinding</t>
-  </si>
-  <si>
-    <t>testResetPassword</t>
-  </si>
-  <si>
-    <t>testSoftDeclineAfterUWQuestions</t>
-  </si>
-  <si>
-    <t>Professional Athlete</t>
-  </si>
-  <si>
-    <t>testRejectSubjectivity</t>
-  </si>
-  <si>
-    <t>submissionName1</t>
-  </si>
-  <si>
-    <t>Mrs. Donny Dare</t>
-  </si>
-  <si>
-    <t>submissionName2</t>
-  </si>
-  <si>
-    <t>Saul Murazik III</t>
-  </si>
-  <si>
-    <t>testClearancesReviewFunctionality</t>
-  </si>
-  <si>
-    <t>All Coverages</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -1239,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
@@ -1553,10 +1553,10 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" s="2">
         <v>20217</v>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F17" s="2">
         <v>25997</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2273,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -2281,12 +2281,12 @@
         <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -2300,16 +2300,16 @@
         <v>22</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="F92" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F92" s="4" t="s">
+      <c r="G92" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -2317,22 +2317,22 @@
         <v>3</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2359,7 +2359,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -2483,7 +2483,7 @@
     <row r="5" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -2491,10 +2491,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -2502,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2705,7 +2705,7 @@
         <v>30000000</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>136</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -3010,7 +3010,7 @@
         <v>100000</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>136</v>
@@ -3472,7 +3472,7 @@
         <v>134</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
@@ -3971,7 +3971,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
@@ -3982,7 +3982,7 @@
         <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
@@ -3993,12 +3993,12 @@
         <v>147</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
@@ -4063,7 +4063,7 @@
         <v>113</v>
       </c>
       <c r="U43" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V43" s="4" t="s">
         <v>115</v>
@@ -4134,12 +4134,12 @@
         <v>1</v>
       </c>
       <c r="V44" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
@@ -4177,10 +4177,10 @@
         <v>106</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>115</v>
@@ -4201,13 +4201,13 @@
         <v>134</v>
       </c>
       <c r="T48" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U48" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V48" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4245,13 +4245,13 @@
         <v>445</v>
       </c>
       <c r="L49" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N49" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O49" s="22" t="s">
         <v>130</v>
@@ -4288,14 +4288,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:B48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.109375" customWidth="1"/>
     <col min="5" max="5" width="28.88671875" customWidth="1"/>
@@ -4834,7 +4834,7 @@
         <v>147</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>123</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -4938,7 +4938,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated the scripts with OMIC product
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="216">
   <si>
     <t>corp</t>
   </si>
@@ -673,6 +673,12 @@
   </si>
   <si>
     <t>venkatqa</t>
+  </si>
+  <si>
+    <t>businessClass3</t>
+  </si>
+  <si>
+    <t>physiciansCount</t>
   </si>
 </sst>
 </file>
@@ -2343,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,12 +2363,12 @@
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2420,8 +2426,20 @@
       <c r="S2" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2479,14 +2497,26 @@
       <c r="S3" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U3" s="5">
+        <v>50</v>
+      </c>
+      <c r="V3" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="W3" s="20">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2497,7 +2527,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2516,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2536,15 +2566,17 @@
     <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2587,8 +2619,20 @@
       <c r="N2" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2631,14 +2675,26 @@
       <c r="N3" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="P3" s="5">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="R3" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2676,7 +2732,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2714,14 +2770,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2732,7 +2788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2743,15 +2799,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2776,8 +2832,14 @@
       <c r="H17" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2797,10 +2859,16 @@
         <v>137</v>
       </c>
       <c r="G18" s="2">
-        <v>34534534</v>
+        <v>100000</v>
       </c>
       <c r="H18" s="2">
-        <v>34534534</v>
+        <v>60</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J18" s="5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3029,10 +3097,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView topLeftCell="J25" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3051,17 +3119,18 @@
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3122,8 +3191,14 @@
       <c r="T2" s="16" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3184,8 +3259,14 @@
       <c r="T3" s="18" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="V3" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3246,8 +3327,14 @@
       <c r="T4" s="18" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="V4" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3267,14 +3354,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3335,8 +3422,14 @@
       <c r="T8" s="16" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3397,8 +3490,14 @@
       <c r="T9" s="18" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="V9" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3408,12 +3507,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3474,8 +3573,14 @@
       <c r="T13" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U13" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3536,13 +3641,19 @@
       <c r="T14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U14" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="V14" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3600,8 +3711,14 @@
       <c r="S18" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -3659,13 +3776,19 @@
       <c r="S19" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T19" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U19" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -3726,8 +3849,14 @@
       <c r="T23" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U23" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -3788,13 +3917,19 @@
       <c r="T24" s="6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="V24" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -3820,7 +3955,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -3846,12 +3981,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3909,8 +4044,14 @@
       <c r="S33" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -3968,13 +4109,19 @@
       <c r="S34" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T34" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U34" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -3985,7 +4132,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -3996,12 +4143,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4068,8 +4215,14 @@
       <c r="V43" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W43" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X43" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4136,13 +4289,19 @@
       <c r="V44" s="23" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W44" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="X44" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4209,8 +4368,14 @@
       <c r="V48" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W48" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X48" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4276,6 +4441,12 @@
       </c>
       <c r="V49" s="2" t="s">
         <v>154</v>
+      </c>
+      <c r="W49" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="X49" s="5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4288,7 +4459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added premium not required test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-qat-33555\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B909EA08-77B4-42D7-9AFE-E451D4B40682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="45972" yWindow="1344" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="219">
   <si>
     <t>corp</t>
   </si>
@@ -679,12 +680,21 @@
   </si>
   <si>
     <t>physiciansCount</t>
+  </si>
+  <si>
+    <t>testNotDisplayPremiumIfReviewRequired</t>
+  </si>
+  <si>
+    <t>Individual/Family - (Non-celebrity/Professional Athlete)</t>
+  </si>
+  <si>
+    <t>$ 100k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1122,28 +1132,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1157,7 +1167,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1209,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1213,13 +1223,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1242,35 +1252,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.69140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" customWidth="1"/>
+    <col min="8" max="8" width="25.69140625" customWidth="1"/>
+    <col min="9" max="9" width="34.53515625" customWidth="1"/>
+    <col min="10" max="10" width="41.53515625" customWidth="1"/>
+    <col min="11" max="11" width="10.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1352,7 +1362,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1393,7 +1403,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1406,13 +1416,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1438,7 +1448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1474,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1490,7 +1500,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1516,13 +1526,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1584,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1600,13 +1610,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1664,7 +1674,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1693,12 +1703,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +1762,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1784,13 +1794,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1819,7 +1829,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1848,7 +1858,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1877,13 +1887,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1909,7 +1919,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1935,7 +1945,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1961,13 +1971,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +1991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -1995,7 +2005,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2009,13 +2019,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2032,7 +2042,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2049,13 +2059,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2097,13 +2107,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2117,7 +2127,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2141,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2145,13 +2155,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -2162,7 +2172,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2173,7 +2183,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2184,13 +2194,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -2204,7 +2214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2218,7 +2228,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2232,14 +2242,14 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2250,7 +2260,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2261,12 +2271,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2282,7 +2292,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -2290,12 +2300,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -2318,7 +2328,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -2348,27 +2358,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2:W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.765625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="19.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2439,7 +2449,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2510,13 +2520,13 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="12.65" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2527,7 +2537,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2545,38 +2555,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" customWidth="1"/>
+    <col min="3" max="3" width="38.765625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.84375" customWidth="1"/>
+    <col min="6" max="6" width="14.23046875" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.4609375" customWidth="1"/>
+    <col min="9" max="9" width="29.07421875" customWidth="1"/>
+    <col min="10" max="10" width="26.4609375" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2632,7 +2642,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>136</v>
@@ -2688,13 +2698,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2732,7 +2742,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2770,14 +2780,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2788,7 +2798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2799,15 +2809,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2839,7 +2849,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>136</v>
@@ -2873,8 +2883,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -2882,31 +2892,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.69140625" customWidth="1"/>
+    <col min="4" max="4" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2926,7 +2936,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2946,12 +2956,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +2987,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3003,12 +3013,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -3049,7 +3059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -3096,41 +3106,41 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView topLeftCell="J25" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33:U34"/>
+    <sheetView tabSelected="1" topLeftCell="K40" workbookViewId="0">
+      <selection activeCell="T49" sqref="T49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3208,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3266,7 +3276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3334,7 +3344,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3354,14 +3364,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3429,7 +3439,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3497,7 +3507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3507,12 +3517,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3580,7 +3590,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3648,12 +3658,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3718,7 +3728,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -3783,12 +3793,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -3856,7 +3866,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -3924,12 +3934,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -3955,7 +3965,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -3981,12 +3991,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -4051,7 +4061,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -4116,12 +4126,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4132,7 +4142,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -4143,12 +4153,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4222,7 +4232,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4296,12 +4306,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4375,7 +4385,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4446,6 +4456,159 @@
         <v>166</v>
       </c>
       <c r="X49" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T54" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="U54" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="V54" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="W54" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X54" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A55" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E55" s="20">
+        <v>237</v>
+      </c>
+      <c r="F55" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G55" s="20">
+        <v>173</v>
+      </c>
+      <c r="H55" s="20">
+        <v>237</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J55" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K55" s="20">
+        <v>445</v>
+      </c>
+      <c r="L55" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="M55" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="O55" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P55" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q55" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="R55" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S55" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="U55" s="2">
+        <v>1</v>
+      </c>
+      <c r="V55" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="W55" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="X55" s="5">
         <v>50</v>
       </c>
     </row>
@@ -4456,34 +4619,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.07421875" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" customWidth="1"/>
+    <col min="6" max="6" width="19.69140625" customWidth="1"/>
+    <col min="7" max="7" width="15.84375" customWidth="1"/>
+    <col min="8" max="9" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.07421875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4512,7 +4675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4541,7 +4704,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4570,7 +4733,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -4599,13 +4762,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4634,7 +4797,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -4663,7 +4826,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -4692,7 +4855,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4721,13 +4884,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -4762,7 +4925,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -4797,7 +4960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -4832,13 +4995,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -4867,7 +5030,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -4896,13 +5059,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -4934,7 +5097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
@@ -4966,12 +5129,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -4997,7 +5160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
@@ -5023,12 +5186,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5048,7 +5211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -5068,12 +5231,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -5090,7 +5253,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -5107,12 +5270,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="24" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -5120,7 +5283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -5130,7 +5293,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
added filesize validation test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="217">
   <si>
     <t>corp</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>physiciansCount</t>
+  </si>
+  <si>
+    <t>testFileSizeValidationForBinder</t>
   </si>
 </sst>
 </file>
@@ -2349,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,6 +2541,153 @@
         <v>210</v>
       </c>
     </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E13" s="20">
+        <v>237</v>
+      </c>
+      <c r="F13" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G13" s="20">
+        <v>173</v>
+      </c>
+      <c r="H13" s="20">
+        <v>237</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="20">
+        <v>445</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N13" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P13" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q13" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U13" s="5">
+        <v>50</v>
+      </c>
+      <c r="V13" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="W13" s="20">
+        <v>445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2548,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
e2e workflow is added added test to check clearances for renewal policy
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="219">
   <si>
     <t>corp</t>
   </si>
@@ -682,6 +682,12 @@
   </si>
   <si>
     <t>testFileSizeValidationForBinder</t>
+  </si>
+  <si>
+    <t>testEndToEndWorkflow</t>
+  </si>
+  <si>
+    <t>testRenewalPolicyClearanceValidation</t>
   </si>
 </sst>
 </file>
@@ -2352,15 +2358,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -2685,6 +2691,153 @@
         <v>1000000</v>
       </c>
       <c r="W13" s="20">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E18" s="20">
+        <v>237</v>
+      </c>
+      <c r="F18" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G18" s="20">
+        <v>173</v>
+      </c>
+      <c r="H18" s="20">
+        <v>237</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K18" s="20">
+        <v>445</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N18" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P18" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S18" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U18" s="5">
+        <v>50</v>
+      </c>
+      <c r="V18" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="W18" s="20">
         <v>445</v>
       </c>
     </row>
@@ -4607,10 +4760,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5278,6 +5431,27 @@
         <v>147</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K18" r:id="rId1"/>

</xml_diff>

<commit_message>
add test for quote ineligible policy
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-394\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BC73AB-AEFF-4D59-AFAC-6D9339EF13FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-33017" yWindow="-5460" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="219">
   <si>
     <t>corp</t>
   </si>
@@ -682,12 +683,18 @@
   </si>
   <si>
     <t>testFileSizeValidationForBinder</t>
+  </si>
+  <si>
+    <t>testIneligiblePolicies</t>
+  </si>
+  <si>
+    <t>H22NGP217535-00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1125,7 +1132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1245,11 +1252,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,6 +2351,35 @@
         <v>200</v>
       </c>
     </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2351,10 +2387,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2695,7 +2731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3023,8 +3059,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -3032,7 +3068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3246,7 +3282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView topLeftCell="J25" workbookViewId="0">
@@ -4606,7 +4642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -5280,7 +5316,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
added application download test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-394\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-434\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BC73AB-AEFF-4D59-AFAC-6D9339EF13FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65F73FE-E479-4FCE-81B0-A564C540251E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-5460" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="220">
   <si>
     <t>corp</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>H22NGP217535-00</t>
+  </si>
+  <si>
+    <t>testDownloadApplicationInQuote</t>
   </si>
 </sst>
 </file>
@@ -1139,21 +1142,21 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1223,13 +1226,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1255,32 +1258,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.69140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" customWidth="1"/>
+    <col min="8" max="8" width="25.69140625" customWidth="1"/>
+    <col min="9" max="9" width="34.53515625" customWidth="1"/>
+    <col min="10" max="10" width="41.53515625" customWidth="1"/>
+    <col min="11" max="11" width="10.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1416,13 +1419,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1526,13 +1529,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1610,13 +1613,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1703,12 +1706,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1765,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1794,13 +1797,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1887,13 +1890,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1971,13 +1974,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2019,13 +2022,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2059,13 +2062,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2107,13 +2110,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2155,13 +2158,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2194,13 +2197,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2242,14 +2245,14 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2271,12 +2274,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2292,7 +2295,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -2300,12 +2303,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -2351,14 +2354,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>2</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>3</v>
       </c>
@@ -2394,20 +2397,20 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.765625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="19.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2549,13 +2552,13 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="12.65" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2566,7 +2569,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2577,12 +2580,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
@@ -2738,31 +2741,31 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" customWidth="1"/>
+    <col min="3" max="3" width="38.765625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.84375" customWidth="1"/>
+    <col min="6" max="6" width="14.23046875" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.4609375" customWidth="1"/>
+    <col min="9" max="9" width="29.07421875" customWidth="1"/>
+    <col min="10" max="10" width="26.4609375" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2874,13 +2877,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2956,14 +2959,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2985,15 +2988,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -3075,24 +3078,24 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.69140625" customWidth="1"/>
+    <col min="4" max="4" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3132,12 +3135,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -3163,7 +3166,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3189,12 +3192,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -3235,7 +3238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -3283,40 +3286,40 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X49"/>
+  <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView topLeftCell="J25" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33:U34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3384,7 +3387,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3520,7 +3523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3540,14 +3543,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3615,7 +3618,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3683,7 +3686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3693,12 +3696,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3834,12 +3837,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3904,7 +3907,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -3969,12 +3972,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -4042,7 +4045,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -4110,12 +4113,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -4167,12 +4170,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -4302,12 +4305,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4318,7 +4321,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -4329,12 +4332,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4408,7 +4411,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4482,12 +4485,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4561,7 +4564,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4634,6 +4637,78 @@
       <c r="X49" s="5">
         <v>50</v>
       </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C58" s="5">
+        <v>237</v>
+      </c>
+      <c r="D58" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4649,27 +4724,27 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.07421875" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" customWidth="1"/>
+    <col min="6" max="6" width="19.69140625" customWidth="1"/>
+    <col min="7" max="7" width="15.84375" customWidth="1"/>
+    <col min="8" max="9" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.07421875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4698,7 +4773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4727,7 +4802,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4756,7 +4831,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -4785,13 +4860,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4820,7 +4895,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -4849,7 +4924,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -4878,7 +4953,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -4907,13 +4982,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -4948,7 +5023,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -4983,7 +5058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -5018,13 +5093,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -5053,7 +5128,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -5082,13 +5157,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -5120,7 +5195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
@@ -5152,12 +5227,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -5183,7 +5258,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
@@ -5209,12 +5284,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5234,7 +5309,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -5254,12 +5329,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -5276,7 +5351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -5293,12 +5368,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="24" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -5306,7 +5381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
QAT-431 still pending as it needs interaction with Snap application Updated/refactored many scripts Fixed some failures
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-394\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BC73AB-AEFF-4D59-AFAC-6D9339EF13FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-5460" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33012" yWindow="-5460" windowWidth="33120" windowHeight="18120" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="221">
   <si>
     <t>corp</t>
   </si>
@@ -689,12 +688,18 @@
   </si>
   <si>
     <t>H22NGP217535-00</t>
+  </si>
+  <si>
+    <t>$ 100K</t>
+  </si>
+  <si>
+    <t>$ 250K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1132,7 +1137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1252,10 +1257,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
@@ -2387,27 +2392,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2471,14 +2479,8 @@
       <c r="U2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2507,10 +2509,10 @@
         <v>116</v>
       </c>
       <c r="J3" s="19">
-        <v>1000000</v>
+        <v>44</v>
       </c>
       <c r="K3" s="20">
-        <v>445</v>
+        <v>44</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>154</v>
@@ -2536,26 +2538,20 @@
       <c r="S3" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="U3" s="5">
-        <v>50</v>
-      </c>
-      <c r="V3" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="W3" s="20">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="U3" s="20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2566,7 +2562,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2577,12 +2573,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2646,14 +2642,8 @@
       <c r="U12" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="V12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
@@ -2682,10 +2672,10 @@
         <v>116</v>
       </c>
       <c r="J13" s="19">
-        <v>1000000</v>
+        <v>44</v>
       </c>
       <c r="K13" s="20">
-        <v>445</v>
+        <v>44</v>
       </c>
       <c r="L13" s="20" t="s">
         <v>154</v>
@@ -2711,17 +2701,11 @@
       <c r="S13" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="U13" s="5">
-        <v>50</v>
-      </c>
-      <c r="V13" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="W13" s="20">
-        <v>445</v>
+      <c r="U13" s="20">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2731,7 +2715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3059,8 +3043,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -3068,23 +3052,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3097,39 +3084,57 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>134</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="5">
         <v>50000</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" s="2" t="s">
         <v>137</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="12">
+        <v>44</v>
+      </c>
+      <c r="H3" s="12">
+        <v>44</v>
+      </c>
+      <c r="I3" s="12">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3137,56 +3142,74 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>134</v>
+      <c r="H7" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="5">
         <v>50000</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="D8" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>137</v>
+      <c r="H8" s="12">
+        <v>44</v>
+      </c>
+      <c r="I8" s="12">
+        <v>44</v>
+      </c>
+      <c r="J8" s="12">
+        <v>44</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -3194,86 +3217,86 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>105</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>147</v>
+      <c r="B14" s="12" t="s">
+        <v>166</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="12">
+        <v>44</v>
+      </c>
+      <c r="F14" s="12">
+        <v>44</v>
+      </c>
+      <c r="G14" s="12">
+        <v>44</v>
+      </c>
+      <c r="H14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="12">
-        <v>4000</v>
-      </c>
-      <c r="G14" s="12">
-        <v>20</v>
-      </c>
-      <c r="H14" s="12">
-        <v>20</v>
-      </c>
-      <c r="I14" s="12">
-        <v>100000</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3282,11 +3305,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="J25" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33:U34"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3656,10 +3679,10 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>154</v>
+        <v>220</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
@@ -4642,7 +4665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -5316,7 +5339,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added test for Bindre documents uplaod
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-391111\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B899F23-4689-4B16-B96C-488DAE3EA04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="222">
   <si>
     <t>corp</t>
   </si>
@@ -691,12 +692,18 @@
   </si>
   <si>
     <t>testDownloadApplicationInQuote</t>
+  </si>
+  <si>
+    <t>testDownloadBinder</t>
+  </si>
+  <si>
+    <t>Binder_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1134,28 +1141,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1183,7 +1190,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1225,13 +1232,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1246,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1254,35 +1261,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.69140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5546875" customWidth="1"/>
-    <col min="10" max="10" width="41.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" customWidth="1"/>
+    <col min="8" max="8" width="25.69140625" customWidth="1"/>
+    <col min="9" max="9" width="34.53515625" customWidth="1"/>
+    <col min="10" max="10" width="41.53515625" customWidth="1"/>
+    <col min="11" max="11" width="10.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1323,7 +1330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1364,7 +1371,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1405,7 +1412,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1418,13 +1425,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1528,13 +1535,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1593,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1612,13 +1619,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1647,7 +1654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1705,12 +1712,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1742,7 +1749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1771,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1796,13 +1803,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1831,7 +1838,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1860,7 +1867,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1889,13 +1896,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1921,7 +1928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1947,7 +1954,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1973,13 +1980,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1993,7 +2000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2021,13 +2028,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2051,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2061,13 +2068,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2081,7 +2088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2095,7 +2102,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2109,13 +2116,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2129,7 +2136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -2143,7 +2150,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2157,13 +2164,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -2174,7 +2181,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2185,7 +2192,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2196,13 +2203,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -2216,7 +2223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2244,14 +2251,14 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2262,7 +2269,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2273,12 +2280,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +2293,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2294,7 +2301,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -2302,12 +2309,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -2353,14 +2360,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2378,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>3</v>
       </c>
@@ -2389,27 +2396,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.765625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="19.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2551,13 +2558,13 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="12.65" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2568,7 +2575,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2579,12 +2586,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2655,7 +2662,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
@@ -2724,6 +2731,56 @@
       </c>
       <c r="W13" s="20">
         <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A19" s="28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2733,38 +2790,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" customWidth="1"/>
+    <col min="3" max="3" width="38.765625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.84375" customWidth="1"/>
+    <col min="6" max="6" width="14.23046875" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" customWidth="1"/>
+    <col min="8" max="8" width="17.4609375" customWidth="1"/>
+    <col min="9" max="9" width="29.07421875" customWidth="1"/>
+    <col min="10" max="10" width="26.4609375" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2820,7 +2877,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2876,13 +2933,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2920,7 +2977,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2958,14 +3015,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2976,7 +3033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2987,15 +3044,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -3027,7 +3084,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -3061,8 +3118,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -3070,31 +3127,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.69140625" customWidth="1"/>
+    <col min="4" max="4" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3114,7 +3171,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3134,12 +3191,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -3165,7 +3222,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3191,12 +3248,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -3237,7 +3294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -3284,41 +3341,41 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:H62"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I63" sqref="A60:I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3386,7 +3443,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3454,7 +3511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3522,7 +3579,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3542,14 +3599,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3617,7 +3674,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3685,7 +3742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3695,12 +3752,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3768,7 +3825,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3836,12 +3893,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3906,7 +3963,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -3971,12 +4028,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -4044,7 +4101,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -4112,12 +4169,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -4143,7 +4200,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -4169,12 +4226,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -4239,7 +4296,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -4304,12 +4361,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4320,7 +4377,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -4331,12 +4388,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4410,7 +4467,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4484,12 +4541,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4563,7 +4620,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4637,10 +4694,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -4650,7 +4707,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="5"/>
@@ -4660,12 +4717,12 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -4691,7 +4748,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -4717,12 +4774,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -4748,7 +4805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
@@ -4781,34 +4838,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.07421875" customWidth="1"/>
+    <col min="5" max="5" width="28.84375" customWidth="1"/>
+    <col min="6" max="6" width="19.69140625" customWidth="1"/>
+    <col min="7" max="7" width="15.84375" customWidth="1"/>
+    <col min="8" max="9" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.07421875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4837,7 +4894,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4866,7 +4923,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4895,7 +4952,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -4924,13 +4981,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4959,7 +5016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -4988,7 +5045,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -5017,7 +5074,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -5046,13 +5103,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -5087,7 +5144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -5122,7 +5179,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -5157,13 +5214,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -5192,7 +5249,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -5221,13 +5278,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -5259,7 +5316,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
@@ -5291,12 +5348,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -5322,7 +5379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
@@ -5348,12 +5405,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5373,7 +5430,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -5393,12 +5450,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -5415,7 +5472,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -5432,12 +5489,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="24" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -5445,7 +5502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -5455,7 +5512,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
completed QAT-459 and some integration bugs
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-391111\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B899F23-4689-4B16-B96C-488DAE3EA04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="223">
   <si>
     <t>corp</t>
   </si>
@@ -698,12 +697,15 @@
   </si>
   <si>
     <t>Binder_</t>
+  </si>
+  <si>
+    <t>testContactUnderwriterModal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1141,28 +1143,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1176,7 +1178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1190,7 +1192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1220,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1232,13 +1234,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1261,35 +1263,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="23.3046875" customWidth="1"/>
-    <col min="8" max="8" width="25.69140625" customWidth="1"/>
-    <col min="9" max="9" width="34.53515625" customWidth="1"/>
-    <col min="10" max="10" width="41.53515625" customWidth="1"/>
-    <col min="11" max="11" width="10.3046875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.5546875" customWidth="1"/>
+    <col min="10" max="10" width="41.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1412,7 +1414,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1425,13 +1427,13 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1511,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1535,13 +1537,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1593,7 +1595,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1619,13 +1621,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1712,12 +1714,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1771,7 +1773,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1803,13 +1805,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1838,7 +1840,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -1896,13 +1898,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1928,7 +1930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1980,13 +1982,13 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +2002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2016,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2028,13 +2030,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2051,7 +2053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
@@ -2068,13 +2070,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2102,7 +2104,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2116,13 +2118,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2136,7 +2138,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2152,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>4</v>
       </c>
@@ -2164,13 +2166,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -2203,13 +2205,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>2</v>
       </c>
@@ -2223,7 +2225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2239,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -2251,14 +2253,14 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -2280,12 +2282,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
@@ -2293,7 +2295,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -2309,12 +2311,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -2360,14 +2362,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>2</v>
       </c>
@@ -2378,7 +2380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>3</v>
       </c>
@@ -2396,27 +2398,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.765625" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.69140625" customWidth="1"/>
-    <col min="15" max="15" width="19.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2480,14 +2487,8 @@
       <c r="U2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2516,10 +2517,10 @@
         <v>116</v>
       </c>
       <c r="J3" s="19">
-        <v>1000000</v>
+        <v>45</v>
       </c>
       <c r="K3" s="20">
-        <v>445</v>
+        <v>45</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>154</v>
@@ -2549,22 +2550,16 @@
         <v>166</v>
       </c>
       <c r="U3" s="5">
-        <v>50</v>
-      </c>
-      <c r="V3" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="W3" s="20">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="12.65" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
@@ -2586,12 +2581,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2655,14 +2650,8 @@
       <c r="U12" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="V12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
@@ -2691,10 +2680,10 @@
         <v>116</v>
       </c>
       <c r="J13" s="19">
-        <v>1000000</v>
+        <v>45</v>
       </c>
       <c r="K13" s="20">
-        <v>445</v>
+        <v>45</v>
       </c>
       <c r="L13" s="20" t="s">
         <v>154</v>
@@ -2724,19 +2713,13 @@
         <v>166</v>
       </c>
       <c r="U13" s="5">
-        <v>50</v>
-      </c>
-      <c r="V13" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="W13" s="20">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2746,7 +2729,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5"/>
@@ -2756,12 +2739,12 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2772,7 +2755,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>3</v>
       </c>
@@ -2781,6 +2764,141 @@
       </c>
       <c r="C21" s="20" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E26" s="20">
+        <v>237</v>
+      </c>
+      <c r="F26" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G26" s="20">
+        <v>173</v>
+      </c>
+      <c r="H26" s="20">
+        <v>237</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="19">
+        <v>45</v>
+      </c>
+      <c r="K26" s="20">
+        <v>45</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N26" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O26" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P26" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q26" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R26" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U26" s="5">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2790,38 +2908,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.07421875" customWidth="1"/>
-    <col min="3" max="3" width="38.765625" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="21.84375" customWidth="1"/>
-    <col min="6" max="6" width="14.23046875" customWidth="1"/>
-    <col min="7" max="7" width="16.69140625" customWidth="1"/>
-    <col min="8" max="8" width="17.4609375" customWidth="1"/>
-    <col min="9" max="9" width="29.07421875" customWidth="1"/>
-    <col min="10" max="10" width="26.4609375" customWidth="1"/>
-    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2877,7 +2995,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2933,13 +3051,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +3095,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3015,14 +3133,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -3033,7 +3151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -3044,15 +3162,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -3084,7 +3202,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -3118,8 +3236,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.profrisk.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -3127,31 +3245,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.69140625" customWidth="1"/>
-    <col min="4" max="4" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3171,7 +3289,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3191,12 +3309,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -3222,7 +3340,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -3248,12 +3366,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -3294,7 +3412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -3341,41 +3459,41 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="I63" sqref="A60:I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.07421875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.07421875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.23046875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3443,7 +3561,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3511,7 +3629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3579,7 +3697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -3599,14 +3717,14 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -3674,7 +3792,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3742,7 +3860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="14"/>
@@ -3752,12 +3870,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3825,7 +3943,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -3893,12 +4011,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -3963,7 +4081,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -4028,12 +4146,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -4101,7 +4219,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -4169,12 +4287,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -4200,7 +4318,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -4226,12 +4344,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -4296,7 +4414,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
@@ -4361,12 +4479,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4377,7 +4495,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
@@ -4388,12 +4506,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -4467,7 +4585,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>3</v>
       </c>
@@ -4541,12 +4659,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -4620,7 +4738,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
         <v>3</v>
       </c>
@@ -4694,10 +4812,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -4707,7 +4825,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="5"/>
@@ -4717,12 +4835,12 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -4748,7 +4866,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>3</v>
       </c>
@@ -4774,12 +4892,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -4805,7 +4923,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
@@ -4838,34 +4956,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.07421875" customWidth="1"/>
-    <col min="5" max="5" width="28.84375" customWidth="1"/>
-    <col min="6" max="6" width="19.69140625" customWidth="1"/>
-    <col min="7" max="7" width="15.84375" customWidth="1"/>
-    <col min="8" max="9" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4894,7 +5012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -4923,7 +5041,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4952,7 +5070,7 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -4981,13 +5099,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -5016,7 +5134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -5045,7 +5163,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -5074,7 +5192,7 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -5103,13 +5221,13 @@
         <v>8414</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -5144,7 +5262,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -5179,7 +5297,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -5214,13 +5332,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -5249,7 +5367,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -5278,13 +5396,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -5316,7 +5434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
@@ -5348,12 +5466,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -5379,7 +5497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
@@ -5405,12 +5523,12 @@
         <v>8006</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5430,7 +5548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -5450,12 +5568,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -5472,7 +5590,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -5489,12 +5607,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -5502,7 +5620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -5512,7 +5630,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="K18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
QAT-546 and 542 completed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18120" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18120" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPageData" sheetId="5" r:id="rId2"/>
-    <sheet name="BindingPageData" sheetId="11" r:id="rId3"/>
+    <sheet name="InsuredPageData" sheetId="6" r:id="rId3"/>
     <sheet name="RatingCriteriaPageData" sheetId="7" r:id="rId4"/>
     <sheet name="UWQuestionsPageData" sheetId="10" r:id="rId5"/>
     <sheet name="QuotesPageData" sheetId="9" r:id="rId6"/>
-    <sheet name="InsuredPageData" sheetId="6" r:id="rId7"/>
+    <sheet name="BindingPageData" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="228">
   <si>
     <t>corp</t>
   </si>
@@ -699,7 +699,22 @@
     <t>Binder_</t>
   </si>
   <si>
-    <t>testContactUnderwriterModal</t>
+    <t>quoteOptionStatus</t>
+  </si>
+  <si>
+    <t>Option Order</t>
+  </si>
+  <si>
+    <t>testConfirmDatesModal</t>
+  </si>
+  <si>
+    <t>Ready to Place Order</t>
+  </si>
+  <si>
+    <t>testContactUnderwriterModalBeforeLock</t>
+  </si>
+  <si>
+    <t>testContactUnderwriterModalAfterLock</t>
   </si>
 </sst>
 </file>
@@ -2399,511 +2414,683 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="19" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H3" s="5">
+        <v>173</v>
+      </c>
+      <c r="I3" s="5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="C5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="5">
         <v>20217</v>
       </c>
-      <c r="E3" s="20">
+      <c r="H10" s="5">
+        <v>173</v>
+      </c>
+      <c r="I10" s="5">
         <v>237</v>
       </c>
-      <c r="F3" s="20">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H11" s="5">
+        <v>237</v>
+      </c>
+      <c r="I11" s="5">
         <v>8006</v>
       </c>
-      <c r="G3" s="20">
-        <v>173</v>
-      </c>
-      <c r="H3" s="20">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I12" s="2">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="5">
+        <v>20217</v>
+      </c>
+      <c r="H17" s="5">
         <v>237</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="19">
+      <c r="I17" s="5">
+        <v>8006</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2">
+        <v>25997</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7166</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8414</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="20">
+      <c r="F22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G23" s="5">
+        <v>237</v>
+      </c>
+      <c r="H23" s="5">
+        <v>8006</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N3" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S3" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U3" s="5">
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5">
+        <v>20217</v>
+      </c>
+      <c r="E28" s="5">
+        <v>237</v>
+      </c>
+      <c r="F28" s="5">
+        <v>8006</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="F32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="5">
+        <v>20217</v>
+      </c>
+      <c r="G33" s="5">
+        <v>237</v>
+      </c>
+      <c r="H33" s="5">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="B37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="19" t="s">
+      <c r="C42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E13" s="20">
-        <v>237</v>
-      </c>
-      <c r="F13" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G13" s="20">
-        <v>173</v>
-      </c>
-      <c r="H13" s="20">
-        <v>237</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" s="19">
-        <v>45</v>
-      </c>
-      <c r="K13" s="20">
-        <v>45</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N13" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O13" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P13" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q13" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R13" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S13" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U13" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="C43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="B47" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="19" t="s">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E26" s="20">
-        <v>237</v>
-      </c>
-      <c r="F26" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G26" s="20">
-        <v>173</v>
-      </c>
-      <c r="H26" s="20">
-        <v>237</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J26" s="19">
-        <v>45</v>
-      </c>
-      <c r="K26" s="20">
-        <v>45</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N26" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P26" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R26" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S26" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T26" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U26" s="5">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3460,10 +3647,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X62"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I63" sqref="A60:I63"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4813,140 +5000,504 @@
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="A53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C54" s="5">
+        <v>237</v>
+      </c>
+      <c r="D54" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" s="2">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="2">
         <v>20217</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C59" s="5">
         <v>237</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D59" s="2">
         <v>8006</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="P63" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="R63" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="D64" s="20">
+        <v>445</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G64" s="21">
+        <v>12000</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I64" s="20">
+        <v>50000</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L64" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N64" s="2">
+        <v>1</v>
+      </c>
+      <c r="O64" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>50</v>
+      </c>
+      <c r="R64" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="2">
+      <c r="G68" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P68" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q68" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R68" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T68" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U68" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D69" s="20">
         <v>20217</v>
       </c>
-      <c r="C62" s="5">
+      <c r="E69" s="20">
         <v>237</v>
       </c>
-      <c r="D62" s="2">
+      <c r="F69" s="20">
         <v>8006</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>129</v>
+      <c r="G69" s="20">
+        <v>173</v>
+      </c>
+      <c r="H69" s="20">
+        <v>237</v>
+      </c>
+      <c r="I69" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J69" s="19">
+        <v>45</v>
+      </c>
+      <c r="K69" s="20">
+        <v>45</v>
+      </c>
+      <c r="L69" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N69" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O69" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P69" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q69" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R69" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S69" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T69" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U69" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P73" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q73" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R73" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S73" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T73" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U73" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E74" s="20">
+        <v>237</v>
+      </c>
+      <c r="F74" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G74" s="20">
+        <v>173</v>
+      </c>
+      <c r="H74" s="20">
+        <v>237</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J74" s="19">
+        <v>45</v>
+      </c>
+      <c r="K74" s="20">
+        <v>45</v>
+      </c>
+      <c r="L74" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N74" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O74" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P74" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q74" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R74" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S74" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U74" s="5">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -4957,682 +5508,365 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E3" s="20">
+        <v>237</v>
+      </c>
+      <c r="F3" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G3" s="20">
+        <v>173</v>
+      </c>
+      <c r="H3" s="20">
+        <v>237</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="19">
         <v>45</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="K3" s="20">
+        <v>45</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N3" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P3" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U3" s="5">
+        <v>45</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="G12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="20">
         <v>20217</v>
       </c>
-      <c r="H3" s="5">
+      <c r="E13" s="20">
+        <v>237</v>
+      </c>
+      <c r="F13" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G13" s="20">
         <v>173</v>
       </c>
-      <c r="I3" s="5">
+      <c r="H13" s="20">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2">
-        <v>25997</v>
-      </c>
-      <c r="H4" s="2">
-        <v>7166</v>
-      </c>
-      <c r="I4" s="2">
-        <v>8414</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2">
-        <v>25997</v>
-      </c>
-      <c r="H5" s="2">
-        <v>7166</v>
-      </c>
-      <c r="I5" s="2">
-        <v>8414</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="I13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="19">
+        <v>45</v>
+      </c>
+      <c r="K13" s="20">
+        <v>45</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N13" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P13" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q13" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U13" s="5">
+        <v>45</v>
+      </c>
+      <c r="V13" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="5">
-        <v>20217</v>
-      </c>
-      <c r="H10" s="5">
-        <v>173</v>
-      </c>
-      <c r="I10" s="5">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="5">
-        <v>20217</v>
-      </c>
-      <c r="H11" s="5">
-        <v>237</v>
-      </c>
-      <c r="I11" s="5">
-        <v>8006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="2">
-        <v>25997</v>
-      </c>
-      <c r="H12" s="2">
-        <v>7166</v>
-      </c>
-      <c r="I12" s="2">
-        <v>8414</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="5">
-        <v>20217</v>
-      </c>
-      <c r="H17" s="5">
-        <v>237</v>
-      </c>
-      <c r="I17" s="5">
-        <v>8006</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="2">
-        <v>25997</v>
-      </c>
-      <c r="H18" s="2">
-        <v>7166</v>
-      </c>
-      <c r="I18" s="2">
-        <v>8414</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="5">
-        <v>20217</v>
-      </c>
-      <c r="G23" s="5">
-        <v>237</v>
-      </c>
-      <c r="H23" s="5">
-        <v>8006</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E28" s="5">
-        <v>237</v>
-      </c>
-      <c r="F28" s="5">
-        <v>8006</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="5">
-        <v>20217</v>
-      </c>
-      <c r="G33" s="5">
-        <v>237</v>
-      </c>
-      <c r="H33" s="5">
-        <v>8006</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>147</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactored quote page tests - file upload related
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18120" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21708" windowHeight="8172" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="232">
   <si>
     <t>corp</t>
   </si>
@@ -402,9 +402,6 @@
   </si>
   <si>
     <t>venkatqa.com</t>
-  </si>
-  <si>
-    <t>testConfirmAndLockQuoteOption</t>
   </si>
   <si>
     <t>testBrokerDownloadConfirmedQuote</t>
@@ -453,9 +450,6 @@
     <t>testAddQuote</t>
   </si>
   <si>
-    <t>testLockQuote</t>
-  </si>
-  <si>
     <t>welcomeText</t>
   </si>
   <si>
@@ -681,9 +675,6 @@
     <t>physiciansCount</t>
   </si>
   <si>
-    <t>testFileSizeValidationForBinder</t>
-  </si>
-  <si>
     <t>testIneligiblePolicies</t>
   </si>
   <si>
@@ -699,9 +690,6 @@
     <t>Binder_</t>
   </si>
   <si>
-    <t>quoteOptionStatus</t>
-  </si>
-  <si>
     <t>Option Order</t>
   </si>
   <si>
@@ -715,6 +703,30 @@
   </si>
   <si>
     <t>testContactUnderwriterModalAfterLock</t>
+  </si>
+  <si>
+    <t>quoteStatusDashboard</t>
+  </si>
+  <si>
+    <t>quoteStatusBinder</t>
+  </si>
+  <si>
+    <t>testLockingQuote</t>
+  </si>
+  <si>
+    <t>testFileUploadValidationsInBinder</t>
+  </si>
+  <si>
+    <t>fileType</t>
+  </si>
+  <si>
+    <t>fileTypeValidation</t>
+  </si>
+  <si>
+    <t>fileSizeValidation</t>
+  </si>
+  <si>
+    <t>testGenerateBinderButtonValidations</t>
   </si>
 </sst>
 </file>
@@ -820,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -877,6 +889,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1251,7 +1275,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -1341,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>22</v>
@@ -1352,10 +1376,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="2">
         <v>20217</v>
@@ -1382,10 +1406,10 @@
         <v>19</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1393,10 +1417,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D4" s="2">
         <v>25997</v>
@@ -1423,10 +1447,10 @@
         <v>19</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1531,7 +1555,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -1589,16 +1613,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F16" s="2">
         <v>20217</v>
@@ -1615,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -1624,7 +1648,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F17" s="2">
         <v>25997</v>
@@ -1694,10 +1718,10 @@
         <v>14</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1714,7 +1738,7 @@
         <v>8414</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>13</v>
@@ -1723,10 +1747,10 @@
         <v>14</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1814,7 +1838,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>73</v>
@@ -1869,7 +1893,7 @@
         <v>8006</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>80</v>
@@ -1881,7 +1905,7 @@
         <v>82</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1898,7 +1922,7 @@
         <v>8414</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>83</v>
@@ -1910,7 +1934,7 @@
         <v>82</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1959,7 +1983,7 @@
         <v>8006</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>85</v>
@@ -1968,7 +1992,7 @@
         <v>82</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1985,7 +2009,7 @@
         <v>8414</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>85</v>
@@ -1994,7 +2018,7 @@
         <v>82</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2270,7 +2294,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2291,15 +2315,15 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2315,7 +2339,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -2323,12 +2347,12 @@
         <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -2342,16 +2366,16 @@
         <v>22</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F92" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="G92" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -2359,27 +2383,27 @@
         <v>3</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2400,10 +2424,10 @@
         <v>3</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2556,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
@@ -2654,7 +2678,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
@@ -2759,7 +2783,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -2829,7 +2853,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>89</v>
@@ -2850,7 +2874,7 @@
         <v>8006</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2885,7 +2909,7 @@
         <v>119</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>28</v>
@@ -2896,7 +2920,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
@@ -2917,10 +2941,10 @@
         <v>121</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -2959,10 +2983,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>123</v>
@@ -2982,7 +3006,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2999,7 +3023,7 @@
         <v>119</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>28</v>
@@ -3010,24 +3034,24 @@
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -3052,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>89</v>
@@ -3066,7 +3090,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -3082,7 +3106,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3158,22 +3182,22 @@
         <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>105</v>
@@ -3187,7 +3211,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>47</v>
@@ -3217,16 +3241,16 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="O3" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P3" s="5">
         <v>50</v>
@@ -3264,22 +3288,22 @@
         <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -3287,10 +3311,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>109</v>
@@ -3311,18 +3335,18 @@
         <v>30000000</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3343,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>47</v>
@@ -3354,7 +3378,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3365,16 +3389,16 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>105</v>
@@ -3383,10 +3407,10 @@
         <v>106</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3394,19 +3418,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C18" s="5">
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="G18" s="2">
         <v>100000</v>
@@ -3415,7 +3439,7 @@
         <v>60</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J18" s="5">
         <v>50</v>
@@ -3464,16 +3488,16 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3481,24 +3505,24 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5">
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -3509,22 +3533,22 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="G7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -3532,30 +3556,30 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="5">
         <v>50000</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="G8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -3578,22 +3602,22 @@
         <v>105</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>106</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K13" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>7</v>
@@ -3604,10 +3628,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>109</v>
@@ -3628,16 +3652,16 @@
         <v>100000</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="L14" s="12" t="s">
-        <v>137</v>
-      </c>
       <c r="M14" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3647,10 +3671,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X74"/>
+  <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3670,12 +3694,14 @@
     <col min="18" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3730,22 +3756,22 @@
         <v>115</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -3753,10 +3779,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>80</v>
@@ -3789,28 +3815,28 @@
         <v>445</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P3" s="11">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="S3" s="5">
         <v>50000</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="V3" s="5">
         <v>50</v>
@@ -3821,10 +3847,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>80</v>
@@ -3857,28 +3883,28 @@
         <v>445</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P4" s="11">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="S4" s="5">
         <v>50000</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="V4" s="5">
         <v>50</v>
@@ -3906,7 +3932,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3961,22 +3987,22 @@
         <v>115</v>
       </c>
       <c r="Q8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="S8" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -3984,10 +4010,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>80</v>
@@ -4020,28 +4046,28 @@
         <v>445</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P9" s="11">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="S9" s="5">
         <v>50000</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="V9" s="5">
         <v>50</v>
@@ -4059,7 +4085,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -4106,28 +4132,28 @@
         <v>115</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="T13" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
@@ -4135,7 +4161,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>80</v>
@@ -4165,45 +4191,45 @@
         <v>445</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N14" s="11">
         <v>12000</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P14" s="5">
         <v>50000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R14" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="S14" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="T14" s="2">
         <v>1</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="V14" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -4247,33 +4273,33 @@
         <v>115</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="S18" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="T18" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>80</v>
@@ -4303,237 +4329,249 @@
         <v>445</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N19" s="11">
         <v>12000</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P19" s="5">
         <v>50000</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="S19" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="S19" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="T19" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="U19" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="U23" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="V23" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="5">
-        <v>7786</v>
-      </c>
-      <c r="G24" s="5">
-        <v>7352</v>
-      </c>
-      <c r="H24" s="5">
-        <v>3362</v>
-      </c>
-      <c r="I24" s="5">
-        <v>173</v>
-      </c>
-      <c r="J24" s="5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>20217</v>
+      </c>
+      <c r="C24" s="5">
         <v>237</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="M24" s="5">
-        <v>445</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P24" s="11">
-        <v>10000</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="R24" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="S24" s="5">
-        <v>50000</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="U24" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="V24" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D24" s="2">
+        <v>8006</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="2">
+        <v>103</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="V28" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="W28" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="X28" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="20">
         <v>20217</v>
       </c>
-      <c r="C29" s="5">
+      <c r="E29" s="20">
         <v>237</v>
       </c>
-      <c r="D29" s="2">
+      <c r="F29" s="20">
         <v>8006</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H29" s="2" t="s">
+      <c r="G29" s="20">
+        <v>173</v>
+      </c>
+      <c r="H29" s="20">
+        <v>237</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J29" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K29" s="20">
+        <v>445</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N29" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O29" s="22" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="P29" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q29" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="R29" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="S29" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="T29" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="U29" s="5">
+        <v>50</v>
+      </c>
+      <c r="V29" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="W29" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="X29" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
@@ -4544,131 +4582,23 @@
         <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S33" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E34" s="20">
-        <v>237</v>
-      </c>
-      <c r="F34" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G34" s="20">
-        <v>173</v>
-      </c>
-      <c r="H34" s="20">
-        <v>237</v>
-      </c>
-      <c r="I34" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J34" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="K34" s="20">
-        <v>445</v>
-      </c>
-      <c r="L34" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M34" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N34" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O34" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P34" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q34" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R34" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S34" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T34" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U34" s="5">
-        <v>50</v>
+        <v>145</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -4679,23 +4609,149 @@
         <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="U38" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="V38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="W38" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>180</v>
+        <v>145</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E39" s="20">
+        <v>237</v>
+      </c>
+      <c r="F39" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G39" s="20">
+        <v>173</v>
+      </c>
+      <c r="H39" s="20">
+        <v>237</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J39" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="K39" s="20">
+        <v>445</v>
+      </c>
+      <c r="L39" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N39" s="21">
+        <v>12000</v>
+      </c>
+      <c r="O39" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="P39" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q39" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="R39" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="S39" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="U39" s="2">
+        <v>1</v>
+      </c>
+      <c r="V39" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="X39" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.3">
@@ -4733,43 +4789,43 @@
         <v>106</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>115</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S43" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="S43" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="T43" s="4" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
       <c r="U43" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V43" s="4" t="s">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="W43" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4777,7 +4833,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>80</v>
@@ -4807,40 +4863,40 @@
         <v>445</v>
       </c>
       <c r="L44" s="20" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N44" s="21">
-        <v>12000</v>
+        <v>184</v>
+      </c>
+      <c r="N44" s="23" t="s">
+        <v>181</v>
       </c>
       <c r="O44" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P44" s="20">
         <v>50000</v>
       </c>
       <c r="Q44" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R44" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="S44" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="S44" s="20" t="s">
-        <v>137</v>
-      </c>
       <c r="T44" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="U44" s="2">
         <v>1</v>
       </c>
-      <c r="V44" s="23" t="s">
-        <v>183</v>
+      <c r="V44" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="X44" s="5">
         <v>50</v>
@@ -4848,7 +4904,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
@@ -4856,155 +4912,59 @@
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N48" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O48" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T48" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="U48" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="V48" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="W48" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="X48" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="20">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="2">
         <v>20217</v>
       </c>
-      <c r="E49" s="20">
+      <c r="C49" s="5">
         <v>237</v>
       </c>
-      <c r="F49" s="20">
+      <c r="D49" s="2">
         <v>8006</v>
       </c>
-      <c r="G49" s="20">
-        <v>173</v>
-      </c>
-      <c r="H49" s="20">
-        <v>237</v>
-      </c>
-      <c r="I49" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J49" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="K49" s="20">
-        <v>445</v>
-      </c>
-      <c r="L49" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="M49" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="N49" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="O49" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P49" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q49" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R49" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S49" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T49" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="U49" s="2">
-        <v>1</v>
-      </c>
-      <c r="V49" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="W49" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="X49" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="E49" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -5021,16 +4981,16 @@
         <v>111</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>3</v>
       </c>
@@ -5044,195 +5004,273 @@
         <v>8006</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="P58" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="R58" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="2">
-        <v>20217</v>
-      </c>
-      <c r="C59" s="5">
-        <v>237</v>
-      </c>
-      <c r="D59" s="2">
-        <v>8006</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H59" s="2" t="s">
+      <c r="B59" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="D59" s="20">
+        <v>445</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G59" s="21">
+        <v>12000</v>
+      </c>
+      <c r="H59" s="22" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I59" s="20">
+        <v>50000</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="L59" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N59" s="2">
+        <v>1</v>
+      </c>
+      <c r="O59" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>50</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="J63" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="K63" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="L63" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="M63" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="N63" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H63" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I63" s="2" t="s">
+      <c r="O63" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P63" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R63" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T63" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="U63" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E64" s="20">
+        <v>237</v>
+      </c>
+      <c r="F64" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G64" s="20">
+        <v>173</v>
+      </c>
+      <c r="H64" s="20">
+        <v>237</v>
+      </c>
+      <c r="I64" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J64" s="19">
+        <v>45</v>
+      </c>
+      <c r="K64" s="20">
+        <v>45</v>
+      </c>
+      <c r="L64" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N64" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O64" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="P64" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q64" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="J63" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M63" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="N63" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="O63" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="P63" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q63" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="R63" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C64" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="D64" s="20">
-        <v>445</v>
-      </c>
-      <c r="E64" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="G64" s="21">
-        <v>12000</v>
-      </c>
-      <c r="H64" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="I64" s="20">
-        <v>50000</v>
-      </c>
-      <c r="J64" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="K64" s="20" t="s">
+      <c r="R64" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="S64" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="L64" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="N64" s="2">
-        <v>1</v>
-      </c>
-      <c r="O64" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="P64" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q64" s="5">
-        <v>50</v>
-      </c>
-      <c r="R64" s="6" t="s">
-        <v>225</v>
+      <c r="T64" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="U64" s="5">
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
@@ -5279,33 +5317,33 @@
         <v>115</v>
       </c>
       <c r="O68" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="S68" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="T68" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="U68" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C69" s="20" t="s">
         <v>80</v>
@@ -5335,168 +5373,33 @@
         <v>45</v>
       </c>
       <c r="L69" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N69" s="21">
         <v>15000</v>
       </c>
       <c r="O69" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P69" s="20">
         <v>50000</v>
       </c>
       <c r="Q69" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R69" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="S69" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="S69" s="20" t="s">
-        <v>137</v>
-      </c>
       <c r="T69" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="U69" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L73" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M73" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N73" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O73" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P73" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q73" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R73" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S73" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T73" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U73" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D74" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E74" s="20">
-        <v>237</v>
-      </c>
-      <c r="F74" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G74" s="20">
-        <v>173</v>
-      </c>
-      <c r="H74" s="20">
-        <v>237</v>
-      </c>
-      <c r="I74" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J74" s="19">
-        <v>45</v>
-      </c>
-      <c r="K74" s="20">
-        <v>45</v>
-      </c>
-      <c r="L74" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M74" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N74" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O74" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P74" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q74" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R74" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S74" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T74" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U74" s="5">
         <v>45</v>
       </c>
     </row>
@@ -5508,21 +5411,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.44140625" bestFit="1" customWidth="1"/>
@@ -5530,7 +5437,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -5538,141 +5445,145 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>115</v>
+        <v>149</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>222</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="29"/>
     </row>
     <row r="3" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E3" s="20">
+      <c r="B3" s="20">
+        <v>173</v>
+      </c>
+      <c r="C3" s="20">
         <v>237</v>
       </c>
+      <c r="D3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="19">
+        <v>45</v>
+      </c>
       <c r="F3" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G3" s="20">
-        <v>173</v>
-      </c>
-      <c r="H3" s="20">
-        <v>237</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="19">
         <v>45</v>
       </c>
+      <c r="G3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" s="21">
+        <v>15000</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>129</v>
+      </c>
       <c r="K3" s="20">
+        <v>50000</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P3" s="5">
         <v>45</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N3" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="S3" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U3" s="5">
-        <v>45</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>223</v>
-      </c>
+      <c r="Q3" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="29"/>
     </row>
     <row r="5" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -5680,10 +5591,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -5691,15 +5602,15 @@
         <v>3</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>208</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -5707,162 +5618,339 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>228</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>151</v>
+      <c r="K12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>133</v>
+        <v>213</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>222</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>80</v>
+      <c r="B13" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="20">
+        <v>173</v>
       </c>
       <c r="D13" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E13" s="20">
         <v>237</v>
       </c>
-      <c r="F13" s="20">
-        <v>8006</v>
+      <c r="E13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="19">
+        <v>45</v>
       </c>
       <c r="G13" s="20">
+        <v>45</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="21">
+        <v>15000</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" s="20">
+        <v>50000</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>45</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S13" s="5">
+        <v>45</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" s="20">
         <v>173</v>
       </c>
-      <c r="H13" s="20">
+      <c r="D14" s="20">
         <v>237</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="E14" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="19">
+      <c r="F14" s="19">
         <v>45</v>
       </c>
-      <c r="K13" s="20">
+      <c r="G14" s="20">
         <v>45</v>
       </c>
-      <c r="L13" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="N13" s="21">
+      <c r="H14" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J14" s="21">
         <v>15000</v>
       </c>
-      <c r="O13" s="22" t="s">
+      <c r="K14" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="20">
+        <v>50000</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>45</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S14" s="5">
+        <v>45</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="P13" s="20">
+      <c r="K23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="20">
+        <v>173</v>
+      </c>
+      <c r="C24" s="20">
+        <v>237</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="19">
+        <v>45</v>
+      </c>
+      <c r="F24" s="20">
+        <v>45</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" s="21">
+        <v>15000</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" s="20">
         <v>50000</v>
       </c>
-      <c r="Q13" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="R13" s="20" t="s">
+      <c r="L24" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N24" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="S13" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U13" s="5">
+      <c r="O24" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P24" s="5">
         <v>45</v>
       </c>
-      <c r="V13" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>210</v>
+      <c r="Q24" s="19" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test data for testVerifyQuoteBinding
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5411,23 +5411,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="3" max="4" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
@@ -5435,417 +5435,382 @@
     <col min="22" max="22" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="29"/>
-    </row>
-    <row r="3" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20">
-        <v>173</v>
-      </c>
-      <c r="C3" s="20">
-        <v>237</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="19">
-        <v>45</v>
-      </c>
-      <c r="F3" s="20">
-        <v>45</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="I3" s="21">
-        <v>15000</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="20">
-        <v>50000</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="P3" s="5">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="29"/>
-    </row>
-    <row r="4" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="29"/>
-    </row>
-    <row r="5" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="20">
+        <v>173</v>
+      </c>
+      <c r="D8" s="20">
+        <v>237</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="19">
+        <v>45</v>
+      </c>
+      <c r="G8" s="20">
+        <v>45</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="21">
+        <v>15000</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="L8" s="20">
+        <v>50000</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>45</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S8" s="5">
+        <v>45</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="20">
+        <v>173</v>
+      </c>
+      <c r="D9" s="20">
+        <v>237</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="19">
+        <v>45</v>
+      </c>
+      <c r="G9" s="20">
+        <v>45</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="21">
+        <v>15000</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="20">
+        <v>50000</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>45</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S9" s="5">
+        <v>45</v>
+      </c>
+      <c r="T9" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="C8" s="20" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="20">
-        <v>173</v>
-      </c>
-      <c r="D13" s="20">
-        <v>237</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="19">
-        <v>45</v>
-      </c>
-      <c r="G13" s="20">
-        <v>45</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="21">
-        <v>15000</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="L13" s="20">
-        <v>50000</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="N13" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>45</v>
-      </c>
-      <c r="R13" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="S13" s="5">
-        <v>45</v>
-      </c>
-      <c r="T13" s="19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="20">
-        <v>173</v>
-      </c>
-      <c r="D14" s="20">
-        <v>237</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="19">
-        <v>45</v>
-      </c>
-      <c r="G14" s="20">
-        <v>45</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="J14" s="21">
-        <v>15000</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="L14" s="20">
-        <v>50000</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="N14" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="O14" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>45</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="S14" s="5">
-        <v>45</v>
-      </c>
-      <c r="T14" s="19" t="s">
-        <v>219</v>
-      </c>
-    </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>217</v>
-      </c>
+      <c r="A17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>208</v>
+      <c r="B19" s="20">
+        <v>173</v>
+      </c>
+      <c r="C19" s="20">
+        <v>237</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="19">
+        <v>45</v>
+      </c>
+      <c r="F19" s="20">
+        <v>45</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="21">
+        <v>15000</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" s="20">
+        <v>50000</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="P19" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
+        <v>200</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">

</xml_diff>

<commit_message>
updated Binder Tests on 9.6 branch
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="235">
   <si>
     <t xml:space="preserve">testLoginFunctionality</t>
   </si>
@@ -723,6 +723,15 @@
   </si>
   <si>
     <t xml:space="preserve">testVerifyQuoteBinding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boundStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testValidateSubjectivitiesAndQuoteStatus</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1057,10 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.33"/>
   </cols>
@@ -1176,7 +1185,7 @@
       <selection pane="topLeft" activeCell="C98" activeCellId="0" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
@@ -2319,7 +2328,7 @@
       <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
@@ -3009,7 +3018,7 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -3354,7 +3363,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3577,15 +3586,15 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="17.67"/>
@@ -5321,11 +5330,11 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
@@ -5334,6 +5343,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.33"/>
@@ -5772,6 +5784,9 @@
       <c r="Q23" s="3" t="s">
         <v>200</v>
       </c>
+      <c r="R23" s="3" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
@@ -5823,6 +5838,120 @@
         <v>45</v>
       </c>
       <c r="Q24" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="R24" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="20" t="n">
+        <v>173</v>
+      </c>
+      <c r="C29" s="20" t="n">
+        <v>237</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="20" t="n">
+        <v>45</v>
+      </c>
+      <c r="F29" s="20" t="n">
+        <v>45</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="I29" s="21" t="n">
+        <v>15000</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="K29" s="20" t="n">
+        <v>50000</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q29" s="20" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed quotes page tests refactoring 90%
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="239">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -678,9 +678,6 @@
     <t>testDownloadApplicationInQuote</t>
   </si>
   <si>
-    <t>testConfirmDatesModal</t>
-  </si>
-  <si>
     <t>testContactUnderwriterModalBeforeLock</t>
   </si>
   <si>
@@ -741,7 +738,16 @@
     <t>Please provide any additional information or file to the underwriter for review.</t>
   </si>
   <si>
-    <t>testAddingQuote</t>
+    <t>$ 10,000</t>
+  </si>
+  <si>
+    <t>testAddingQuoteToExistingSubmission</t>
+  </si>
+  <si>
+    <t>testAddingQuoteToNewSubmission</t>
+  </si>
+  <si>
+    <t>testValidateConfirmDatesModal</t>
   </si>
 </sst>
 </file>
@@ -847,7 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -909,6 +915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3747,15 +3754,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X69"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
@@ -3765,7 +3772,9 @@
     <col min="8" max="8" width="43.21875" customWidth="1"/>
     <col min="9" max="9" width="24.109375" customWidth="1"/>
     <col min="10" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" customWidth="1"/>
@@ -4109,8 +4118,8 @@
       <c r="L9" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="M9" s="16">
-        <v>10000</v>
+      <c r="M9" s="29" t="s">
+        <v>235</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>161</v>
@@ -5076,7 +5085,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
@@ -5193,7 +5202,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
@@ -5261,7 +5270,7 @@
         <v>157</v>
       </c>
       <c r="V63" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5329,12 +5338,12 @@
         <v>45</v>
       </c>
       <c r="V64" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
@@ -5402,7 +5411,7 @@
         <v>157</v>
       </c>
       <c r="V68" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
@@ -5470,12 +5479,147 @@
         <v>45</v>
       </c>
       <c r="V69" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O73" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="P73" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q73" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R73" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="S73" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T73" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="U73" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C74" s="20">
+        <v>1000000</v>
+      </c>
+      <c r="D74" s="20">
+        <v>445</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G74" s="21">
+        <v>12000</v>
+      </c>
+      <c r="H74" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="I74" s="20">
+        <v>50000</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="K74" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="L74" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M74" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N74" s="3">
+        <v>1</v>
+      </c>
+      <c r="O74" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="P74" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q74" s="5">
+        <v>50</v>
+      </c>
+      <c r="R74" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="T74" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U74" s="29" t="s">
         <v>235</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5510,7 +5654,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -5518,10 +5662,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -5529,15 +5673,15 @@
         <v>5</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>221</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -5545,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>150</v>
@@ -5607,7 +5751,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="20">
         <v>173</v>
@@ -5669,7 +5813,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="20">
         <v>173</v>
@@ -5728,7 +5872,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -5739,7 +5883,7 @@
         <v>192</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -5747,15 +5891,15 @@
         <v>5</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -5882,7 +6026,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -5938,7 +6082,7 @@
         <v>199</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5994,12 +6138,12 @@
         <v>203</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Refactored Binder Tests 2
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8064" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8064" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="240">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -3764,7 +3764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O68" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="O68" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S81" sqref="S81"/>
     </sheetView>
   </sheetViews>
@@ -5734,10 +5734,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6196,7 +6196,7 @@
     </row>
     <row r="24" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B24" s="20">
         <v>173</v>
@@ -6250,114 +6250,170 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="25" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="20">
+        <v>173</v>
+      </c>
+      <c r="C25" s="20">
+        <v>237</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="20">
+        <v>45</v>
+      </c>
+      <c r="F25" s="20">
+        <v>45</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="I25" s="21">
+        <v>15000</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="K25" s="20">
+        <v>50000</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N25" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="P25" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q25" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="R25" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="N29" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="O29" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="P29" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Q28" s="3" t="s">
+      <c r="Q29" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+    <row r="30" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B30" s="20">
         <v>173</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C30" s="20">
         <v>237</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D30" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E30" s="20">
         <v>45</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F30" s="20">
         <v>45</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H30" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I30" s="21">
         <v>15000</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J30" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="K29" s="20">
+      <c r="K30" s="20">
         <v>50000</v>
       </c>
-      <c r="L29" s="20" t="s">
+      <c r="L30" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="M30" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="N30" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="O29" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="P29" s="5">
+      <c r="P30" s="5">
         <v>45</v>
       </c>
-      <c r="Q29" s="20" t="s">
+      <c r="Q30" s="20" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added scroll to top method
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="241">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t>testNotDisplayPremiumIfReviewRequired</t>
+  </si>
+  <si>
+    <t>testValidateConfirmDatesPlaceOrderFunctionality</t>
   </si>
 </sst>
 </file>
@@ -5734,15 +5737,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.21875" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
@@ -6417,6 +6420,123 @@
         <v>205</v>
       </c>
     </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="20">
+        <v>173</v>
+      </c>
+      <c r="C35" s="20">
+        <v>237</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E35" s="20">
+        <v>45</v>
+      </c>
+      <c r="F35" s="20">
+        <v>45</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="I35" s="21">
+        <v>15000</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="K35" s="20">
+        <v>50000</v>
+      </c>
+      <c r="L35" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="P35" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q35" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="R35" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fixed failures in quote tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8064" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="241">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -748,6 +748,12 @@
   </si>
   <si>
     <t>testValidateConfirmDatesPlaceOrderFunctionality</t>
+  </si>
+  <si>
+    <t>modalText</t>
+  </si>
+  <si>
+    <t>Please provide any additional information or file to the underwriter for review.</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -3757,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="L49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W62" sqref="W62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5352,12 +5358,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>1</v>
       </c>
@@ -5421,8 +5427,11 @@
       <c r="U68" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V68" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
         <v>5</v>
       </c>
@@ -5485,6 +5494,9 @@
       </c>
       <c r="U69" s="5">
         <v>45</v>
+      </c>
+      <c r="V69" s="20" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added automation for testDownloadApplicationInQuote
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snap QA\automation_project\brokerPortalUI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-qat-534\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06C784-62F5-4F7D-9570-82630B25DD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="241">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -748,12 +749,18 @@
   </si>
   <si>
     <t>testValidateConfirmDatesPlaceOrderFunctionality</t>
+  </si>
+  <si>
+    <t>fileNamePDF</t>
+  </si>
+  <si>
+    <t>fileName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0_);[Red]&quot;($&quot;#,##0\)"/>
   </numFmts>
@@ -853,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -912,6 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1260,7 +1268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1380,10 +1388,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -2520,7 +2528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
@@ -3194,7 +3202,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1"/>
+    <hyperlink ref="K18" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3202,7 +3210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
@@ -3530,8 +3538,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3539,7 +3547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3754,11 +3762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="G34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3773,6 +3781,8 @@
     <col min="8" max="8" width="43.21875" customWidth="1"/>
     <col min="9" max="9" width="24.109375" customWidth="1"/>
     <col min="10" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.6640625" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" customWidth="1"/>
     <col min="18" max="19" width="17.77734375" customWidth="1"/>
@@ -5016,6 +5026,21 @@
       <c r="H48" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="I48" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M48" s="28" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
@@ -5042,6 +5067,21 @@
       <c r="H49" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="I49" s="20">
+        <v>45</v>
+      </c>
+      <c r="J49" s="20">
+        <v>45</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="L49" s="5">
+        <v>45</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -5073,6 +5113,21 @@
       <c r="H53" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="I53" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M53" s="28" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -5099,6 +5154,21 @@
       <c r="H54" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="I54" s="20">
+        <v>45</v>
+      </c>
+      <c r="J54" s="20">
+        <v>45</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="L54" s="5">
+        <v>45</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -5489,16 +5559,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="E14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixing file upload method using JavaScript Added JavaScriptHelper
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="242">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>Please provide any additional information or file to the underwriter for review.</t>
+  </si>
+  <si>
+    <t>testAddingQuoteToExistingSubmission</t>
   </si>
 </sst>
 </file>
@@ -859,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -917,6 +920,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3761,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X69"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W62" sqref="W62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4163,81 +4170,121 @@
         <v>50</v>
       </c>
     </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="18"/>
+    </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="18"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="P13" s="3" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="T13" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="U13" s="3" t="s">
         <v>159</v>
@@ -4246,66 +4293,66 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="5">
-        <v>20217</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="E14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="5">
+        <v>7786</v>
+      </c>
+      <c r="G14" s="5">
+        <v>7352</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3362</v>
+      </c>
+      <c r="I14" s="5">
+        <v>173</v>
+      </c>
+      <c r="J14" s="5">
         <v>237</v>
       </c>
-      <c r="F14" s="5">
-        <v>8006</v>
-      </c>
-      <c r="G14" s="5">
-        <v>173</v>
-      </c>
-      <c r="H14" s="5">
-        <v>237</v>
-      </c>
-      <c r="I14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="J14" s="6">
+      <c r="L14" s="6">
         <v>1000000</v>
       </c>
-      <c r="K14" s="5">
+      <c r="M14" s="5">
         <v>445</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="O14" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="N14" s="16">
-        <v>12000</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="P14" s="5">
+      <c r="P14" s="16">
+        <v>10000</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="S14" s="5">
         <v>50000</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="T14" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="T14" s="3">
-        <v>1</v>
       </c>
       <c r="U14" s="6" t="s">
         <v>166</v>
@@ -4314,12 +4361,46 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="18"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -4378,13 +4459,16 @@
         <v>158</v>
       </c>
       <c r="T18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U18" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="U18" s="3" t="s">
+      <c r="V18" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -4442,226 +4526,211 @@
       <c r="S19" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="3">
+        <v>1</v>
+      </c>
+      <c r="U19" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="U19" s="5">
+      <c r="V19" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="5">
         <v>20217</v>
       </c>
-      <c r="C24" s="5">
+      <c r="E24" s="5">
         <v>237</v>
       </c>
-      <c r="D24" s="3">
+      <c r="F24" s="5">
         <v>8006</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G24" s="5">
+        <v>173</v>
+      </c>
+      <c r="H24" s="5">
+        <v>237</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="K24" s="5">
+        <v>445</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N24" s="16">
+        <v>12000</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="P24" s="5">
+        <v>50000</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="S24" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U24" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>20</v>
+        <v>195</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U28" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="V28" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="X28" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="20">
+      <c r="B29" s="3">
         <v>20217</v>
       </c>
-      <c r="E29" s="20">
+      <c r="C29" s="5">
         <v>237</v>
       </c>
-      <c r="F29" s="20">
+      <c r="D29" s="3">
         <v>8006</v>
       </c>
-      <c r="G29" s="20">
-        <v>173</v>
-      </c>
-      <c r="H29" s="20">
-        <v>237</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="J29" s="20">
-        <v>1000000</v>
-      </c>
-      <c r="K29" s="20">
-        <v>445</v>
-      </c>
-      <c r="L29" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="N29" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O29" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="P29" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q29" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="R29" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="S29" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="T29" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U29" s="5">
-        <v>50</v>
-      </c>
-      <c r="V29" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="W29" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="X29" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="E29" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
@@ -4672,10 +4741,73 @@
         <v>28</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V33" s="3" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W33" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="X33" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>5</v>
       </c>
@@ -4683,12 +4815,75 @@
         <v>49</v>
       </c>
       <c r="C34" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E34" s="20">
+        <v>237</v>
+      </c>
+      <c r="F34" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G34" s="20">
+        <v>173</v>
+      </c>
+      <c r="H34" s="20">
+        <v>237</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="J34" s="20">
+        <v>1000000</v>
+      </c>
+      <c r="K34" s="20">
+        <v>445</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="M34" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="N34" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O34" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="P34" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q34" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="R34" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="S34" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="T34" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U34" s="5">
+        <v>50</v>
+      </c>
+      <c r="V34" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="W34" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="X34" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -4699,73 +4894,10 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q38" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R38" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T38" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="U38" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="V38" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="W38" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="X38" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>5</v>
       </c>
@@ -4773,75 +4905,12 @@
         <v>49</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E39" s="20">
-        <v>237</v>
-      </c>
-      <c r="F39" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G39" s="20">
-        <v>173</v>
-      </c>
-      <c r="H39" s="20">
-        <v>237</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="J39" s="20">
-        <v>1000000</v>
-      </c>
-      <c r="K39" s="20">
-        <v>445</v>
-      </c>
-      <c r="L39" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="M39" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="N39" s="21">
-        <v>12000</v>
-      </c>
-      <c r="O39" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="P39" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q39" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="R39" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="S39" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="T39" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="U39" s="3">
-        <v>1</v>
-      </c>
-      <c r="V39" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="W39" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="X39" s="5">
-        <v>50</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.3">
@@ -4879,10 +4948,10 @@
         <v>162</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="N43" s="3" t="s">
         <v>183</v>
@@ -4903,13 +4972,13 @@
         <v>158</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="U43" s="3" t="s">
         <v>191</v>
       </c>
       <c r="V43" s="3" t="s">
-        <v>216</v>
+        <v>183</v>
       </c>
       <c r="W43" s="3" t="s">
         <v>159</v>
@@ -4953,13 +5022,13 @@
         <v>445</v>
       </c>
       <c r="L44" s="20" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="N44" s="23" t="s">
-        <v>211</v>
+        <v>186</v>
+      </c>
+      <c r="N44" s="21">
+        <v>12000</v>
       </c>
       <c r="O44" s="22" t="s">
         <v>192</v>
@@ -4982,8 +5051,8 @@
       <c r="U44" s="3">
         <v>1</v>
       </c>
-      <c r="V44" s="3" t="s">
-        <v>186</v>
+      <c r="V44" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="W44" s="6" t="s">
         <v>166</v>
@@ -4994,7 +5063,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
@@ -5002,59 +5071,155 @@
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="G48" s="3" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="20">
         <v>20217</v>
       </c>
-      <c r="C49" s="5">
+      <c r="E49" s="20">
         <v>237</v>
       </c>
-      <c r="D49" s="3">
+      <c r="F49" s="20">
         <v>8006</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="G49" s="20">
+        <v>173</v>
+      </c>
+      <c r="H49" s="20">
+        <v>237</v>
+      </c>
+      <c r="I49" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="J49" s="20">
+        <v>1000000</v>
+      </c>
+      <c r="K49" s="20">
+        <v>445</v>
+      </c>
+      <c r="L49" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="M49" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="P49" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q49" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="R49" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="S49" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="U49" s="3">
+        <v>1</v>
+      </c>
+      <c r="V49" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="W49" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="X49" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>1</v>
       </c>
@@ -5080,7 +5245,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
@@ -5106,261 +5271,183 @@
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>168</v>
+        <v>19</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>162</v>
+        <v>21</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="M58" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="N58" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q58" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="R58" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C59" s="20">
-        <v>1000000</v>
-      </c>
-      <c r="D59" s="20">
-        <v>445</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="G59" s="21">
-        <v>12000</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="I59" s="20">
-        <v>50000</v>
-      </c>
-      <c r="J59" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="K59" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="L59" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="M59" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="N59" s="3">
-        <v>1</v>
-      </c>
-      <c r="O59" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="P59" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q59" s="5">
-        <v>50</v>
-      </c>
-      <c r="R59" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B59" s="3">
+        <v>20217</v>
+      </c>
+      <c r="C59" s="5">
+        <v>237</v>
+      </c>
+      <c r="D59" s="3">
+        <v>8006</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>28</v>
+        <v>168</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L63" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M63" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="M63" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="N63" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="O63" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="O63" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="P63" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S63" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T63" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U63" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>80</v>
+        <v>185</v>
+      </c>
+      <c r="C64" s="20">
+        <v>1000000</v>
       </c>
       <c r="D64" s="20">
-        <v>20217</v>
-      </c>
-      <c r="E64" s="20">
-        <v>237</v>
-      </c>
-      <c r="F64" s="20">
-        <v>8006</v>
-      </c>
-      <c r="G64" s="20">
-        <v>173</v>
-      </c>
-      <c r="H64" s="20">
-        <v>237</v>
-      </c>
-      <c r="I64" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="J64" s="20">
-        <v>45</v>
-      </c>
-      <c r="K64" s="20">
-        <v>45</v>
+        <v>445</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G64" s="21">
+        <v>12000</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="I64" s="20">
+        <v>50000</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="L64" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="M64" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M64" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="N64" s="21">
-        <v>15000</v>
-      </c>
-      <c r="O64" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="P64" s="20">
-        <v>50000</v>
-      </c>
-      <c r="Q64" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="R64" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="S64" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="T64" s="6" t="s">
+      <c r="N64" s="3">
+        <v>1</v>
+      </c>
+      <c r="O64" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="P64" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="U64" s="5">
-        <v>45</v>
+      <c r="Q64" s="5">
+        <v>50</v>
+      </c>
+      <c r="R64" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
@@ -5427,11 +5514,8 @@
       <c r="U68" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="V68" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
         <v>5</v>
       </c>
@@ -5495,7 +5579,145 @@
       <c r="U69" s="5">
         <v>45</v>
       </c>
-      <c r="V69" s="20" t="s">
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="O73" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="P73" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q73" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R73" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S73" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T73" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="U73" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V73" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="20">
+        <v>20217</v>
+      </c>
+      <c r="E74" s="20">
+        <v>237</v>
+      </c>
+      <c r="F74" s="20">
+        <v>8006</v>
+      </c>
+      <c r="G74" s="20">
+        <v>173</v>
+      </c>
+      <c r="H74" s="20">
+        <v>237</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="J74" s="20">
+        <v>45</v>
+      </c>
+      <c r="K74" s="20">
+        <v>45</v>
+      </c>
+      <c r="L74" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="N74" s="21">
+        <v>15000</v>
+      </c>
+      <c r="O74" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="P74" s="20">
+        <v>50000</v>
+      </c>
+      <c r="Q74" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="R74" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="S74" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U74" s="5">
+        <v>45</v>
+      </c>
+      <c r="V74" s="20" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed failures in dashboard, insured and etc
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="243">
   <si>
     <t xml:space="preserve">testLoginFunctionality</t>
   </si>
@@ -1089,7 +1089,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1217,7 +1217,7 @@
       <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
@@ -2359,13 +2359,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
@@ -2537,502 +2537,446 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="3" t="n">
+        <v>25997</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>7166</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="5" t="n">
         <v>20217</v>
       </c>
-      <c r="H10" s="5" t="n">
-        <v>173</v>
-      </c>
-      <c r="I10" s="5" t="n">
+      <c r="H15" s="5" t="n">
         <v>237</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="I15" s="5" t="n">
+        <v>8006</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G16" s="3" t="n">
+        <v>25997</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>7166</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>8414</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="5" t="n">
         <v>20217</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="G21" s="5" t="n">
         <v>237</v>
       </c>
-      <c r="I11" s="5" t="n">
+      <c r="H21" s="5" t="n">
         <v>8006</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="I21" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>20217</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>237</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>8006</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>20217</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>237</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>8006</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E41" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>25997</v>
-      </c>
-      <c r="H12" s="3" t="n">
-        <v>7166</v>
-      </c>
-      <c r="I12" s="3" t="n">
-        <v>8414</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>20217</v>
-      </c>
-      <c r="H17" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="I17" s="5" t="n">
-        <v>8006</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="3" t="n">
-        <v>25997</v>
-      </c>
-      <c r="H18" s="3" t="n">
-        <v>7166</v>
-      </c>
-      <c r="I18" s="3" t="n">
-        <v>8414</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>20217</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>8006</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D28" s="5" t="n">
-        <v>20217</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="F28" s="5" t="n">
-        <v>8006</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="5" t="n">
-        <v>20217</v>
-      </c>
-      <c r="G33" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="H33" s="5" t="n">
-        <v>8006</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" display="https://macm.net/"/>
+    <hyperlink ref="K16" r:id="rId1" display="https://macm.net/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3055,7 +2999,7 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -3400,7 +3344,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3619,11 +3563,11 @@
   </sheetPr>
   <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q36" activeCellId="0" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
@@ -5592,7 +5536,7 @@
       <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>

</xml_diff>

<commit_message>
executed tests on linux and fixed failures
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="243">
   <si>
     <t xml:space="preserve">testLoginFunctionality</t>
   </si>
@@ -1089,7 +1089,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1217,7 +1217,7 @@
       <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
@@ -2361,11 +2361,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
@@ -2999,7 +2999,7 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -3344,7 +3344,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3561,13 +3561,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X74"/>
+  <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q36" activeCellId="0" sqref="Q36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
@@ -3820,6 +3820,7 @@
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
     </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>188</v>
@@ -4329,6 +4330,8 @@
         <v>50</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>194</v>
@@ -4464,6 +4467,8 @@
         <v>50</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>195</v>
@@ -4521,6 +4526,8 @@
         <v>202</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>203</v>
@@ -4674,6 +4681,8 @@
         <v>209</v>
       </c>
     </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>210</v>
@@ -4701,6 +4710,8 @@
         <v>209</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>211</v>
@@ -4854,6 +4865,8 @@
         <v>50</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>213</v>
@@ -5007,243 +5020,352 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>19</v>
+        <v>196</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>20</v>
+        <v>197</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="3" t="n">
-        <v>20217</v>
-      </c>
-      <c r="C54" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="D54" s="3" t="n">
-        <v>8006</v>
+      <c r="B54" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H54" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="G54" s="22" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I54" s="22" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="J54" s="22" t="n">
+        <v>445</v>
+      </c>
+      <c r="K54" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="L54" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M54" s="23" t="n">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>19</v>
+        <v>168</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>20</v>
+        <v>161</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>191</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="3" t="n">
-        <v>20217</v>
-      </c>
-      <c r="C59" s="5" t="n">
-        <v>237</v>
-      </c>
-      <c r="D59" s="3" t="n">
-        <v>8006</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="22" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="D59" s="22" t="n">
+        <v>445</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G59" s="23" t="n">
+        <v>12000</v>
+      </c>
+      <c r="H59" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="I59" s="22" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J59" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K59" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L59" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O59" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q59" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I63" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="J63" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="K63" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="L63" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="M63" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="N63" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="O63" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="P63" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J63" s="3" t="s">
+      <c r="Q63" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="K63" s="3" t="s">
+      <c r="R63" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L63" s="3" t="s">
+      <c r="S63" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M63" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="N63" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="O63" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="P63" s="3" t="s">
+      <c r="T63" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="Q63" s="3" t="s">
+      <c r="U63" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="R63" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="22" t="n">
+        <v>20217</v>
+      </c>
+      <c r="E64" s="22" t="n">
+        <v>237</v>
+      </c>
+      <c r="F64" s="22" t="n">
+        <v>8006</v>
+      </c>
+      <c r="G64" s="22" t="n">
+        <v>173</v>
+      </c>
+      <c r="H64" s="22" t="n">
+        <v>237</v>
+      </c>
+      <c r="I64" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="C64" s="22" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="D64" s="22" t="n">
-        <v>445</v>
-      </c>
-      <c r="E64" s="22" t="s">
+      <c r="J64" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="K64" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="L64" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="F64" s="22" t="s">
+      <c r="M64" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="G64" s="23" t="n">
-        <v>12000</v>
-      </c>
-      <c r="H64" s="24" t="s">
+      <c r="N64" s="23" t="n">
+        <v>15000</v>
+      </c>
+      <c r="O64" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="I64" s="22" t="n">
+      <c r="P64" s="22" t="n">
         <v>50000</v>
       </c>
-      <c r="J64" s="22" t="s">
+      <c r="Q64" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="R64" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="L64" s="22" t="s">
+      <c r="S64" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="M64" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="N64" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O64" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="P64" s="6" t="s">
+      <c r="T64" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="Q64" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="R64" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U64" s="5" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>1</v>
       </c>
@@ -5307,8 +5429,11 @@
       <c r="U68" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="V68" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
         <v>5</v>
       </c>
@@ -5372,148 +5497,15 @@
       <c r="U69" s="5" t="n">
         <v>45</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M73" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N73" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O73" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P73" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q73" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R73" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S73" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T73" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U73" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="V73" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D74" s="22" t="n">
-        <v>20217</v>
-      </c>
-      <c r="E74" s="22" t="n">
-        <v>237</v>
-      </c>
-      <c r="F74" s="22" t="n">
-        <v>8006</v>
-      </c>
-      <c r="G74" s="22" t="n">
-        <v>173</v>
-      </c>
-      <c r="H74" s="22" t="n">
-        <v>237</v>
-      </c>
-      <c r="I74" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="J74" s="22" t="n">
-        <v>45</v>
-      </c>
-      <c r="K74" s="22" t="n">
-        <v>45</v>
-      </c>
-      <c r="L74" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="M74" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="N74" s="23" t="n">
-        <v>15000</v>
-      </c>
-      <c r="O74" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="P74" s="22" t="n">
-        <v>50000</v>
-      </c>
-      <c r="Q74" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="R74" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="S74" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="T74" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="U74" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="V74" s="22" t="s">
+      <c r="V69" s="22" t="s">
         <v>224</v>
       </c>
     </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5536,7 +5528,7 @@
       <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>

</xml_diff>

<commit_message>
fixed some failures in existing quote tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -884,7 +884,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -945,11 +945,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,23 +957,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,6 +971,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1089,7 +1085,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1217,7 +1213,7 @@
       <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
@@ -2365,7 +2361,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
@@ -2999,7 +2995,7 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -3344,7 +3340,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3561,42 +3557,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="13.03"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3654,7 +3647,7 @@
       <c r="S2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="3" t="s">
         <v>156</v>
       </c>
       <c r="U2" s="3" t="s">
@@ -3664,7 +3657,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -3710,7 +3703,7 @@
       <c r="O3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="P3" s="16" t="n">
+      <c r="P3" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
@@ -3722,7 +3715,7 @@
       <c r="S3" s="5" t="n">
         <v>50000</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="6" t="s">
         <v>163</v>
       </c>
       <c r="U3" s="6" t="s">
@@ -3732,7 +3725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3778,7 +3771,7 @@
       <c r="O4" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="P4" s="16" t="n">
+      <c r="P4" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
@@ -3790,7 +3783,7 @@
       <c r="S4" s="5" t="n">
         <v>50000</v>
       </c>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="6" t="s">
         <v>163</v>
       </c>
       <c r="U4" s="6" t="s">
@@ -3800,35 +3793,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -3886,7 +3858,7 @@
       <c r="S8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="T8" s="3" t="s">
         <v>156</v>
       </c>
       <c r="U8" s="3" t="s">
@@ -3896,7 +3868,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -3942,7 +3914,7 @@
       <c r="O9" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="P9" s="16" t="n">
+      <c r="P9" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
@@ -3954,7 +3926,7 @@
       <c r="S9" s="5" t="n">
         <v>50000</v>
       </c>
-      <c r="T9" s="17" t="s">
+      <c r="T9" s="6" t="s">
         <v>163</v>
       </c>
       <c r="U9" s="6" t="s">
@@ -3964,62 +3936,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="18"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="18"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -4077,7 +3999,7 @@
       <c r="S13" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="T13" s="15" t="s">
+      <c r="T13" s="16" t="s">
         <v>156</v>
       </c>
       <c r="U13" s="3" t="s">
@@ -4087,7 +4009,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -4133,7 +4055,7 @@
       <c r="O14" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="P14" s="16" t="n">
+      <c r="P14" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q14" s="5" t="s">
@@ -4155,46 +4077,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="18"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -4262,219 +4150,235 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="19" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="19" t="n">
         <v>20217</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="19" t="n">
         <v>237</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="19" t="n">
         <v>8006</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="19" t="n">
         <v>173</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="19" t="n">
         <v>237</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="J19" s="6" t="n">
+      <c r="J19" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="19" t="n">
         <v>445</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N19" s="16" t="n">
+      <c r="N19" s="20" t="n">
         <v>12000</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="O19" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P19" s="5" t="n">
+      <c r="P19" s="19" t="n">
         <v>50000</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="Q19" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="S19" s="5" t="s">
+      <c r="S19" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="T19" s="3" t="n">
+      <c r="T19" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="U19" s="6" t="s">
+      <c r="U19" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="V19" s="5" t="n">
+      <c r="V19" s="19" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="N23" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="P23" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="Q23" s="3" t="s">
+      <c r="Q23" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="R23" s="3" t="s">
+      <c r="R23" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="S23" s="3" t="s">
+      <c r="S23" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="T23" s="3" t="s">
+      <c r="T23" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="U23" s="3" t="s">
+      <c r="U23" s="18" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="24" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" s="19" t="n">
         <v>20217</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="19" t="n">
         <v>237</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" s="19" t="n">
         <v>8006</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" s="19" t="n">
         <v>173</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="19" t="n">
         <v>237</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="J24" s="6" t="n">
+      <c r="J24" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="19" t="n">
         <v>445</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N24" s="16" t="n">
+      <c r="N24" s="20" t="n">
         <v>12000</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="O24" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P24" s="5" t="n">
+      <c r="P24" s="19" t="n">
         <v>50000</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="Q24" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="R24" s="5" t="s">
+      <c r="R24" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="S24" s="5" t="s">
+      <c r="S24" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="T24" s="6" t="s">
+      <c r="T24" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="U24" s="5" t="n">
+      <c r="U24" s="19" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -4500,40 +4404,38 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="19" t="n">
         <v>237</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>1</v>
       </c>
@@ -4607,62 +4509,62 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="22" t="s">
+    <row r="34" customFormat="false" ht="16.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="22" t="n">
+      <c r="D34" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="E34" s="22" t="n">
+      <c r="E34" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="F34" s="22" t="n">
+      <c r="F34" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="G34" s="22" t="n">
+      <c r="G34" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="H34" s="22" t="n">
+      <c r="H34" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="I34" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J34" s="22" t="n">
+      <c r="J34" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="K34" s="22" t="n">
+      <c r="K34" s="18" t="n">
         <v>445</v>
       </c>
-      <c r="L34" s="22" t="s">
+      <c r="L34" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M34" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N34" s="23" t="n">
+      <c r="N34" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="O34" s="24" t="s">
+      <c r="O34" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P34" s="22" t="n">
+      <c r="P34" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="Q34" s="22" t="s">
+      <c r="Q34" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R34" s="22" t="s">
+      <c r="R34" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="S34" s="22" t="s">
+      <c r="S34" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T34" s="6" t="s">
@@ -4681,14 +4583,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -4699,25 +4599,23 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="22" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
@@ -4791,62 +4689,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="22" t="s">
+    <row r="44" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="22" t="n">
+      <c r="D44" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="E44" s="22" t="n">
+      <c r="E44" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="F44" s="22" t="n">
+      <c r="F44" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="G44" s="22" t="n">
+      <c r="G44" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="H44" s="22" t="n">
+      <c r="H44" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I44" s="22" t="s">
+      <c r="I44" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J44" s="22" t="n">
+      <c r="J44" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="K44" s="22" t="n">
+      <c r="K44" s="18" t="n">
         <v>445</v>
       </c>
-      <c r="L44" s="22" t="s">
+      <c r="L44" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M44" s="22" t="s">
+      <c r="M44" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N44" s="23" t="n">
+      <c r="N44" s="20" t="n">
         <v>12000</v>
       </c>
-      <c r="O44" s="24" t="s">
+      <c r="O44" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P44" s="22" t="n">
+      <c r="P44" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="Q44" s="22" t="s">
+      <c r="Q44" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R44" s="22" t="s">
+      <c r="R44" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="S44" s="22" t="s">
+      <c r="S44" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T44" s="3" t="s">
@@ -4855,7 +4753,7 @@
       <c r="U44" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="V44" s="25" t="s">
+      <c r="V44" s="24" t="s">
         <v>212</v>
       </c>
       <c r="W44" s="6" t="s">
@@ -4865,14 +4763,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>1</v>
       </c>
@@ -4946,62 +4842,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="22" t="s">
+    <row r="49" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="22" t="n">
+      <c r="D49" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="E49" s="22" t="n">
+      <c r="E49" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="F49" s="22" t="n">
+      <c r="F49" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="G49" s="22" t="n">
+      <c r="G49" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="H49" s="22" t="n">
+      <c r="H49" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I49" s="22" t="s">
+      <c r="I49" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J49" s="22" t="n">
+      <c r="J49" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="K49" s="22" t="n">
+      <c r="K49" s="18" t="n">
         <v>445</v>
       </c>
-      <c r="L49" s="22" t="s">
+      <c r="L49" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="M49" s="22" t="s">
+      <c r="M49" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="N49" s="25" t="s">
+      <c r="N49" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="O49" s="24" t="s">
+      <c r="O49" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P49" s="22" t="n">
+      <c r="P49" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="Q49" s="22" t="s">
+      <c r="Q49" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R49" s="22" t="s">
+      <c r="R49" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="S49" s="22" t="s">
+      <c r="S49" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T49" s="3" t="s">
@@ -5020,7 +4916,6 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>219</v>
@@ -5083,28 +4978,28 @@
       <c r="E54" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="G54" s="22" t="n">
+      <c r="G54" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="H54" s="22" t="s">
+      <c r="H54" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="I54" s="22" t="n">
+      <c r="I54" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="J54" s="22" t="n">
+      <c r="J54" s="18" t="n">
         <v>445</v>
       </c>
-      <c r="K54" s="22" t="s">
+      <c r="K54" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="L54" s="22" t="s">
+      <c r="L54" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M54" s="23" t="n">
+      <c r="M54" s="20" t="n">
         <v>12000</v>
       </c>
     </row>
@@ -5173,37 +5068,37 @@
       <c r="A59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="22" t="n">
+      <c r="C59" s="18" t="n">
         <v>1000000</v>
       </c>
-      <c r="D59" s="22" t="n">
+      <c r="D59" s="18" t="n">
         <v>445</v>
       </c>
-      <c r="E59" s="22" t="s">
+      <c r="E59" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="G59" s="23" t="n">
+      <c r="G59" s="20" t="n">
         <v>12000</v>
       </c>
-      <c r="H59" s="24" t="s">
+      <c r="H59" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="I59" s="22" t="n">
+      <c r="I59" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="J59" s="22" t="s">
+      <c r="J59" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="K59" s="22" t="s">
+      <c r="K59" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="L59" s="22" t="s">
+      <c r="L59" s="18" t="s">
         <v>165</v>
       </c>
       <c r="M59" s="3" t="s">
@@ -5212,7 +5107,7 @@
       <c r="N59" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="O59" s="25" t="s">
+      <c r="O59" s="24" t="s">
         <v>212</v>
       </c>
       <c r="P59" s="6" t="s">
@@ -5295,62 +5190,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="22" t="s">
+    <row r="64" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D64" s="22" t="n">
+      <c r="D64" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="E64" s="22" t="n">
+      <c r="E64" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="F64" s="22" t="n">
+      <c r="F64" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="G64" s="22" t="n">
+      <c r="G64" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="H64" s="22" t="n">
+      <c r="H64" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I64" s="22" t="s">
+      <c r="I64" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J64" s="22" t="n">
+      <c r="J64" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="K64" s="22" t="n">
+      <c r="K64" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="L64" s="22" t="s">
+      <c r="L64" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M64" s="22" t="s">
+      <c r="M64" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N64" s="23" t="n">
+      <c r="N64" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="O64" s="24" t="s">
+      <c r="O64" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P64" s="22" t="n">
+      <c r="P64" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="Q64" s="22" t="s">
+      <c r="Q64" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R64" s="22" t="s">
+      <c r="R64" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="S64" s="22" t="s">
+      <c r="S64" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T64" s="6" t="s">
@@ -5434,61 +5329,61 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" s="22" t="s">
+      <c r="A69" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C69" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D69" s="22" t="n">
+      <c r="D69" s="18" t="n">
         <v>20217</v>
       </c>
-      <c r="E69" s="22" t="n">
+      <c r="E69" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="F69" s="22" t="n">
+      <c r="F69" s="18" t="n">
         <v>8006</v>
       </c>
-      <c r="G69" s="22" t="n">
+      <c r="G69" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="H69" s="22" t="n">
+      <c r="H69" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="I69" s="22" t="s">
+      <c r="I69" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J69" s="22" t="n">
+      <c r="J69" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="K69" s="22" t="n">
+      <c r="K69" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="L69" s="22" t="s">
+      <c r="L69" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="M69" s="22" t="s">
+      <c r="M69" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="N69" s="23" t="n">
+      <c r="N69" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="O69" s="24" t="s">
+      <c r="O69" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P69" s="22" t="n">
+      <c r="P69" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="Q69" s="22" t="s">
+      <c r="Q69" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="R69" s="22" t="s">
+      <c r="R69" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="S69" s="22" t="s">
+      <c r="S69" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T69" s="6" t="s">
@@ -5497,22 +5392,17 @@
       <c r="U69" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="V69" s="22" t="s">
+      <c r="V69" s="18" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5524,11 +5414,11 @@
   </sheetPr>
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
@@ -5550,7 +5440,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5566,13 +5456,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5644,49 +5534,49 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="22" t="n">
+      <c r="C8" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="D8" s="22" t="n">
+      <c r="D8" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="F8" s="22" t="n">
+      <c r="F8" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G8" s="22" t="n">
+      <c r="G8" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="J8" s="23" t="n">
+      <c r="J8" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="L8" s="22" t="n">
+      <c r="L8" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="18" t="s">
         <v>165</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -5695,60 +5585,60 @@
       <c r="Q8" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="R8" s="22" t="s">
+      <c r="R8" s="18" t="s">
         <v>208</v>
       </c>
       <c r="S8" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="T8" s="22" t="s">
+      <c r="T8" s="18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="22" t="n">
+      <c r="C9" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="D9" s="22" t="n">
+      <c r="D9" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="22" t="n">
+      <c r="F9" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G9" s="22" t="n">
+      <c r="G9" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="J9" s="23" t="n">
+      <c r="J9" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="L9" s="22" t="n">
+      <c r="L9" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="18" t="s">
         <v>165</v>
       </c>
       <c r="P9" s="6" t="s">
@@ -5757,18 +5647,18 @@
       <c r="Q9" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="R9" s="22" t="s">
+      <c r="R9" s="18" t="s">
         <v>208</v>
       </c>
       <c r="S9" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>234</v>
       </c>
     </row>
@@ -5784,13 +5674,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="18" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5798,22 +5688,22 @@
       <c r="A17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
@@ -5869,46 +5759,46 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="22" t="n">
+      <c r="A19" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="C19" s="22" t="n">
+      <c r="C19" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="22" t="n">
+      <c r="E19" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="F19" s="22" t="n">
+      <c r="F19" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I19" s="23" t="n">
+      <c r="I19" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="22" t="n">
+      <c r="K19" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="L19" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="M19" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="N19" s="22" t="s">
+      <c r="N19" s="18" t="s">
         <v>165</v>
       </c>
       <c r="O19" s="6" t="s">
@@ -5917,7 +5807,7 @@
       <c r="P19" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="Q19" s="22" t="s">
+      <c r="Q19" s="18" t="s">
         <v>208</v>
       </c>
     </row>
@@ -5986,46 +5876,46 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="22" t="n">
+      <c r="A24" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="C24" s="22" t="n">
+      <c r="C24" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="E24" s="22" t="n">
+      <c r="E24" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="F24" s="22" t="n">
+      <c r="F24" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I24" s="23" t="n">
+      <c r="I24" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="K24" s="22" t="n">
+      <c r="K24" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="N24" s="22" t="s">
+      <c r="N24" s="18" t="s">
         <v>165</v>
       </c>
       <c r="O24" s="6" t="s">
@@ -6034,13 +5924,13 @@
       <c r="P24" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="Q24" s="22" t="s">
+      <c r="Q24" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="R24" s="22" t="s">
+      <c r="R24" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="S24" s="22" t="s">
+      <c r="S24" s="18" t="s">
         <v>208</v>
       </c>
     </row>
@@ -6103,46 +5993,46 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="22" t="n">
+      <c r="A29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="C29" s="22" t="n">
+      <c r="C29" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="22" t="n">
+      <c r="E29" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="F29" s="22" t="n">
+      <c r="F29" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I29" s="23" t="n">
+      <c r="I29" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="J29" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="K29" s="22" t="n">
+      <c r="K29" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="L29" s="22" t="s">
+      <c r="L29" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="18" t="s">
         <v>165</v>
       </c>
       <c r="O29" s="6" t="s">
@@ -6151,7 +6041,7 @@
       <c r="P29" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="Q29" s="22" t="s">
+      <c r="Q29" s="18" t="s">
         <v>208</v>
       </c>
     </row>
@@ -6217,46 +6107,46 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="22" t="n">
+      <c r="A34" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="18" t="n">
         <v>173</v>
       </c>
-      <c r="C34" s="22" t="n">
+      <c r="C34" s="18" t="n">
         <v>237</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="22" t="n">
+      <c r="E34" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="F34" s="22" t="n">
+      <c r="F34" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I34" s="23" t="n">
+      <c r="I34" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="J34" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="K34" s="22" t="n">
+      <c r="K34" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="L34" s="22" t="s">
+      <c r="L34" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M34" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="N34" s="22" t="s">
+      <c r="N34" s="18" t="s">
         <v>165</v>
       </c>
       <c r="O34" s="6" t="s">
@@ -6265,10 +6155,10 @@
       <c r="P34" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="Q34" s="22" t="s">
+      <c r="Q34" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="R34" s="22" t="s">
+      <c r="R34" s="18" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed quote tests based on omic and aao coverages
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-576\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E05A09-CA63-4AED-B290-98DBFD0048C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339CDE32-2C29-4C5B-8A94-AC0B30871057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="245">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -761,6 +761,12 @@
   </si>
   <si>
     <t>testValidateConfirmDatesPlaceOrderFunctionality</t>
+  </si>
+  <si>
+    <t>coverageOmic</t>
+  </si>
+  <si>
+    <t>testNotDisplayPremiumIfReviewRequired</t>
   </si>
 </sst>
 </file>
@@ -866,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -929,6 +935,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3749,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X69"/>
+  <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" topLeftCell="K50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V69" sqref="V69:V73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3772,6 +3787,7 @@
     <col min="17" max="17" width="16.88671875" customWidth="1"/>
     <col min="18" max="18" width="17.44140625" customWidth="1"/>
     <col min="20" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -4499,8 +4515,11 @@
       <c r="U23" s="18" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V23" s="29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>5</v>
       </c>
@@ -4563,6 +4582,9 @@
       </c>
       <c r="U24" s="19">
         <v>50</v>
+      </c>
+      <c r="V24" s="30" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
@@ -5532,7 +5554,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
         <v>5</v>
       </c>
@@ -5596,13 +5618,158 @@
       <c r="U69" s="5">
         <v>45</v>
       </c>
-      <c r="V69" s="18" t="s">
+      <c r="V69" s="21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V70" s="31"/>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V71" s="31"/>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M72" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="O72" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P72" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q72" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="T72" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V72" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="A73" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" s="18">
+        <v>20217</v>
+      </c>
+      <c r="E73" s="18">
+        <v>237</v>
+      </c>
+      <c r="F73" s="18">
+        <v>8006</v>
+      </c>
+      <c r="G73" s="18">
+        <v>173</v>
+      </c>
+      <c r="H73" s="18">
+        <v>237</v>
+      </c>
+      <c r="I73" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J73" s="18">
+        <v>45</v>
+      </c>
+      <c r="K73" s="18">
+        <v>45</v>
+      </c>
+      <c r="L73" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="M73" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="N73" s="20">
+        <v>15000</v>
+      </c>
+      <c r="O73" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="P73" s="18">
+        <v>50000</v>
+      </c>
+      <c r="Q73" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="R73" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="S73" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="T73" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="U73" s="5">
+        <v>45</v>
+      </c>
+      <c r="V73" s="21" t="s">
         <v>224</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
added multicoverage product for OMIC
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auulu\Documents\bp-ui-tests-QAT-576\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339CDE32-2C29-4C5B-8A94-AC0B30871057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF67AA-AC9B-4EF9-B43D-44882598F8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="249">
   <si>
     <t>testLoginFunctionality</t>
   </si>
@@ -767,6 +767,18 @@
   </si>
   <si>
     <t>testNotDisplayPremiumIfReviewRequired</t>
+  </si>
+  <si>
+    <t>coverageAAO</t>
+  </si>
+  <si>
+    <t>American Academy of Ophthalmology (AAO) - e-MD®/Broad Regulatory Protection Plus</t>
+  </si>
+  <si>
+    <t>$ 10,000</t>
+  </si>
+  <si>
+    <t>testMultiCoverageInQuote</t>
   </si>
 </sst>
 </file>
@@ -872,7 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -944,6 +956,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3764,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X73"/>
+  <dimension ref="A1:Z77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V69" sqref="V69:V73"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3788,6 +3803,9 @@
     <col min="18" max="18" width="17.44140625" customWidth="1"/>
     <col min="20" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="17.109375" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="25" max="25" width="23.33203125" customWidth="1"/>
+    <col min="26" max="26" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -4285,12 +4303,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -4358,7 +4376,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>5</v>
       </c>
@@ -4426,7 +4444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>194</v>
       </c>
@@ -4451,7 +4469,7 @@
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
@@ -4518,8 +4536,11 @@
       <c r="V23" s="29" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="W23" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>5</v>
       </c>
@@ -4586,13 +4607,16 @@
       <c r="V24" s="30" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W24" s="30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -4618,7 +4642,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
@@ -4644,12 +4668,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>1</v>
       </c>
@@ -4723,7 +4747,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>5</v>
       </c>
@@ -4797,12 +4821,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -4813,7 +4837,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>5</v>
       </c>
@@ -4824,12 +4848,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
@@ -4902,8 +4926,14 @@
       <c r="X43" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y43" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z43" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>5</v>
       </c>
@@ -4968,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="V44" s="24" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="W44" s="6" t="s">
         <v>166</v>
@@ -4976,13 +5006,19 @@
       <c r="X44" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y44" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z44" s="30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>1</v>
       </c>
@@ -5765,6 +5801,105 @@
       </c>
       <c r="V73" s="21" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M76" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="G77" s="18">
+        <v>50000</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="I77" s="18">
+        <v>1000000</v>
+      </c>
+      <c r="J77" s="18">
+        <v>445</v>
+      </c>
+      <c r="K77" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="L77" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="M77" s="20">
+        <v>12000</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="O77" s="5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created json test data for quote, binder and details page tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="250">
   <si>
     <t xml:space="preserve">testLoginFunctionality</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t xml:space="preserve">testClearancesReviewFunctionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testRenewalPolicyClearanceValidation</t>
   </si>
   <si>
     <t xml:space="preserve">testBusinessClassRatingCriteria</t>
@@ -902,7 +905,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -997,14 +1000,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1115,10 +1110,10 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.33"/>
   </cols>
@@ -1239,19 +1234,19 @@
   </sheetPr>
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.56"/>
@@ -2385,20 +2380,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="36.11"/>
@@ -2995,6 +2990,27 @@
         <v>5</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3023,7 +3039,7 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -3043,7 +3059,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -3073,34 +3089,34 @@
         <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,16 +3154,16 @@
         <v>50000</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P3" s="5" t="n">
         <v>50</v>
@@ -3161,7 +3177,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -3173,34 +3189,34 @@
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>64</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,16 +3224,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>100000</v>
@@ -3232,18 +3248,18 @@
         <v>30000000</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3275,7 +3291,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,28 +3302,28 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,13 +3337,13 @@
         <v>50000</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>100000</v>
@@ -3336,7 +3352,7 @@
         <v>60</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J18" s="5" t="n">
         <v>50</v>
@@ -3368,7 +3384,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3382,7 +3398,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,16 +3409,16 @@
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,18 +3432,18 @@
         <v>50000</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3438,22 +3454,22 @@
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3467,24 +3483,24 @@
         <v>50000</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3495,34 +3511,34 @@
         <v>28</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>64</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M13" s="14" t="s">
         <v>17</v>
@@ -3536,13 +3552,13 @@
         <v>49</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F14" s="14" t="n">
         <v>4000</v>
@@ -3557,13 +3573,13 @@
         <v>100000</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>29</v>
@@ -3591,33 +3607,33 @@
       <selection pane="topLeft" activeCell="Q76" activeCellId="0" sqref="Q76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3648,46 +3664,46 @@
         <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3695,7 +3711,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>49</v>
@@ -3722,7 +3738,7 @@
         <v>237</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L3" s="6" t="n">
         <v>1000000</v>
@@ -3731,28 +3747,28 @@
         <v>445</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P3" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="S3" s="5" t="n">
         <v>50000</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V3" s="5" t="n">
         <v>50</v>
@@ -3763,7 +3779,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>49</v>
@@ -3790,7 +3806,7 @@
         <v>237</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L4" s="6" t="n">
         <v>1000000</v>
@@ -3799,28 +3815,28 @@
         <v>445</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P4" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="S4" s="5" t="n">
         <v>50000</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V4" s="5" t="n">
         <v>50</v>
@@ -3828,7 +3844,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3859,46 +3875,46 @@
         <v>21</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,7 +3922,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>49</v>
@@ -3933,7 +3949,7 @@
         <v>237</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L9" s="6" t="n">
         <v>1000000</v>
@@ -3942,28 +3958,28 @@
         <v>445</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P9" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="S9" s="5" t="n">
         <v>50000</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V9" s="5" t="n">
         <v>50</v>
@@ -3971,7 +3987,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,46 +4016,46 @@
         <v>21</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="T13" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V13" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="T13" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,7 +4063,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>49</v>
@@ -4074,7 +4090,7 @@
         <v>237</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L14" s="6" t="n">
         <v>1000000</v>
@@ -4083,28 +4099,28 @@
         <v>445</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P14" s="15" t="n">
         <v>10000</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="S14" s="5" t="n">
         <v>50000</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V14" s="5" t="n">
         <v>50</v>
@@ -4112,7 +4128,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,52 +4151,52 @@
         <v>21</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V18" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="U18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4225,7 @@
         <v>237</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J19" s="18" t="n">
         <v>1000000</v>
@@ -4218,34 +4234,34 @@
         <v>445</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N19" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P19" s="19" t="n">
         <v>50000</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S19" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T19" s="18" t="n">
         <v>1</v>
       </c>
       <c r="U19" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V19" s="19" t="n">
         <v>50</v>
@@ -4253,7 +4269,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -4296,55 +4312,55 @@
         <v>21</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J23" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q23" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="T23" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="U23" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="K23" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="L23" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="M23" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="N23" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="O23" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="P23" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q23" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="R23" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="S23" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="T23" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="U23" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="V23" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="W23" s="25" t="s">
+      <c r="V23" s="18" t="s">
         <v>196</v>
+      </c>
+      <c r="W23" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="100.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4373,7 +4389,7 @@
         <v>237</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J24" s="18" t="n">
         <v>1000000</v>
@@ -4382,45 +4398,45 @@
         <v>445</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N24" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="O24" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P24" s="19" t="n">
         <v>50000</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R24" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S24" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T24" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U24" s="19" t="n">
         <v>50</v>
       </c>
       <c r="V24" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="W24" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,16 +4453,16 @@
         <v>21</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4463,21 +4479,21 @@
         <v>8006</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,58 +4516,58 @@
         <v>21</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U33" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T33" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="V33" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="W33" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4580,7 +4596,7 @@
         <v>237</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J34" s="18" t="n">
         <v>1000000</v>
@@ -4589,48 +4605,48 @@
         <v>445</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N34" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="O34" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P34" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q34" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R34" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S34" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U34" s="5" t="n">
         <v>50</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="W34" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="X34" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4641,7 +4657,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4652,12 +4668,12 @@
         <v>49</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,64 +4696,64 @@
         <v>21</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="U43" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="V43" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="W43" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X43" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M43" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N43" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O43" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q43" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R43" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S43" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T43" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="U43" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="V43" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="W43" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="X43" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y43" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z43" s="25" t="s">
+      <c r="Y43" s="21" t="s">
         <v>196</v>
+      </c>
+      <c r="Z43" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4766,7 +4782,7 @@
         <v>237</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J44" s="18" t="n">
         <v>1000000</v>
@@ -4775,54 +4791,54 @@
         <v>445</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N44" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P44" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q44" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R44" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S44" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U44" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="V44" s="26" t="s">
-        <v>215</v>
+      <c r="V44" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X44" s="5" t="n">
         <v>50</v>
       </c>
       <c r="Y44" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Z44" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,58 +4861,58 @@
         <v>21</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J48" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X48" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="M48" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="N48" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O48" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R48" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S48" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T48" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="U48" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="V48" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="W48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="X48" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4925,7 +4941,7 @@
         <v>237</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J49" s="18" t="n">
         <v>1000000</v>
@@ -4934,40 +4950,40 @@
         <v>445</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M49" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="N49" s="26" t="s">
         <v>222</v>
       </c>
+      <c r="N49" s="24" t="s">
+        <v>223</v>
+      </c>
       <c r="O49" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P49" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q49" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R49" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S49" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T49" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U49" s="3" t="n">
         <v>1</v>
       </c>
       <c r="V49" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X49" s="5" t="n">
         <v>50</v>
@@ -4975,7 +4991,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4983,46 +4999,46 @@
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F53" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="H53" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O53" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="N53" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="O53" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5030,25 +5046,25 @@
         <v>5</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G54" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I54" s="18" t="n">
         <v>1000000</v>
@@ -5057,16 +5073,16 @@
         <v>445</v>
       </c>
       <c r="K54" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L54" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M54" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O54" s="5" t="n">
         <v>50</v>
@@ -5074,7 +5090,7 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,55 +5098,55 @@
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q58" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="M58" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="N58" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q58" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="R58" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5154,7 @@
         <v>5</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C59" s="18" t="n">
         <v>1000000</v>
@@ -5147,51 +5163,51 @@
         <v>445</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G59" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I59" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K59" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L59" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N59" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="O59" s="26" t="s">
-        <v>222</v>
+      <c r="O59" s="24" t="s">
+        <v>223</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q59" s="5" t="n">
         <v>50</v>
       </c>
       <c r="R59" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5214,49 +5230,49 @@
         <v>21</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J63" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R63" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S63" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T63" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U63" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L63" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M63" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N63" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O63" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P63" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q63" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R63" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S63" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T63" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U63" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5285,7 +5301,7 @@
         <v>237</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J64" s="18" t="n">
         <v>45</v>
@@ -5294,31 +5310,31 @@
         <v>45</v>
       </c>
       <c r="L64" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M64" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N64" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="O64" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P64" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q64" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R64" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S64" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U64" s="5" t="n">
         <v>45</v>
@@ -5326,7 +5342,7 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5349,52 +5365,52 @@
         <v>21</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J68" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M68" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O68" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P68" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T68" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U68" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K68" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M68" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N68" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O68" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P68" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q68" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R68" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S68" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T68" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U68" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="V68" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5423,7 +5439,7 @@
         <v>237</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J69" s="18" t="n">
         <v>45</v>
@@ -5432,47 +5448,47 @@
         <v>45</v>
       </c>
       <c r="L69" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M69" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N69" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P69" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q69" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R69" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S69" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U69" s="5" t="n">
         <v>45</v>
       </c>
       <c r="V69" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V70" s="27"/>
+      <c r="V70" s="25"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="V71" s="27"/>
+        <v>230</v>
+      </c>
+      <c r="V71" s="25"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
@@ -5494,52 +5510,52 @@
         <v>21</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J72" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M72" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O72" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="P72" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q72" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="T72" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U72" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K72" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M72" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N72" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O72" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="P72" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q72" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R72" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S72" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="T72" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="U72" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="V72" s="14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5568,7 +5584,7 @@
         <v>237</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J73" s="18" t="n">
         <v>45</v>
@@ -5577,42 +5593,42 @@
         <v>45</v>
       </c>
       <c r="L73" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M73" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N73" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P73" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="Q73" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R73" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S73" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T73" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U73" s="5" t="n">
         <v>45</v>
       </c>
       <c r="V73" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5620,55 +5636,55 @@
         <v>1</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="H76" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M76" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O76" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="J76" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="L76" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="M76" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="N76" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="O76" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="P76" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R76" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5676,25 +5692,25 @@
         <v>5</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G77" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="H77" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I77" s="18" t="n">
         <v>1000000</v>
@@ -5703,28 +5719,28 @@
         <v>445</v>
       </c>
       <c r="K77" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L77" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M77" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O77" s="5" t="n">
         <v>50</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Q77" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R77" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -5745,11 +5761,11 @@
   </sheetPr>
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
@@ -5758,7 +5774,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.33"/>
@@ -5771,8 +5787,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>231</v>
+      <c r="A1" s="26" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5780,10 +5796,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,15 +5807,15 @@
         <v>5</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5807,61 +5823,61 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="R7" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5869,7 +5885,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C8" s="18" t="n">
         <v>173</v>
@@ -5878,7 +5894,7 @@
         <v>237</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F8" s="18" t="n">
         <v>45</v>
@@ -5887,43 +5903,43 @@
         <v>45</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J8" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L8" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q8" s="5" t="n">
         <v>45</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="S8" s="5" t="n">
         <v>45</v>
       </c>
       <c r="T8" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,7 +5947,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C9" s="18" t="n">
         <v>173</v>
@@ -5940,7 +5956,7 @@
         <v>237</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F9" s="18" t="n">
         <v>45</v>
@@ -5949,48 +5965,48 @@
         <v>45</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J9" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L9" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q9" s="5" t="n">
         <v>45</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="S9" s="5" t="n">
         <v>45</v>
       </c>
       <c r="T9" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="s">
-        <v>240</v>
+      <c r="A12" s="26" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,10 +6014,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6009,84 +6025,84 @@
         <v>5</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
+        <v>243</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="Q18" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6100,7 +6116,7 @@
         <v>237</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E19" s="18" t="n">
         <v>45</v>
@@ -6109,42 +6125,42 @@
         <v>45</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I19" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K19" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M19" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P19" s="5" t="n">
         <v>45</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6152,58 +6168,58 @@
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P23" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="Q23" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6217,7 +6233,7 @@
         <v>237</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E24" s="18" t="n">
         <v>45</v>
@@ -6226,48 +6242,48 @@
         <v>45</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I24" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K24" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N24" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P24" s="5" t="n">
         <v>45</v>
       </c>
       <c r="Q24" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R24" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6275,52 +6291,52 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="Q28" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,7 +6350,7 @@
         <v>237</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E29" s="18" t="n">
         <v>45</v>
@@ -6343,42 +6359,42 @@
         <v>45</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I29" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K29" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P29" s="5" t="n">
         <v>45</v>
       </c>
       <c r="Q29" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6386,55 +6402,55 @@
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P33" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="Q33" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6448,7 +6464,7 @@
         <v>237</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E34" s="18" t="n">
         <v>45</v>
@@ -6457,40 +6473,40 @@
         <v>45</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I34" s="20" t="n">
         <v>15000</v>
       </c>
       <c r="J34" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K34" s="18" t="n">
         <v>50000</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N34" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P34" s="5" t="n">
         <v>45</v>
       </c>
       <c r="Q34" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R34" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>